<commit_message>
updated graphics and colors on battleship
</commit_message>
<xml_diff>
--- a/battleship.xlsx
+++ b/battleship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEDE273-0A75-CB4F-AF94-062957878ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697A9CB7-2057-7B4D-9436-5B320C412478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="725">
   <si>
     <t>CALL CLEAR</t>
   </si>
@@ -1839,15 +1839,6 @@
     <t>IF HORIZONTAL=1 THEN SERIAL(I)=COORDS(I) ELSE SERIAL(I)=ASC(COORDS$(I))-64</t>
   </si>
   <si>
-    <t>CALL COLOR(9,2,1) :: REM BLACK ON TRANSPARENT</t>
-  </si>
-  <si>
-    <t>CALL COLOR(10,2,12) :: REM BLACK ON LIGHT YELLOW</t>
-  </si>
-  <si>
-    <t>CALL COLOR(11,2,3) :: REM BLACK ON MED GREEN</t>
-  </si>
-  <si>
     <t>CALL COLOR(13,2,16) :: REM BLACK ON WHITE</t>
   </si>
   <si>
@@ -1857,9 +1848,6 @@
     <t>HOLECHAR=96 :: CALL CHAR(HOLECHAR,"3C4299A5A599423C") :: REM SET 9</t>
   </si>
   <si>
-    <t>TENCHAR=97 :: CALL CHAR(TENCHAR,"004FC949494949EF") :: REM SET 9</t>
-  </si>
-  <si>
     <t>HITCHAR=104 :: CALL CHAR(HITCHAR,"003C7E7E7E7E3C00") :: REM SET 10</t>
   </si>
   <si>
@@ -2194,6 +2182,39 @@
   </si>
   <si>
     <t>DEBUG=1</t>
+  </si>
+  <si>
+    <t>TENCHAR=120 :: CALL CHAR(TENCHAR,"004FC949494949EF") :: REM SET 12</t>
+  </si>
+  <si>
+    <t>CALL COLOR(12,2,1) :: REM BLACK ON TRANSPARENT</t>
+  </si>
+  <si>
+    <t>FILLCHAR=97 :: CALL CHAR(FILLCHAR,"0000000000000000") :: REM SET 9</t>
+  </si>
+  <si>
+    <t>CALL HCHAR(Y+I,X,FILLCHAR,19)</t>
+  </si>
+  <si>
+    <t>CALL COLOR(9,2,8) :: REM BLACK ON CYAN</t>
+  </si>
+  <si>
+    <t>CALL COLOR(11,2,15) :: REM BLACK ON GREY</t>
+  </si>
+  <si>
+    <t>CALL COLOR(10,2,11) :: REM BLACK ON DARK YELLOW</t>
+  </si>
+  <si>
+    <t>RENDERHOLES</t>
+  </si>
+  <si>
+    <t>RENDERBACKBOARD</t>
+  </si>
+  <si>
+    <t>FOR I=0 TO 18</t>
+  </si>
+  <si>
+    <t>CALL SCREEN(4)</t>
   </si>
 </sst>
 </file>
@@ -2681,7 +2702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3D0CF-00CA-1047-A168-192C0697CE9E}">
-  <dimension ref="A1:E487"/>
+  <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
@@ -2723,17 +2744,8 @@
       <c r="B3">
         <v>110</v>
       </c>
-      <c r="C3" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D3,A:A,0),0)," :: REM CALL ",D3,"")</f>
-        <v>GOSUB 180 :: REM CALL INIT</v>
-      </c>
-      <c r="D3" t="str">
-        <f>A10</f>
-        <v>INIT</v>
-      </c>
-      <c r="E3">
-        <f>_xlfn.IFNA(MATCH(D3,A:A,0),"")</f>
-        <v>10</v>
+      <c r="C3" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2742,15 +2754,15 @@
       </c>
       <c r="C4" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D4,A:A,0),0)," :: REM CALL ",D4,"")</f>
-        <v>GOSUB 320 :: REM CALL SETCHARS</v>
+        <v>GOSUB 190 :: REM CALL INIT</v>
       </c>
       <c r="D4" t="str">
-        <f>A24</f>
-        <v>SETCHARS</v>
+        <f>A11</f>
+        <v>INIT</v>
       </c>
       <c r="E4">
         <f>_xlfn.IFNA(MATCH(D4,A:A,0),"")</f>
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2759,15 +2771,15 @@
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D5,A:A,0),0)," :: REM CALL ",D5,"")</f>
-        <v>GOSUB 400 :: REM CALL SETCOLORSCHEME</v>
+        <v>GOSUB 330 :: REM CALL SETCHARS</v>
       </c>
       <c r="D5" t="str">
-        <f>A32</f>
-        <v>SETCOLORSCHEME</v>
+        <f>A25</f>
+        <v>SETCHARS</v>
       </c>
       <c r="E5">
         <f>_xlfn.IFNA(MATCH(D5,A:A,0),"")</f>
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2776,15 +2788,15 @@
       </c>
       <c r="C6" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D6,A:A,0),0)," :: REM CALL ",D6,"")</f>
-        <v>GOSUB 470 :: REM CALL RENDERBOARDS</v>
+        <v>GOSUB 420 :: REM CALL SETCOLORSCHEME</v>
       </c>
       <c r="D6" t="str">
-        <f>A39</f>
-        <v>RENDERBOARDS</v>
+        <f>A34</f>
+        <v>SETCOLORSCHEME</v>
       </c>
       <c r="E6">
         <f>_xlfn.IFNA(MATCH(D6,A:A,0),"")</f>
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2793,27 +2805,32 @@
       </c>
       <c r="C7" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D7,A:A,0),0)," :: REM CALL ",D7,"")</f>
-        <v>GOSUB 540 :: REM CALL DEPLOYSHIPS</v>
+        <v>GOSUB 500 :: REM CALL RENDERBOARDS</v>
       </c>
       <c r="D7" t="str">
-        <f>A46</f>
-        <v>DEPLOYSHIPS</v>
+        <f>A42</f>
+        <v>RENDERBOARDS</v>
       </c>
       <c r="E7">
         <f>_xlfn.IFNA(MATCH(D7,A:A,0),"")</f>
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>160</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="str">
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D8,A:A,0),0)," :: REM CALL ",D8,"")</f>
+        <v>GOSUB 560 :: REM CALL DEPLOYSHIPS</v>
+      </c>
+      <c r="D8" t="str">
+        <f>A48</f>
+        <v>DEPLOYSHIPS</v>
+      </c>
+      <c r="E8">
         <f>_xlfn.IFNA(MATCH(D8,A:A,0),"")</f>
-        <v/>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2821,7 +2838,7 @@
         <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E9" t="str">
         <f>_xlfn.IFNA(MATCH(D9,A:A,0),"")</f>
@@ -2829,15 +2846,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>5</v>
-      </c>
       <c r="B10">
         <v>180</v>
       </c>
-      <c r="C10" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A10,"***")</f>
-        <v>REM SUBROUTINE ***INIT***</v>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
       <c r="E10" t="str">
         <f>_xlfn.IFNA(MATCH(D10,A:A,0),"")</f>
@@ -2845,11 +2858,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>5</v>
+      </c>
       <c r="B11">
         <v>190</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A11,"***")</f>
+        <v>REM SUBROUTINE ***INIT***</v>
       </c>
       <c r="E11" t="str">
         <f>_xlfn.IFNA(MATCH(D11,A:A,0),"")</f>
@@ -2861,7 +2878,11 @@
         <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>717</v>
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f>_xlfn.IFNA(MATCH(D12,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2869,11 +2890,7 @@
         <v>210</v>
       </c>
       <c r="C13" t="s">
-        <v>553</v>
-      </c>
-      <c r="E13" t="str">
-        <f>_xlfn.IFNA(MATCH(D13,A:A,0),"")</f>
-        <v/>
+        <v>713</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2881,7 +2898,7 @@
         <v>220</v>
       </c>
       <c r="C14" t="s">
-        <v>673</v>
+        <v>553</v>
       </c>
       <c r="E14" t="str">
         <f>_xlfn.IFNA(MATCH(D14,A:A,0),"")</f>
@@ -2893,7 +2910,7 @@
         <v>230</v>
       </c>
       <c r="C15" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="E15" t="str">
         <f>_xlfn.IFNA(MATCH(D15,A:A,0),"")</f>
@@ -2905,7 +2922,7 @@
         <v>240</v>
       </c>
       <c r="C16" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="E16" t="str">
         <f>_xlfn.IFNA(MATCH(D16,A:A,0),"")</f>
@@ -2917,7 +2934,7 @@
         <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>703</v>
+        <v>670</v>
       </c>
       <c r="E17" t="str">
         <f>_xlfn.IFNA(MATCH(D17,A:A,0),"")</f>
@@ -2929,7 +2946,7 @@
         <v>260</v>
       </c>
       <c r="C18" t="s">
-        <v>555</v>
+        <v>699</v>
       </c>
       <c r="E18" t="str">
         <f>_xlfn.IFNA(MATCH(D18,A:A,0),"")</f>
@@ -2941,7 +2958,7 @@
         <v>270</v>
       </c>
       <c r="C19" t="s">
-        <v>701</v>
+        <v>555</v>
       </c>
       <c r="E19" t="str">
         <f>_xlfn.IFNA(MATCH(D19,A:A,0),"")</f>
@@ -2953,7 +2970,7 @@
         <v>280</v>
       </c>
       <c r="C20" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="E20" t="str">
         <f>_xlfn.IFNA(MATCH(D20,A:A,0),"")</f>
@@ -2965,7 +2982,7 @@
         <v>290</v>
       </c>
       <c r="C21" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="E21" t="str">
         <f>_xlfn.IFNA(MATCH(D21,A:A,0),"")</f>
@@ -2977,7 +2994,7 @@
         <v>300</v>
       </c>
       <c r="C22" t="s">
-        <v>589</v>
+        <v>696</v>
       </c>
       <c r="E22" t="str">
         <f>_xlfn.IFNA(MATCH(D22,A:A,0),"")</f>
@@ -2989,7 +3006,7 @@
         <v>310</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>589</v>
       </c>
       <c r="E23" t="str">
         <f>_xlfn.IFNA(MATCH(D23,A:A,0),"")</f>
@@ -2997,15 +3014,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>10</v>
-      </c>
       <c r="B24">
         <v>320</v>
       </c>
-      <c r="C24" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A24,"***")</f>
-        <v>REM SUBROUTINE ***SETCHARS***</v>
+      <c r="C24" t="s">
+        <v>9</v>
       </c>
       <c r="E24" t="str">
         <f>_xlfn.IFNA(MATCH(D24,A:A,0),"")</f>
@@ -3013,11 +3026,15 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>10</v>
+      </c>
       <c r="B25">
         <v>330</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>604</v>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A25,"***")</f>
+        <v>REM SUBROUTINE ***SETCHARS***</v>
       </c>
       <c r="E25" t="str">
         <f>_xlfn.IFNA(MATCH(D25,A:A,0),"")</f>
@@ -3028,8 +3045,8 @@
       <c r="B26">
         <v>340</v>
       </c>
-      <c r="C26" t="s">
-        <v>605</v>
+      <c r="C26" s="5" t="s">
+        <v>601</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.IFNA(MATCH(D26,A:A,0),"")</f>
@@ -3040,20 +3057,16 @@
       <c r="B27">
         <v>350</v>
       </c>
-      <c r="C27" t="s">
-        <v>606</v>
-      </c>
-      <c r="E27" t="str">
-        <f>_xlfn.IFNA(MATCH(D27,A:A,0),"")</f>
-        <v/>
+      <c r="C27" s="5" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>360</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>607</v>
+      <c r="C28" t="s">
+        <v>602</v>
       </c>
       <c r="E28" t="str">
         <f>_xlfn.IFNA(MATCH(D28,A:A,0),"")</f>
@@ -3065,7 +3078,7 @@
         <v>370</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="E29" t="str">
         <f>_xlfn.IFNA(MATCH(D29,A:A,0),"")</f>
@@ -3076,20 +3089,16 @@
       <c r="B30">
         <v>380</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>610</v>
-      </c>
-      <c r="E30" t="str">
-        <f>_xlfn.IFNA(MATCH(D30,A:A,0),"")</f>
-        <v/>
+      <c r="C30" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>390</v>
       </c>
-      <c r="C31" t="s">
-        <v>9</v>
+      <c r="C31" s="5" t="s">
+        <v>604</v>
       </c>
       <c r="E31" t="str">
         <f>_xlfn.IFNA(MATCH(D31,A:A,0),"")</f>
@@ -3097,15 +3106,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="B32">
         <v>400</v>
       </c>
-      <c r="C32" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A32,"***")</f>
-        <v>REM SUBROUTINE ***SETCOLORSCHEME***</v>
+      <c r="C32" s="5" t="s">
+        <v>606</v>
       </c>
       <c r="E32" t="str">
         <f>_xlfn.IFNA(MATCH(D32,A:A,0),"")</f>
@@ -3116,8 +3121,8 @@
       <c r="B33">
         <v>410</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>599</v>
+      <c r="C33" t="s">
+        <v>9</v>
       </c>
       <c r="E33" t="str">
         <f>_xlfn.IFNA(MATCH(D33,A:A,0),"")</f>
@@ -3125,11 +3130,15 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="B34">
         <v>420</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>600</v>
+      <c r="C34" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A34,"***")</f>
+        <v>REM SUBROUTINE ***SETCOLORSCHEME***</v>
       </c>
       <c r="E34" t="str">
         <f>_xlfn.IFNA(MATCH(D34,A:A,0),"")</f>
@@ -3141,7 +3150,7 @@
         <v>430</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>601</v>
+        <v>718</v>
       </c>
       <c r="E35" t="str">
         <f>_xlfn.IFNA(MATCH(D35,A:A,0),"")</f>
@@ -3152,8 +3161,8 @@
       <c r="B36">
         <v>440</v>
       </c>
-      <c r="C36" t="s">
-        <v>602</v>
+      <c r="C36" s="5" t="s">
+        <v>720</v>
       </c>
       <c r="E36" t="str">
         <f>_xlfn.IFNA(MATCH(D36,A:A,0),"")</f>
@@ -3164,8 +3173,8 @@
       <c r="B37">
         <v>450</v>
       </c>
-      <c r="C37" t="s">
-        <v>603</v>
+      <c r="C37" s="5" t="s">
+        <v>719</v>
       </c>
       <c r="E37" t="str">
         <f>_xlfn.IFNA(MATCH(D37,A:A,0),"")</f>
@@ -3176,24 +3185,16 @@
       <c r="B38">
         <v>460</v>
       </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" t="str">
-        <f>_xlfn.IFNA(MATCH(D38,A:A,0),"")</f>
-        <v/>
+      <c r="C38" s="5" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>616</v>
-      </c>
       <c r="B39">
         <v>470</v>
       </c>
-      <c r="C39" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A39,"***")</f>
-        <v>REM SUBROUTINE ***RENDERBOARDS***</v>
+      <c r="C39" t="s">
+        <v>599</v>
       </c>
       <c r="E39" t="str">
         <f>_xlfn.IFNA(MATCH(D39,A:A,0),"")</f>
@@ -3205,7 +3206,7 @@
         <v>480</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E40" t="str">
         <f>_xlfn.IFNA(MATCH(D40,A:A,0),"")</f>
@@ -3217,7 +3218,7 @@
         <v>490</v>
       </c>
       <c r="C41" t="s">
-        <v>571</v>
+        <v>9</v>
       </c>
       <c r="E41" t="str">
         <f>_xlfn.IFNA(MATCH(D41,A:A,0),"")</f>
@@ -3225,152 +3226,147 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>612</v>
+      </c>
       <c r="B42">
         <v>500</v>
       </c>
       <c r="C42" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D42,A:A,0),0)," :: REM CALL ",D42,"")</f>
-        <v>GOSUB 580 :: REM CALL RENDERBOARD</v>
-      </c>
-      <c r="D42" t="str">
-        <f>A50</f>
-        <v>RENDERBOARD</v>
-      </c>
-      <c r="E42">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A42,"***")</f>
+        <v>REM SUBROUTINE ***RENDERBOARDS***</v>
+      </c>
+      <c r="E42" t="str">
         <f>_xlfn.IFNA(MATCH(D42,A:A,0),"")</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43">
         <v>510</v>
       </c>
-      <c r="C43" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D43,A:A,0),0)," :: REM CALL ",D43,"")</f>
-        <v>GOSUB 660 :: REM CALL RENDERAXES</v>
-      </c>
-      <c r="D43" t="str">
-        <f>A58</f>
-        <v>RENDERAXES</v>
-      </c>
-      <c r="E43">
+      <c r="C43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="str">
         <f>_xlfn.IFNA(MATCH(D43,A:A,0),"")</f>
-        <v>58</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44">
         <v>520</v>
       </c>
-      <c r="C44" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D44,A:A,0),0)," :: REM CALL ",D44,"")</f>
-        <v>GOSUB 770 :: REM CALL RENDERAUX</v>
-      </c>
-      <c r="D44" t="str">
-        <f>A69</f>
-        <v>RENDERAUX</v>
-      </c>
-      <c r="E44">
+      <c r="C44" t="s">
+        <v>571</v>
+      </c>
+      <c r="E44" t="str">
         <f>_xlfn.IFNA(MATCH(D44,A:A,0),"")</f>
-        <v>69</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45">
         <v>530</v>
       </c>
-      <c r="C45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" t="str">
+      <c r="C45" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D45,A:A,0),0)," :: REM CALL ",D45,"")</f>
+        <v>GOSUB 600 :: REM CALL RENDERBOARD</v>
+      </c>
+      <c r="D45" t="str">
+        <f>A52</f>
+        <v>RENDERBOARD</v>
+      </c>
+      <c r="E45">
         <f>_xlfn.IFNA(MATCH(D45,A:A,0),"")</f>
-        <v/>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>614</v>
-      </c>
       <c r="B46">
         <v>540</v>
       </c>
       <c r="C46" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A46,"***")</f>
-        <v>REM SUBROUTINE ***DEPLOYSHIPS***</v>
-      </c>
-      <c r="E46" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D46,A:A,0),0)," :: REM CALL ",D46,"")</f>
+        <v>GOSUB 900 :: REM CALL RENDERAUX</v>
+      </c>
+      <c r="D46" t="str">
+        <f>A82</f>
+        <v>RENDERAUX</v>
+      </c>
+      <c r="E46">
         <f>_xlfn.IFNA(MATCH(D46,A:A,0),"")</f>
-        <v/>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B47">
         <v>550</v>
       </c>
-      <c r="C47" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D47,A:A,0),0)," :: REM CALL ",D47,"")</f>
-        <v>GOSUB 830 :: REM CALL PLAYERDELOY</v>
-      </c>
-      <c r="D47" t="str">
-        <f>A75</f>
-        <v>PLAYERDELOY</v>
-      </c>
-      <c r="E47">
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="str">
         <f>_xlfn.IFNA(MATCH(D47,A:A,0),"")</f>
-        <v>75</v>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>610</v>
+      </c>
       <c r="B48">
         <v>560</v>
       </c>
       <c r="C48" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D48,A:A,0),0)," :: REM CALL ",D48,"")</f>
-        <v>GOSUB 1200 :: REM CALL COMPUTERDEPLOY</v>
-      </c>
-      <c r="D48" t="str">
-        <f>A112</f>
-        <v>COMPUTERDEPLOY</v>
-      </c>
-      <c r="E48">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A48,"***")</f>
+        <v>REM SUBROUTINE ***DEPLOYSHIPS***</v>
+      </c>
+      <c r="E48" t="str">
         <f>_xlfn.IFNA(MATCH(D48,A:A,0),"")</f>
-        <v>112</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49">
         <v>570</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" t="str">
+      <c r="C49" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D49,A:A,0),0)," :: REM CALL ",D49,"")</f>
+        <v>GOSUB 960 :: REM CALL PLAYERDELOY</v>
+      </c>
+      <c r="D49" t="str">
+        <f>A88</f>
+        <v>PLAYERDELOY</v>
+      </c>
+      <c r="E49">
         <f>_xlfn.IFNA(MATCH(D49,A:A,0),"")</f>
-        <v/>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>692</v>
-      </c>
       <c r="B50">
         <v>580</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A50,"***")</f>
-        <v>REM SUBROUTINE ***RENDERBOARD***</v>
-      </c>
-      <c r="E50" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D50,A:A,0),0)," :: REM CALL ",D50,"")</f>
+        <v>GOSUB 1330 :: REM CALL COMPUTERDEPLOY</v>
+      </c>
+      <c r="D50" t="str">
+        <f>A125</f>
+        <v>COMPUTERDEPLOY</v>
+      </c>
+      <c r="E50">
         <f>_xlfn.IFNA(MATCH(D50,A:A,0),"")</f>
-        <v/>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51">
         <v>590</v>
       </c>
-      <c r="C51" t="s">
-        <v>698</v>
+      <c r="C51" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E51" t="str">
         <f>_xlfn.IFNA(MATCH(D51,A:A,0),"")</f>
@@ -3378,11 +3374,15 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>688</v>
+      </c>
       <c r="B52">
         <v>600</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>617</v>
+      <c r="C52" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A52,"***")</f>
+        <v>REM SUBROUTINE ***RENDERBOARD***</v>
       </c>
       <c r="E52" t="str">
         <f>_xlfn.IFNA(MATCH(D52,A:A,0),"")</f>
@@ -3393,72 +3393,67 @@
       <c r="B53">
         <v>610</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="E53" t="str">
-        <f>_xlfn.IFNA(MATCH(D53,A:A,0),"")</f>
-        <v/>
+      <c r="C53" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D53,A:A,0),0)," :: REM CALL ",D53,"")</f>
+        <v>GOSUB 650 :: REM CALL RENDERBACKBOARD</v>
+      </c>
+      <c r="D53" t="str">
+        <f>A57</f>
+        <v>RENDERBACKBOARD</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>620</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>623</v>
-      </c>
-      <c r="E54" t="str">
-        <f>_xlfn.IFNA(MATCH(D54,A:A,0),"")</f>
-        <v/>
+      <c r="C54" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D54,A:A,0),0)," :: REM CALL ",D54,"")</f>
+        <v>GOSUB 790 :: REM CALL RENDERAXES</v>
+      </c>
+      <c r="D54" t="str">
+        <f>A71</f>
+        <v>RENDERAXES</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55">
         <v>630</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" t="str">
-        <f>_xlfn.IFNA(MATCH(D55,A:A,0),"")</f>
-        <v/>
+      <c r="C55" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D55,A:A,0),0)," :: REM CALL ",D55,"")</f>
+        <v>GOSUB 710 :: REM CALL RENDERHOLES</v>
+      </c>
+      <c r="D55" t="str">
+        <f>A63</f>
+        <v>RENDERHOLES</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56">
         <v>640</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" t="str">
-        <f>_xlfn.IFNA(MATCH(D56,A:A,0),"")</f>
-        <v/>
+      <c r="C56" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="17" t="s">
+        <v>722</v>
+      </c>
       <c r="B57">
         <v>650</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" t="str">
-        <f>_xlfn.IFNA(MATCH(D57,A:A,0),"")</f>
-        <v/>
+      <c r="C57" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A57,"***")</f>
+        <v>REM SUBROUTINE ***RENDERBACKBOARD***</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>693</v>
-      </c>
       <c r="B58">
         <v>660</v>
       </c>
-      <c r="C58" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A58,"***")</f>
-        <v>REM SUBROUTINE ***RENDERAXES***</v>
+      <c r="C58" t="s">
+        <v>694</v>
       </c>
       <c r="E58" t="str">
         <f>_xlfn.IFNA(MATCH(D58,A:A,0),"")</f>
@@ -3469,12 +3464,8 @@
       <c r="B59">
         <v>670</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="E59" t="str">
-        <f>_xlfn.IFNA(MATCH(D59,A:A,0),"")</f>
-        <v/>
+      <c r="C59" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3482,11 +3473,7 @@
         <v>680</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="E60" t="str">
-        <f>_xlfn.IFNA(MATCH(D60,A:A,0),"")</f>
-        <v/>
+        <v>717</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -3494,11 +3481,7 @@
         <v>690</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="E61" t="str">
-        <f>_xlfn.IFNA(MATCH(D61,A:A,0),"")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -3506,35 +3489,27 @@
         <v>700</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E62" t="str">
-        <f>_xlfn.IFNA(MATCH(D62,A:A,0),"")</f>
-        <v/>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
+        <v>721</v>
+      </c>
       <c r="B63">
         <v>710</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="E63" t="str">
-        <f>_xlfn.IFNA(MATCH(D63,A:A,0),"")</f>
-        <v/>
+      <c r="C63" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A63,"***")</f>
+        <v>REM SUBROUTINE ***RENDERHOLES***</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64">
         <v>720</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="E64" t="str">
-        <f>_xlfn.IFNA(MATCH(D64,A:A,0),"")</f>
-        <v/>
+      <c r="C64" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -3542,7 +3517,7 @@
         <v>730</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>34</v>
+        <v>613</v>
       </c>
       <c r="E65" t="str">
         <f>_xlfn.IFNA(MATCH(D65,A:A,0),"")</f>
@@ -3554,7 +3529,7 @@
         <v>740</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>618</v>
+        <v>552</v>
       </c>
       <c r="E66" t="str">
         <f>_xlfn.IFNA(MATCH(D66,A:A,0),"")</f>
@@ -3566,7 +3541,7 @@
         <v>750</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>1</v>
+        <v>619</v>
       </c>
       <c r="E67" t="str">
         <f>_xlfn.IFNA(MATCH(D67,A:A,0),"")</f>
@@ -3578,7 +3553,7 @@
         <v>760</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E68" t="str">
         <f>_xlfn.IFNA(MATCH(D68,A:A,0),"")</f>
@@ -3586,15 +3561,11 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
-        <v>699</v>
-      </c>
       <c r="B69">
         <v>770</v>
       </c>
-      <c r="C69" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A69,"***")</f>
-        <v>REM SUBROUTINE ***RENDERAUX***</v>
+      <c r="C69" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="E69" t="str">
         <f>_xlfn.IFNA(MATCH(D69,A:A,0),"")</f>
@@ -3606,7 +3577,7 @@
         <v>780</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>695</v>
+        <v>9</v>
       </c>
       <c r="E70" t="str">
         <f>_xlfn.IFNA(MATCH(D70,A:A,0),"")</f>
@@ -3614,11 +3585,15 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>689</v>
+      </c>
       <c r="B71">
         <v>790</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>18</v>
+      <c r="C71" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A71,"***")</f>
+        <v>REM SUBROUTINE ***RENDERAXES***</v>
       </c>
       <c r="E71" t="str">
         <f>_xlfn.IFNA(MATCH(D71,A:A,0),"")</f>
@@ -3630,7 +3605,7 @@
         <v>800</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="E72" t="str">
         <f>_xlfn.IFNA(MATCH(D72,A:A,0),"")</f>
@@ -3642,7 +3617,7 @@
         <v>810</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>1</v>
+        <v>551</v>
       </c>
       <c r="E73" t="str">
         <f>_xlfn.IFNA(MATCH(D73,A:A,0),"")</f>
@@ -3654,7 +3629,7 @@
         <v>820</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>9</v>
+        <v>617</v>
       </c>
       <c r="E74" t="str">
         <f>_xlfn.IFNA(MATCH(D74,A:A,0),"")</f>
@@ -3662,15 +3637,11 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
-        <v>685</v>
-      </c>
       <c r="B75">
         <v>830</v>
       </c>
-      <c r="C75" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A75,"***")</f>
-        <v>REM SUBROUTINE ***PLAYERDELOY***</v>
+      <c r="C75" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="E75" t="str">
         <f>_xlfn.IFNA(MATCH(D75,A:A,0),"")</f>
@@ -3681,17 +3652,12 @@
       <c r="B76">
         <v>840</v>
       </c>
-      <c r="C76" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D76,A:A,0),0)," :: REM CALL ",D76,"")</f>
-        <v>GOSUB 1400 :: REM CALL CLEARMENU</v>
-      </c>
-      <c r="D76" t="str">
-        <f>A132</f>
-        <v>CLEARMENU</v>
-      </c>
-      <c r="E76">
+      <c r="C76" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="E76" t="str">
         <f>_xlfn.IFNA(MATCH(D76,A:A,0),"")</f>
-        <v>132</v>
+        <v/>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -3699,7 +3665,7 @@
         <v>850</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>664</v>
+        <v>615</v>
       </c>
       <c r="E77" t="str">
         <f>_xlfn.IFNA(MATCH(D77,A:A,0),"")</f>
@@ -3711,7 +3677,7 @@
         <v>860</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>665</v>
+        <v>34</v>
       </c>
       <c r="E78" t="str">
         <f>_xlfn.IFNA(MATCH(D78,A:A,0),"")</f>
@@ -3723,7 +3689,7 @@
         <v>870</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>666</v>
+        <v>614</v>
       </c>
       <c r="E79" t="str">
         <f>_xlfn.IFNA(MATCH(D79,A:A,0),"")</f>
@@ -3735,7 +3701,7 @@
         <v>880</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>677</v>
+        <v>1</v>
       </c>
       <c r="E80" t="str">
         <f>_xlfn.IFNA(MATCH(D80,A:A,0),"")</f>
@@ -3747,7 +3713,7 @@
         <v>890</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>678</v>
+        <v>9</v>
       </c>
       <c r="E81" t="str">
         <f>_xlfn.IFNA(MATCH(D81,A:A,0),"")</f>
@@ -3755,11 +3721,15 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>695</v>
+      </c>
       <c r="B82">
         <v>900</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>679</v>
+      <c r="C82" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A82,"***")</f>
+        <v>REM SUBROUTINE ***RENDERAUX***</v>
       </c>
       <c r="E82" t="str">
         <f>_xlfn.IFNA(MATCH(D82,A:A,0),"")</f>
@@ -3770,13 +3740,12 @@
       <c r="B83">
         <v>910</v>
       </c>
-      <c r="C83" s="5" t="str">
-        <f>_xlfn.CONCAT("IF AUTODEPLOY$=""N"" THEN ",INDEX(B:B,MATCH(D83,A:A,0),0)," :: REM GOTO ",D83,"")</f>
-        <v>IF AUTODEPLOY$="N" THEN 1020 :: REM GOTO PLAYERDEPLOYSHIPS</v>
-      </c>
-      <c r="D83" t="str">
-        <f>A94</f>
-        <v>PLAYERDEPLOYSHIPS</v>
+      <c r="C83" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="E83" t="str">
+        <f>_xlfn.IFNA(MATCH(D83,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -3784,7 +3753,11 @@
         <v>920</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>714</v>
+        <v>18</v>
+      </c>
+      <c r="E84" t="str">
+        <f>_xlfn.IFNA(MATCH(D84,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -3792,7 +3765,11 @@
         <v>930</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>715</v>
+        <v>605</v>
+      </c>
+      <c r="E85" t="str">
+        <f>_xlfn.IFNA(MATCH(D85,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -3800,32 +3777,35 @@
         <v>940</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>716</v>
+        <v>1</v>
+      </c>
+      <c r="E86" t="str">
+        <f>_xlfn.IFNA(MATCH(D86,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B87">
         <v>950</v>
       </c>
-      <c r="C87" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D87,A:A,0),0)," :: REM CALL ",D87,"")</f>
-        <v>GOSUB 1200 :: REM CALL COMPUTERDEPLOY</v>
-      </c>
-      <c r="D87" t="str">
-        <f>A112</f>
-        <v>COMPUTERDEPLOY</v>
-      </c>
-      <c r="E87">
+      <c r="C87" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="str">
         <f>_xlfn.IFNA(MATCH(D87,A:A,0),"")</f>
-        <v>112</v>
+        <v/>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="17" t="s">
+        <v>681</v>
+      </c>
       <c r="B88">
         <v>960</v>
       </c>
-      <c r="C88" s="5" t="s">
-        <v>625</v>
+      <c r="C88" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A88,"***")</f>
+        <v>REM SUBROUTINE ***PLAYERDELOY***</v>
       </c>
       <c r="E88" t="str">
         <f>_xlfn.IFNA(MATCH(D88,A:A,0),"")</f>
@@ -3836,12 +3816,17 @@
       <c r="B89">
         <v>970</v>
       </c>
-      <c r="C89" t="s">
-        <v>670</v>
-      </c>
-      <c r="E89" t="str">
+      <c r="C89" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D89,A:A,0),0)," :: REM CALL ",D89,"")</f>
+        <v>GOSUB 1530 :: REM CALL CLEARMENU</v>
+      </c>
+      <c r="D89" t="str">
+        <f>A145</f>
+        <v>CLEARMENU</v>
+      </c>
+      <c r="E89">
         <f>_xlfn.IFNA(MATCH(D89,A:A,0),"")</f>
-        <v/>
+        <v>145</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -3849,7 +3834,7 @@
         <v>980</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
       <c r="E90" t="str">
         <f>_xlfn.IFNA(MATCH(D90,A:A,0),"")</f>
@@ -3861,7 +3846,7 @@
         <v>990</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>17</v>
+        <v>661</v>
       </c>
       <c r="E91" t="str">
         <f>_xlfn.IFNA(MATCH(D91,A:A,0),"")</f>
@@ -3873,7 +3858,7 @@
         <v>1000</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>1</v>
+        <v>662</v>
       </c>
       <c r="E92" t="str">
         <f>_xlfn.IFNA(MATCH(D92,A:A,0),"")</f>
@@ -3884,25 +3869,20 @@
       <c r="B93">
         <v>1010</v>
       </c>
-      <c r="C93" s="5" t="str">
-        <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D93,A:A,0),0)," :: REM GOTO ",D93,"")</f>
-        <v>GOTO 1160 :: REM GOTO PLAYERRENDERSHIPS</v>
-      </c>
-      <c r="D93" t="str">
-        <f>A108</f>
-        <v>PLAYERRENDERSHIPS</v>
+      <c r="C93" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="E93" t="str">
+        <f>_xlfn.IFNA(MATCH(D93,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="19" t="s">
-        <v>686</v>
-      </c>
       <c r="B94">
         <v>1020</v>
       </c>
-      <c r="C94" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A94,"***")</f>
-        <v>REM LABEL ***PLAYERDEPLOYSHIPS***</v>
+      <c r="C94" s="5" t="s">
+        <v>674</v>
       </c>
       <c r="E94" t="str">
         <f>_xlfn.IFNA(MATCH(D94,A:A,0),"")</f>
@@ -3910,126 +3890,93 @@
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="19"/>
       <c r="B95">
         <v>1030</v>
       </c>
-      <c r="C95" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D95,A:A,0),0)," :: REM CALL ",D95,"")</f>
-        <v>GOSUB 1400 :: REM CALL CLEARMENU</v>
-      </c>
-      <c r="D95" t="str">
-        <f>A132</f>
-        <v>CLEARMENU</v>
-      </c>
-      <c r="E95">
+      <c r="C95" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="E95" t="str">
         <f>_xlfn.IFNA(MATCH(D95,A:A,0),"")</f>
-        <v>132</v>
+        <v/>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="19"/>
       <c r="B96">
         <v>1040</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>624</v>
-      </c>
-      <c r="E96" t="str">
-        <f>_xlfn.IFNA(MATCH(D96,A:A,0),"")</f>
-        <v/>
+      <c r="C96" s="5" t="str">
+        <f>_xlfn.CONCAT("IF AUTODEPLOY$=""N"" THEN ",INDEX(B:B,MATCH(D96,A:A,0),0)," :: REM GOTO ",D96,"")</f>
+        <v>IF AUTODEPLOY$="N" THEN 1150 :: REM GOTO PLAYERDEPLOYSHIPS</v>
+      </c>
+      <c r="D96" t="str">
+        <f>A107</f>
+        <v>PLAYERDEPLOYSHIPS</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="19" t="s">
-        <v>687</v>
-      </c>
       <c r="B97">
         <v>1050</v>
       </c>
-      <c r="C97" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A97,"***")</f>
-        <v>REM LABEL ***PLAYERDEPLOYSHIP***</v>
-      </c>
-      <c r="E97" t="str">
-        <f>_xlfn.IFNA(MATCH(D97,A:A,0),"")</f>
-        <v/>
+      <c r="C97" s="5" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98">
         <v>1060</v>
       </c>
-      <c r="C98" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D98,A:A,0),0)," :: REM CALL ",D98,"")</f>
-        <v>GOSUB 1430 :: REM CALL PLAYERDEPLOYMENU</v>
-      </c>
-      <c r="D98" t="str">
-        <f>A135</f>
-        <v>PLAYERDEPLOYMENU</v>
-      </c>
-      <c r="E98">
-        <f>_xlfn.IFNA(MATCH(D98,A:A,0),"")</f>
-        <v>135</v>
+      <c r="C98" s="5" t="s">
+        <v>711</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99">
         <v>1070</v>
       </c>
-      <c r="C99" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D99,A:A,0),0)," :: REM CALL ",D99,"")</f>
-        <v>GOSUB 1550 :: REM CALL PLAYERDEPLOYINPUT</v>
-      </c>
-      <c r="D99" t="str">
-        <f>A147</f>
-        <v>PLAYERDEPLOYINPUT</v>
-      </c>
-      <c r="E99">
-        <f>_xlfn.IFNA(MATCH(D99,A:A,0),"")</f>
-        <v>147</v>
+      <c r="C99" s="5" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100">
         <v>1080</v>
       </c>
-      <c r="C100" t="s">
-        <v>708</v>
-      </c>
-      <c r="E100" t="str">
+      <c r="C100" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D100,A:A,0),0)," :: REM CALL ",D100,"")</f>
+        <v>GOSUB 1330 :: REM CALL COMPUTERDEPLOY</v>
+      </c>
+      <c r="D100" t="str">
+        <f>A125</f>
+        <v>COMPUTERDEPLOY</v>
+      </c>
+      <c r="E100">
         <f>_xlfn.IFNA(MATCH(D100,A:A,0),"")</f>
-        <v/>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B101">
         <v>1090</v>
       </c>
-      <c r="C101" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D101,A:A,0),0)," :: REM CALL ",D101,"")</f>
-        <v>GOSUB 1680 :: REM CALL VALIDATESHIP</v>
-      </c>
-      <c r="D101" t="str">
-        <f>A160</f>
-        <v>VALIDATESHIP</v>
-      </c>
-      <c r="E101">
+      <c r="C101" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="E101" t="str">
         <f>_xlfn.IFNA(MATCH(D101,A:A,0),"")</f>
-        <v>160</v>
+        <v/>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B102">
         <v>1100</v>
       </c>
-      <c r="C102" s="5" t="str">
-        <f>_xlfn.CONCAT("IF SHIPERR=1 THEN ",INDEX(B:B,MATCH(D102,A:A,0),0)," :: REM GOTO ",D102,"")</f>
-        <v>IF SHIPERR=1 THEN 1050 :: REM GOTO PLAYERDEPLOYSHIP</v>
-      </c>
-      <c r="D102" t="str">
-        <f>A97</f>
-        <v>PLAYERDEPLOYSHIP</v>
+      <c r="C102" t="s">
+        <v>666</v>
+      </c>
+      <c r="E102" t="str">
+        <f>_xlfn.IFNA(MATCH(D102,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -4037,7 +3984,7 @@
         <v>1110</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="E103" t="str">
         <f>_xlfn.IFNA(MATCH(D103,A:A,0),"")</f>
@@ -4049,7 +3996,7 @@
         <v>1120</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>680</v>
+        <v>17</v>
       </c>
       <c r="E104" t="str">
         <f>_xlfn.IFNA(MATCH(D104,A:A,0),"")</f>
@@ -4072,25 +4019,25 @@
       <c r="B106">
         <v>1140</v>
       </c>
-      <c r="C106" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D106,A:A,0),0)," :: REM CALL ",D106,"")</f>
-        <v>GOSUB 1780 :: REM CALL RENDERSHIP</v>
+      <c r="C106" s="5" t="str">
+        <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D106,A:A,0),0)," :: REM GOTO ",D106,"")</f>
+        <v>GOTO 1290 :: REM GOTO PLAYERRENDERSHIPS</v>
       </c>
       <c r="D106" t="str">
-        <f>A170</f>
-        <v>RENDERSHIP</v>
-      </c>
-      <c r="E106">
-        <f>_xlfn.IFNA(MATCH(D106,A:A,0),"")</f>
-        <v>170</v>
+        <f>A121</f>
+        <v>PLAYERRENDERSHIPS</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="19" t="s">
+        <v>682</v>
+      </c>
       <c r="B107">
         <v>1150</v>
       </c>
-      <c r="C107" s="5" t="s">
-        <v>556</v>
+      <c r="C107" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A107,"***")</f>
+        <v>REM LABEL ***PLAYERDEPLOYSHIPS***</v>
       </c>
       <c r="E107" t="str">
         <f>_xlfn.IFNA(MATCH(D107,A:A,0),"")</f>
@@ -4098,85 +4045,84 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="19" t="s">
-        <v>688</v>
-      </c>
+      <c r="A108" s="19"/>
       <c r="B108">
         <v>1160</v>
       </c>
       <c r="C108" t="str">
         <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D108,A:A,0),0)," :: REM CALL ",D108,"")</f>
-        <v>GOSUB 1840 :: REM CALL RENDERSHIPSAUX</v>
+        <v>GOSUB 1530 :: REM CALL CLEARMENU</v>
       </c>
       <c r="D108" t="str">
-        <f>A176</f>
-        <v>RENDERSHIPSAUX</v>
+        <f>A145</f>
+        <v>CLEARMENU</v>
       </c>
       <c r="E108">
         <f>_xlfn.IFNA(MATCH(D108,A:A,0),"")</f>
-        <v>176</v>
+        <v>145</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="19"/>
       <c r="B109">
         <v>1170</v>
       </c>
-      <c r="C109" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D109,A:A,0),0)," :: REM CALL ",D109,"")</f>
-        <v>GOSUB 580 :: REM CALL RENDERBOARD</v>
-      </c>
-      <c r="D109" t="str">
-        <f>A50</f>
-        <v>RENDERBOARD</v>
-      </c>
-      <c r="E109">
+      <c r="C109" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="E109" t="str">
         <f>_xlfn.IFNA(MATCH(D109,A:A,0),"")</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="19" t="s">
+        <v>683</v>
+      </c>
       <c r="B110">
         <v>1180</v>
       </c>
-      <c r="C110" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D110,A:A,0),0)," :: REM CALL ",D110,"")</f>
-        <v>GOSUB 1920 :: REM CALL PLAYERDEPLOYED</v>
-      </c>
-      <c r="D110" t="str">
-        <f>A184</f>
-        <v>PLAYERDEPLOYED</v>
-      </c>
-      <c r="E110">
+      <c r="C110" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A110,"***")</f>
+        <v>REM LABEL ***PLAYERDEPLOYSHIP***</v>
+      </c>
+      <c r="E110" t="str">
         <f>_xlfn.IFNA(MATCH(D110,A:A,0),"")</f>
-        <v>184</v>
+        <v/>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B111">
         <v>1190</v>
       </c>
-      <c r="C111" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" t="str">
+      <c r="C111" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D111,A:A,0),0)," :: REM CALL ",D111,"")</f>
+        <v>GOSUB 1560 :: REM CALL PLAYERDEPLOYMENU</v>
+      </c>
+      <c r="D111" t="str">
+        <f>A148</f>
+        <v>PLAYERDEPLOYMENU</v>
+      </c>
+      <c r="E111">
         <f>_xlfn.IFNA(MATCH(D111,A:A,0),"")</f>
-        <v/>
+        <v>148</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
-        <v>689</v>
-      </c>
       <c r="B112">
         <v>1200</v>
       </c>
       <c r="C112" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A112,"***")</f>
-        <v>REM SUBROUTINE ***COMPUTERDEPLOY***</v>
-      </c>
-      <c r="E112" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D112,A:A,0),0)," :: REM CALL ",D112,"")</f>
+        <v>GOSUB 1680 :: REM CALL PLAYERDEPLOYINPUT</v>
+      </c>
+      <c r="D112" t="str">
+        <f>A160</f>
+        <v>PLAYERDEPLOYINPUT</v>
+      </c>
+      <c r="E112">
         <f>_xlfn.IFNA(MATCH(D112,A:A,0),"")</f>
-        <v/>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -4184,7 +4130,7 @@
         <v>1210</v>
       </c>
       <c r="C113" t="s">
-        <v>624</v>
+        <v>704</v>
       </c>
       <c r="E113" t="str">
         <f>_xlfn.IFNA(MATCH(D113,A:A,0),"")</f>
@@ -4192,39 +4138,41 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="19" t="s">
-        <v>707</v>
-      </c>
       <c r="B114">
         <v>1220</v>
       </c>
-      <c r="C114" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A114,"***")</f>
-        <v>REM LABEL ***COMPUTERDEPLOYSHIP***</v>
-      </c>
-      <c r="E114" t="str">
+      <c r="C114" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D114,A:A,0),0)," :: REM CALL ",D114,"")</f>
+        <v>GOSUB 1810 :: REM CALL VALIDATESHIP</v>
+      </c>
+      <c r="D114" t="str">
+        <f>A173</f>
+        <v>VALIDATESHIP</v>
+      </c>
+      <c r="E114">
         <f>_xlfn.IFNA(MATCH(D114,A:A,0),"")</f>
-        <v/>
+        <v>173</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B115">
         <v>1230</v>
       </c>
-      <c r="C115" t="s">
-        <v>704</v>
-      </c>
-      <c r="E115" t="str">
-        <f>_xlfn.IFNA(MATCH(D115,A:A,0),"")</f>
-        <v/>
+      <c r="C115" s="5" t="str">
+        <f>_xlfn.CONCAT("IF SHIPERR=1 THEN ",INDEX(B:B,MATCH(D115,A:A,0),0)," :: REM GOTO ",D115,"")</f>
+        <v>IF SHIPERR=1 THEN 1180 :: REM GOTO PLAYERDEPLOYSHIP</v>
+      </c>
+      <c r="D115" t="str">
+        <f>A110</f>
+        <v>PLAYERDEPLOYSHIP</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B116">
         <v>1240</v>
       </c>
-      <c r="C116" t="s">
-        <v>711</v>
+      <c r="C116" s="5" t="s">
+        <v>664</v>
       </c>
       <c r="E116" t="str">
         <f>_xlfn.IFNA(MATCH(D116,A:A,0),"")</f>
@@ -4235,8 +4183,8 @@
       <c r="B117">
         <v>1250</v>
       </c>
-      <c r="C117" t="s">
-        <v>705</v>
+      <c r="C117" s="5" t="s">
+        <v>676</v>
       </c>
       <c r="E117" t="str">
         <f>_xlfn.IFNA(MATCH(D117,A:A,0),"")</f>
@@ -4247,8 +4195,8 @@
       <c r="B118">
         <v>1260</v>
       </c>
-      <c r="C118" t="s">
-        <v>668</v>
+      <c r="C118" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="E118" t="str">
         <f>_xlfn.IFNA(MATCH(D118,A:A,0),"")</f>
@@ -4259,20 +4207,25 @@
       <c r="B119">
         <v>1270</v>
       </c>
-      <c r="C119" t="s">
-        <v>713</v>
-      </c>
-      <c r="E119" t="str">
+      <c r="C119" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D119,A:A,0),0)," :: REM CALL ",D119,"")</f>
+        <v>GOSUB 1910 :: REM CALL RENDERSHIP</v>
+      </c>
+      <c r="D119" t="str">
+        <f>A183</f>
+        <v>RENDERSHIP</v>
+      </c>
+      <c r="E119">
         <f>_xlfn.IFNA(MATCH(D119,A:A,0),"")</f>
-        <v/>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B120">
         <v>1280</v>
       </c>
-      <c r="C120" t="s">
-        <v>706</v>
+      <c r="C120" s="5" t="s">
+        <v>556</v>
       </c>
       <c r="E120" t="str">
         <f>_xlfn.IFNA(MATCH(D120,A:A,0),"")</f>
@@ -4280,290 +4233,308 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="19" t="s">
+        <v>684</v>
+      </c>
       <c r="B121">
         <v>1290</v>
       </c>
-      <c r="C121" t="s">
-        <v>1</v>
-      </c>
-      <c r="E121" t="str">
+      <c r="C121" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D121,A:A,0),0)," :: REM CALL ",D121,"")</f>
+        <v>GOSUB 1970 :: REM CALL RENDERSHIPSAUX</v>
+      </c>
+      <c r="D121" t="str">
+        <f>A189</f>
+        <v>RENDERSHIPSAUX</v>
+      </c>
+      <c r="E121">
         <f>_xlfn.IFNA(MATCH(D121,A:A,0),"")</f>
-        <v/>
+        <v>189</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B122">
         <v>1300</v>
       </c>
-      <c r="C122" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="E122" t="str">
+      <c r="C122" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D122,A:A,0),0)," :: REM CALL ",D122,"")</f>
+        <v>GOSUB 710 :: REM CALL RENDERHOLES</v>
+      </c>
+      <c r="D122" t="str">
+        <f>A63</f>
+        <v>RENDERHOLES</v>
+      </c>
+      <c r="E122">
         <f>_xlfn.IFNA(MATCH(D122,A:A,0),"")</f>
-        <v/>
+        <v>63</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B123">
         <v>1310</v>
       </c>
-      <c r="C123" s="5" t="s">
-        <v>710</v>
-      </c>
-      <c r="E123" t="str">
+      <c r="C123" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D123,A:A,0),0)," :: REM CALL ",D123,"")</f>
+        <v>GOSUB 2050 :: REM CALL PLAYERDEPLOYED</v>
+      </c>
+      <c r="D123" t="str">
+        <f>A197</f>
+        <v>PLAYERDEPLOYED</v>
+      </c>
+      <c r="E123">
         <f>_xlfn.IFNA(MATCH(D123,A:A,0),"")</f>
-        <v/>
+        <v>197</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B124">
         <v>1320</v>
       </c>
-      <c r="C124" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D124,A:A,0),0)," :: REM CALL ",D124,"")</f>
-        <v>GOSUB 2010 :: REM CALL CHECKOVERLAP</v>
-      </c>
-      <c r="D124" t="str">
-        <f>A193</f>
-        <v>CHECKOVERLAP</v>
-      </c>
-      <c r="E124">
+      <c r="C124" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" t="str">
         <f>_xlfn.IFNA(MATCH(D124,A:A,0),"")</f>
-        <v>193</v>
+        <v/>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="17" t="s">
+        <v>685</v>
+      </c>
       <c r="B125">
         <v>1330</v>
       </c>
       <c r="C125" t="str">
-        <f>_xlfn.CONCAT("IF SHIPERR=1 THEN ",INDEX(B:B,MATCH(D125,A:A,0),0)," :: REM GOTO ",D125,"")</f>
-        <v>IF SHIPERR=1 THEN 1220 :: REM GOTO COMPUTERDEPLOYSHIP</v>
-      </c>
-      <c r="D125" t="str">
-        <f>A114</f>
-        <v>COMPUTERDEPLOYSHIP</v>
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A125,"***")</f>
+        <v>REM SUBROUTINE ***COMPUTERDEPLOY***</v>
+      </c>
+      <c r="E125" t="str">
+        <f>_xlfn.IFNA(MATCH(D125,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B126">
         <v>1340</v>
       </c>
-      <c r="C126" s="5" t="s">
-        <v>668</v>
+      <c r="C126" t="s">
+        <v>620</v>
+      </c>
+      <c r="E126" t="str">
+        <f>_xlfn.IFNA(MATCH(D126,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="19" t="s">
+        <v>703</v>
+      </c>
       <c r="B127">
         <v>1350</v>
       </c>
-      <c r="C127" s="5" t="s">
-        <v>712</v>
+      <c r="C127" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A127,"***")</f>
+        <v>REM LABEL ***COMPUTERDEPLOYSHIP***</v>
+      </c>
+      <c r="E127" t="str">
+        <f>_xlfn.IFNA(MATCH(D127,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B128">
         <v>1360</v>
       </c>
-      <c r="C128" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C128" t="s">
+        <v>700</v>
+      </c>
+      <c r="E128" t="str">
+        <f>_xlfn.IFNA(MATCH(D128,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B129">
         <v>1370</v>
       </c>
-      <c r="C129" t="str">
-        <f>_xlfn.CONCAT("IF DEBUG=1 THEN GOSUB ",INDEX(B:B,MATCH(D129,A:A,0),0)," :: REM CALL ",D129,"")</f>
-        <v>IF DEBUG=1 THEN GOSUB 1780 :: REM CALL RENDERSHIP</v>
-      </c>
-      <c r="D129" t="str">
-        <f>A170</f>
-        <v>RENDERSHIP</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C129" t="s">
+        <v>707</v>
+      </c>
+      <c r="E129" t="str">
+        <f>_xlfn.IFNA(MATCH(D129,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B130">
         <v>1380</v>
       </c>
       <c r="C130" t="s">
-        <v>556</v>
+        <v>701</v>
       </c>
       <c r="E130" t="str">
         <f>_xlfn.IFNA(MATCH(D130,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B131">
         <v>1390</v>
       </c>
-      <c r="C131" s="5" t="s">
-        <v>9</v>
+      <c r="C131" t="s">
+        <v>664</v>
       </c>
       <c r="E131" t="str">
         <f>_xlfn.IFNA(MATCH(D131,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="17" t="s">
-        <v>595</v>
-      </c>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B132">
         <v>1400</v>
       </c>
-      <c r="C132" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A132,"***")</f>
-        <v>REM SUBROUTINE ***CLEARMENU***</v>
+      <c r="C132" t="s">
+        <v>709</v>
       </c>
       <c r="E132" t="str">
         <f>_xlfn.IFNA(MATCH(D132,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B133">
         <v>1410</v>
       </c>
-      <c r="C133" s="5" t="s">
-        <v>596</v>
+      <c r="C133" t="s">
+        <v>702</v>
       </c>
       <c r="E133" t="str">
         <f>_xlfn.IFNA(MATCH(D133,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B134">
         <v>1420</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>9</v>
+      <c r="C134" t="s">
+        <v>1</v>
       </c>
       <c r="E134" t="str">
         <f>_xlfn.IFNA(MATCH(D134,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="17" t="s">
-        <v>690</v>
-      </c>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B135">
         <v>1430</v>
       </c>
-      <c r="C135" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A135,"***")</f>
-        <v>REM SUBROUTINE ***PLAYERDEPLOYMENU***</v>
+      <c r="C135" s="5" t="s">
+        <v>576</v>
       </c>
       <c r="E135" t="str">
         <f>_xlfn.IFNA(MATCH(D135,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B136">
         <v>1440</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>567</v>
+        <v>706</v>
       </c>
       <c r="E136" t="str">
         <f>_xlfn.IFNA(MATCH(D136,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B137">
         <v>1450</v>
       </c>
-      <c r="C137" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="E137" t="str">
+      <c r="C137" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D137,A:A,0),0)," :: REM CALL ",D137,"")</f>
+        <v>GOSUB 2140 :: REM CALL CHECKOVERLAP</v>
+      </c>
+      <c r="D137" t="str">
+        <f>A206</f>
+        <v>CHECKOVERLAP</v>
+      </c>
+      <c r="E137">
         <f>_xlfn.IFNA(MATCH(D137,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B138">
         <v>1460</v>
       </c>
-      <c r="C138" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="E138" t="str">
-        <f>_xlfn.IFNA(MATCH(D138,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C138" t="str">
+        <f>_xlfn.CONCAT("IF SHIPERR=1 THEN ",INDEX(B:B,MATCH(D138,A:A,0),0)," :: REM GOTO ",D138,"")</f>
+        <v>IF SHIPERR=1 THEN 1350 :: REM GOTO COMPUTERDEPLOYSHIP</v>
+      </c>
+      <c r="D138" t="str">
+        <f>A127</f>
+        <v>COMPUTERDEPLOYSHIP</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B139">
         <v>1470</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>570</v>
-      </c>
-      <c r="E139" t="str">
-        <f>_xlfn.IFNA(MATCH(D139,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B140">
         <v>1480</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>675</v>
-      </c>
-      <c r="E140" t="str">
-        <f>_xlfn.IFNA(MATCH(D140,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B141">
         <v>1490</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="E141" t="str">
-        <f>_xlfn.IFNA(MATCH(D141,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B142">
         <v>1500</v>
       </c>
-      <c r="C142" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E142" t="str">
-        <f>_xlfn.IFNA(MATCH(D142,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C142" t="str">
+        <f>_xlfn.CONCAT("IF DEBUG=1 THEN GOSUB ",INDEX(B:B,MATCH(D142,A:A,0),0)," :: REM CALL ",D142,"")</f>
+        <v>IF DEBUG=1 THEN GOSUB 1910 :: REM CALL RENDERSHIP</v>
+      </c>
+      <c r="D142" t="str">
+        <f>A183</f>
+        <v>RENDERSHIP</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B143">
         <v>1510</v>
       </c>
-      <c r="C143" s="5" t="s">
-        <v>669</v>
+      <c r="C143" t="s">
+        <v>556</v>
       </c>
       <c r="E143" t="str">
         <f>_xlfn.IFNA(MATCH(D143,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B144">
         <v>1520</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>597</v>
+        <v>9</v>
       </c>
       <c r="E144" t="str">
         <f>_xlfn.IFNA(MATCH(D144,A:A,0),"")</f>
@@ -4571,11 +4542,15 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="17" t="s">
+        <v>595</v>
+      </c>
       <c r="B145">
         <v>1530</v>
       </c>
-      <c r="C145" s="5" t="s">
-        <v>1</v>
+      <c r="C145" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A145,"***")</f>
+        <v>REM SUBROUTINE ***CLEARMENU***</v>
       </c>
       <c r="E145" t="str">
         <f>_xlfn.IFNA(MATCH(D145,A:A,0),"")</f>
@@ -4587,7 +4562,7 @@
         <v>1540</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>9</v>
+        <v>596</v>
       </c>
       <c r="E146" t="str">
         <f>_xlfn.IFNA(MATCH(D146,A:A,0),"")</f>
@@ -4595,15 +4570,11 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="17" t="s">
-        <v>691</v>
-      </c>
       <c r="B147">
         <v>1550</v>
       </c>
-      <c r="C147" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A147,"***")</f>
-        <v>REM SUBROUTINE ***PLAYERDEPLOYINPUT***</v>
+      <c r="C147" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E147" t="str">
         <f>_xlfn.IFNA(MATCH(D147,A:A,0),"")</f>
@@ -4611,11 +4582,15 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="17" t="s">
+        <v>686</v>
+      </c>
       <c r="B148">
         <v>1560</v>
       </c>
-      <c r="C148" s="5" t="s">
-        <v>25</v>
+      <c r="C148" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A148,"***")</f>
+        <v>REM SUBROUTINE ***PLAYERDEPLOYMENU***</v>
       </c>
       <c r="E148" t="str">
         <f>_xlfn.IFNA(MATCH(D148,A:A,0),"")</f>
@@ -4627,7 +4602,7 @@
         <v>1570</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>668</v>
+        <v>567</v>
       </c>
       <c r="E149" t="str">
         <f>_xlfn.IFNA(MATCH(D149,A:A,0),"")</f>
@@ -4635,15 +4610,11 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="19" t="s">
-        <v>557</v>
-      </c>
       <c r="B150">
         <v>1580</v>
       </c>
-      <c r="C150" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A150,"***")</f>
-        <v>REM LABEL ***INPUTROW***</v>
+      <c r="C150" s="5" t="s">
+        <v>566</v>
       </c>
       <c r="E150" t="str">
         <f>_xlfn.IFNA(MATCH(D150,A:A,0),"")</f>
@@ -4655,7 +4626,7 @@
         <v>1590</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E151" t="str">
         <f>_xlfn.IFNA(MATCH(D151,A:A,0),"")</f>
@@ -4666,25 +4637,20 @@
       <c r="B152">
         <v>1600</v>
       </c>
-      <c r="C152" s="5" t="str">
-        <f>_xlfn.CONCAT("IF COORDS$(I)="""" THEN  ",INDEX(B:B,MATCH(D152,A:A,0),0)," :: REM GOTO ",D152,"")</f>
-        <v>IF COORDS$(I)="" THEN  1580 :: REM GOTO INPUTROW</v>
-      </c>
-      <c r="D152" t="str">
-        <f>A150</f>
-        <v>INPUTROW</v>
+      <c r="C152" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="E152" t="str">
+        <f>_xlfn.IFNA(MATCH(D152,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="19" t="s">
-        <v>574</v>
-      </c>
       <c r="B153">
         <v>1610</v>
       </c>
-      <c r="C153" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A153,"***")</f>
-        <v>REM LABEL ***INPUTCOL***</v>
+      <c r="C153" s="5" t="s">
+        <v>671</v>
       </c>
       <c r="E153" t="str">
         <f>_xlfn.IFNA(MATCH(D153,A:A,0),"")</f>
@@ -4696,7 +4662,7 @@
         <v>1620</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="E154" t="str">
         <f>_xlfn.IFNA(MATCH(D154,A:A,0),"")</f>
@@ -4707,26 +4673,24 @@
       <c r="B155">
         <v>1630</v>
       </c>
-      <c r="C155" s="5" t="str">
-        <f>_xlfn.CONCAT("IF COORDS(I)&gt;10 THEN  ",INDEX(B:B,MATCH(D155,A:A,0),0)," :: REM GOTO ",D155,"")</f>
-        <v>IF COORDS(I)&gt;10 THEN  1610 :: REM GOTO INPUTCOL</v>
-      </c>
-      <c r="D155" t="str">
-        <f>A153</f>
-        <v>INPUTCOL</v>
+      <c r="C155" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E155" t="str">
+        <f>_xlfn.IFNA(MATCH(D155,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B156">
         <v>1640</v>
       </c>
-      <c r="C156" s="5" t="str">
-        <f>_xlfn.CONCAT("IF COORDS(I)&lt;1 THEN  ",INDEX(B:B,MATCH(D156,A:A,0),0)," :: REM GOTO ",D156,"")</f>
-        <v>IF COORDS(I)&lt;1 THEN  1610 :: REM GOTO INPUTCOL</v>
-      </c>
-      <c r="D156" t="str">
-        <f>A153</f>
-        <v>INPUTCOL</v>
+      <c r="C156" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="E156" t="str">
+        <f>_xlfn.IFNA(MATCH(D156,A:A,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -4734,7 +4698,7 @@
         <v>1650</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>1</v>
+        <v>597</v>
       </c>
       <c r="E157" t="str">
         <f>_xlfn.IFNA(MATCH(D157,A:A,0),"")</f>
@@ -4746,7 +4710,7 @@
         <v>1660</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>569</v>
+        <v>1</v>
       </c>
       <c r="E158" t="str">
         <f>_xlfn.IFNA(MATCH(D158,A:A,0),"")</f>
@@ -4767,14 +4731,14 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
-        <v>575</v>
+        <v>687</v>
       </c>
       <c r="B160">
         <v>1680</v>
       </c>
       <c r="C160" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A160,"***")</f>
-        <v>REM SUBROUTINE ***VALIDATESHIP***</v>
+        <v>REM SUBROUTINE ***PLAYERDEPLOYINPUT***</v>
       </c>
       <c r="E160" t="str">
         <f>_xlfn.IFNA(MATCH(D160,A:A,0),"")</f>
@@ -4786,7 +4750,7 @@
         <v>1690</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>576</v>
+        <v>25</v>
       </c>
       <c r="E161" t="str">
         <f>_xlfn.IFNA(MATCH(D161,A:A,0),"")</f>
@@ -4797,25 +4761,24 @@
       <c r="B162">
         <v>1700</v>
       </c>
-      <c r="C162" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D162,A:A,0),0)," :: REM CALL ",D162,"")</f>
-        <v>GOSUB 2120 :: REM CALL CHECKHORIZONTAL</v>
-      </c>
-      <c r="D162" t="str">
-        <f>A204</f>
-        <v>CHECKHORIZONTAL</v>
-      </c>
-      <c r="E162">
+      <c r="C162" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="E162" t="str">
         <f>_xlfn.IFNA(MATCH(D162,A:A,0),"")</f>
-        <v>204</v>
+        <v/>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="19" t="s">
+        <v>557</v>
+      </c>
       <c r="B163">
         <v>1710</v>
       </c>
-      <c r="C163" s="5" t="s">
-        <v>668</v>
+      <c r="C163" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A163,"***")</f>
+        <v>REM LABEL ***INPUTROW***</v>
       </c>
       <c r="E163" t="str">
         <f>_xlfn.IFNA(MATCH(D163,A:A,0),"")</f>
@@ -4827,7 +4790,7 @@
         <v>1720</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>598</v>
+        <v>572</v>
       </c>
       <c r="E164" t="str">
         <f>_xlfn.IFNA(MATCH(D164,A:A,0),"")</f>
@@ -4838,37 +4801,37 @@
       <c r="B165">
         <v>1730</v>
       </c>
-      <c r="C165" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E165" t="str">
-        <f>_xlfn.IFNA(MATCH(D165,A:A,0),"")</f>
-        <v/>
+      <c r="C165" s="5" t="str">
+        <f>_xlfn.CONCAT("IF COORDS$(I)="""" THEN  ",INDEX(B:B,MATCH(D165,A:A,0),0)," :: REM GOTO ",D165,"")</f>
+        <v>IF COORDS$(I)="" THEN  1710 :: REM GOTO INPUTROW</v>
+      </c>
+      <c r="D165" t="str">
+        <f>A163</f>
+        <v>INPUTROW</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" s="19" t="s">
+        <v>574</v>
+      </c>
       <c r="B166">
         <v>1740</v>
       </c>
-      <c r="C166" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D166,A:A,0),0)," :: REM CALL ",D166,"")</f>
-        <v>GOSUB 2190 :: REM CALL CHECKSEQUENCE</v>
-      </c>
-      <c r="D166" t="str">
-        <f>A211</f>
-        <v>CHECKSEQUENCE</v>
-      </c>
-      <c r="E166">
+      <c r="C166" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A166,"***")</f>
+        <v>REM LABEL ***INPUTCOL***</v>
+      </c>
+      <c r="E166" t="str">
         <f>_xlfn.IFNA(MATCH(D166,A:A,0),"")</f>
-        <v>211</v>
+        <v/>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B167">
         <v>1750</v>
       </c>
-      <c r="C167" t="s">
-        <v>588</v>
+      <c r="C167" s="5" t="s">
+        <v>573</v>
       </c>
       <c r="E167" t="str">
         <f>_xlfn.IFNA(MATCH(D167,A:A,0),"")</f>
@@ -4879,41 +4842,34 @@
       <c r="B168">
         <v>1760</v>
       </c>
-      <c r="C168" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D168,A:A,0),0)," :: REM CALL ",D168,"")</f>
-        <v>GOSUB 2010 :: REM CALL CHECKOVERLAP</v>
+      <c r="C168" s="5" t="str">
+        <f>_xlfn.CONCAT("IF COORDS(I)&gt;10 THEN  ",INDEX(B:B,MATCH(D168,A:A,0),0)," :: REM GOTO ",D168,"")</f>
+        <v>IF COORDS(I)&gt;10 THEN  1740 :: REM GOTO INPUTCOL</v>
       </c>
       <c r="D168" t="str">
-        <f>A193</f>
-        <v>CHECKOVERLAP</v>
-      </c>
-      <c r="E168">
-        <f>_xlfn.IFNA(MATCH(D168,A:A,0),"")</f>
-        <v>193</v>
+        <f>A166</f>
+        <v>INPUTCOL</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B169">
         <v>1770</v>
       </c>
-      <c r="C169" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E169" t="str">
-        <f>_xlfn.IFNA(MATCH(D169,A:A,0),"")</f>
-        <v/>
+      <c r="C169" s="5" t="str">
+        <f>_xlfn.CONCAT("IF COORDS(I)&lt;1 THEN  ",INDEX(B:B,MATCH(D169,A:A,0),0)," :: REM GOTO ",D169,"")</f>
+        <v>IF COORDS(I)&lt;1 THEN  1740 :: REM GOTO INPUTCOL</v>
+      </c>
+      <c r="D169" t="str">
+        <f>A166</f>
+        <v>INPUTCOL</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A170" s="17" t="s">
-        <v>615</v>
-      </c>
       <c r="B170">
         <v>1780</v>
       </c>
-      <c r="C170" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A170,"***")</f>
-        <v>REM SUBROUTINE ***RENDERSHIP***</v>
+      <c r="C170" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="E170" t="str">
         <f>_xlfn.IFNA(MATCH(D170,A:A,0),"")</f>
@@ -4924,8 +4880,8 @@
       <c r="B171">
         <v>1790</v>
       </c>
-      <c r="C171" t="s">
-        <v>698</v>
+      <c r="C171" s="5" t="s">
+        <v>569</v>
       </c>
       <c r="E171" t="str">
         <f>_xlfn.IFNA(MATCH(D171,A:A,0),"")</f>
@@ -4937,7 +4893,7 @@
         <v>1800</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>668</v>
+        <v>9</v>
       </c>
       <c r="E172" t="str">
         <f>_xlfn.IFNA(MATCH(D172,A:A,0),"")</f>
@@ -4945,11 +4901,15 @@
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" s="17" t="s">
+        <v>575</v>
+      </c>
       <c r="B173">
         <v>1810</v>
       </c>
-      <c r="C173" s="5" t="s">
-        <v>697</v>
+      <c r="C173" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A173,"***")</f>
+        <v>REM SUBROUTINE ***VALIDATESHIP***</v>
       </c>
       <c r="E173" t="str">
         <f>_xlfn.IFNA(MATCH(D173,A:A,0),"")</f>
@@ -4961,7 +4921,7 @@
         <v>1820</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>1</v>
+        <v>576</v>
       </c>
       <c r="E174" t="str">
         <f>_xlfn.IFNA(MATCH(D174,A:A,0),"")</f>
@@ -4972,24 +4932,25 @@
       <c r="B175">
         <v>1830</v>
       </c>
-      <c r="C175" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E175" t="str">
+      <c r="C175" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D175,A:A,0),0)," :: REM CALL ",D175,"")</f>
+        <v>GOSUB 2250 :: REM CALL CHECKHORIZONTAL</v>
+      </c>
+      <c r="D175" t="str">
+        <f>A217</f>
+        <v>CHECKHORIZONTAL</v>
+      </c>
+      <c r="E175">
         <f>_xlfn.IFNA(MATCH(D175,A:A,0),"")</f>
-        <v/>
+        <v>217</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A176" s="17" t="s">
-        <v>694</v>
-      </c>
       <c r="B176">
         <v>1840</v>
       </c>
-      <c r="C176" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A176,"***")</f>
-        <v>REM SUBROUTINE ***RENDERSHIPSAUX***</v>
+      <c r="C176" s="5" t="s">
+        <v>664</v>
       </c>
       <c r="E176" t="str">
         <f>_xlfn.IFNA(MATCH(D176,A:A,0),"")</f>
@@ -5001,7 +4962,7 @@
         <v>1850</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>695</v>
+        <v>598</v>
       </c>
       <c r="E177" t="str">
         <f>_xlfn.IFNA(MATCH(D177,A:A,0),"")</f>
@@ -5013,7 +4974,7 @@
         <v>1860</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>625</v>
+        <v>1</v>
       </c>
       <c r="E178" t="str">
         <f>_xlfn.IFNA(MATCH(D178,A:A,0),"")</f>
@@ -5024,20 +4985,25 @@
       <c r="B179">
         <v>1870</v>
       </c>
-      <c r="C179" t="s">
-        <v>670</v>
-      </c>
-      <c r="E179" t="str">
+      <c r="C179" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D179,A:A,0),0)," :: REM CALL ",D179,"")</f>
+        <v>GOSUB 2320 :: REM CALL CHECKSEQUENCE</v>
+      </c>
+      <c r="D179" t="str">
+        <f>A224</f>
+        <v>CHECKSEQUENCE</v>
+      </c>
+      <c r="E179">
         <f>_xlfn.IFNA(MATCH(D179,A:A,0),"")</f>
-        <v/>
+        <v>224</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B180">
         <v>1880</v>
       </c>
-      <c r="C180" s="5" t="s">
-        <v>696</v>
+      <c r="C180" t="s">
+        <v>588</v>
       </c>
       <c r="E180" t="str">
         <f>_xlfn.IFNA(MATCH(D180,A:A,0),"")</f>
@@ -5048,12 +5014,17 @@
       <c r="B181">
         <v>1890</v>
       </c>
-      <c r="C181" t="s">
-        <v>17</v>
-      </c>
-      <c r="E181" t="str">
+      <c r="C181" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D181,A:A,0),0)," :: REM CALL ",D181,"")</f>
+        <v>GOSUB 2140 :: REM CALL CHECKOVERLAP</v>
+      </c>
+      <c r="D181" t="str">
+        <f>A206</f>
+        <v>CHECKOVERLAP</v>
+      </c>
+      <c r="E181">
         <f>_xlfn.IFNA(MATCH(D181,A:A,0),"")</f>
-        <v/>
+        <v>206</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -5061,7 +5032,7 @@
         <v>1900</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E182" t="str">
         <f>_xlfn.IFNA(MATCH(D182,A:A,0),"")</f>
@@ -5069,11 +5040,15 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183" s="17" t="s">
+        <v>611</v>
+      </c>
       <c r="B183">
         <v>1910</v>
       </c>
-      <c r="C183" s="5" t="s">
-        <v>9</v>
+      <c r="C183" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A183,"***")</f>
+        <v>REM SUBROUTINE ***RENDERSHIP***</v>
       </c>
       <c r="E183" t="str">
         <f>_xlfn.IFNA(MATCH(D183,A:A,0),"")</f>
@@ -5081,15 +5056,11 @@
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" s="17" t="s">
-        <v>613</v>
-      </c>
       <c r="B184">
         <v>1920</v>
       </c>
-      <c r="C184" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A184,"***")</f>
-        <v>REM SUBROUTINE ***PLAYERDEPLOYED***</v>
+      <c r="C184" t="s">
+        <v>694</v>
       </c>
       <c r="E184" t="str">
         <f>_xlfn.IFNA(MATCH(D184,A:A,0),"")</f>
@@ -5100,17 +5071,12 @@
       <c r="B185">
         <v>1930</v>
       </c>
-      <c r="C185" t="str">
-        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D185,A:A,0),0)," :: REM CALL ",D185,"")</f>
-        <v>GOSUB 1400 :: REM CALL CLEARMENU</v>
-      </c>
-      <c r="D185" t="str">
-        <f>A132</f>
-        <v>CLEARMENU</v>
-      </c>
-      <c r="E185">
+      <c r="C185" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="E185" t="str">
         <f>_xlfn.IFNA(MATCH(D185,A:A,0),"")</f>
-        <v>132</v>
+        <v/>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -5118,7 +5084,7 @@
         <v>1940</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>611</v>
+        <v>693</v>
       </c>
       <c r="E186" t="str">
         <f>_xlfn.IFNA(MATCH(D186,A:A,0),"")</f>
@@ -5130,7 +5096,7 @@
         <v>1950</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>612</v>
+        <v>1</v>
       </c>
       <c r="E187" t="str">
         <f>_xlfn.IFNA(MATCH(D187,A:A,0),"")</f>
@@ -5142,7 +5108,7 @@
         <v>1960</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>681</v>
+        <v>9</v>
       </c>
       <c r="E188" t="str">
         <f>_xlfn.IFNA(MATCH(D188,A:A,0),"")</f>
@@ -5150,11 +5116,15 @@
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189" s="17" t="s">
+        <v>690</v>
+      </c>
       <c r="B189">
         <v>1970</v>
       </c>
-      <c r="C189" s="5" t="s">
-        <v>682</v>
+      <c r="C189" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A189,"***")</f>
+        <v>REM SUBROUTINE ***RENDERSHIPSAUX***</v>
       </c>
       <c r="E189" t="str">
         <f>_xlfn.IFNA(MATCH(D189,A:A,0),"")</f>
@@ -5166,7 +5136,7 @@
         <v>1980</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
       <c r="E190" t="str">
         <f>_xlfn.IFNA(MATCH(D190,A:A,0),"")</f>
@@ -5178,7 +5148,7 @@
         <v>1990</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>684</v>
+        <v>621</v>
       </c>
       <c r="E191" t="str">
         <f>_xlfn.IFNA(MATCH(D191,A:A,0),"")</f>
@@ -5189,8 +5159,8 @@
       <c r="B192">
         <v>2000</v>
       </c>
-      <c r="C192" s="5" t="s">
-        <v>9</v>
+      <c r="C192" t="s">
+        <v>666</v>
       </c>
       <c r="E192" t="str">
         <f>_xlfn.IFNA(MATCH(D192,A:A,0),"")</f>
@@ -5198,15 +5168,11 @@
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="17" t="s">
-        <v>591</v>
-      </c>
       <c r="B193">
         <v>2010</v>
       </c>
-      <c r="C193" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A193,"***")</f>
-        <v>REM SUBROUTINE ***CHECKOVERLAP***</v>
+      <c r="C193" s="5" t="s">
+        <v>692</v>
       </c>
       <c r="E193" t="str">
         <f>_xlfn.IFNA(MATCH(D193,A:A,0),"")</f>
@@ -5218,7 +5184,7 @@
         <v>2020</v>
       </c>
       <c r="C194" t="s">
-        <v>593</v>
+        <v>17</v>
       </c>
       <c r="E194" t="str">
         <f>_xlfn.IFNA(MATCH(D194,A:A,0),"")</f>
@@ -5229,8 +5195,8 @@
       <c r="B195">
         <v>2030</v>
       </c>
-      <c r="C195" t="s">
-        <v>670</v>
+      <c r="C195" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="E195" t="str">
         <f>_xlfn.IFNA(MATCH(D195,A:A,0),"")</f>
@@ -5241,8 +5207,8 @@
       <c r="B196">
         <v>2040</v>
       </c>
-      <c r="C196" t="s">
-        <v>709</v>
+      <c r="C196" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E196" t="str">
         <f>_xlfn.IFNA(MATCH(D196,A:A,0),"")</f>
@@ -5250,11 +5216,15 @@
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="17" t="s">
+        <v>609</v>
+      </c>
       <c r="B197">
         <v>2050</v>
       </c>
-      <c r="C197" t="s">
-        <v>672</v>
+      <c r="C197" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A197,"***")</f>
+        <v>REM SUBROUTINE ***PLAYERDEPLOYED***</v>
       </c>
       <c r="E197" t="str">
         <f>_xlfn.IFNA(MATCH(D197,A:A,0),"")</f>
@@ -5265,20 +5235,25 @@
       <c r="B198">
         <v>2060</v>
       </c>
-      <c r="C198" t="s">
-        <v>594</v>
-      </c>
-      <c r="E198" t="str">
+      <c r="C198" t="str">
+        <f>_xlfn.CONCAT("GOSUB ",INDEX(B:B,MATCH(D198,A:A,0),0)," :: REM CALL ",D198,"")</f>
+        <v>GOSUB 1530 :: REM CALL CLEARMENU</v>
+      </c>
+      <c r="D198" t="str">
+        <f>A145</f>
+        <v>CLEARMENU</v>
+      </c>
+      <c r="E198">
         <f>_xlfn.IFNA(MATCH(D198,A:A,0),"")</f>
-        <v/>
+        <v>145</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B199">
         <v>2070</v>
       </c>
-      <c r="C199" t="s">
-        <v>592</v>
+      <c r="C199" s="5" t="s">
+        <v>607</v>
       </c>
       <c r="E199" t="str">
         <f>_xlfn.IFNA(MATCH(D199,A:A,0),"")</f>
@@ -5289,8 +5264,8 @@
       <c r="B200">
         <v>2080</v>
       </c>
-      <c r="C200" t="s">
-        <v>87</v>
+      <c r="C200" s="5" t="s">
+        <v>608</v>
       </c>
       <c r="E200" t="str">
         <f>_xlfn.IFNA(MATCH(D200,A:A,0),"")</f>
@@ -5301,8 +5276,8 @@
       <c r="B201">
         <v>2090</v>
       </c>
-      <c r="C201" t="s">
-        <v>17</v>
+      <c r="C201" s="5" t="s">
+        <v>677</v>
       </c>
       <c r="E201" t="str">
         <f>_xlfn.IFNA(MATCH(D201,A:A,0),"")</f>
@@ -5313,8 +5288,8 @@
       <c r="B202">
         <v>2100</v>
       </c>
-      <c r="C202" t="s">
-        <v>1</v>
+      <c r="C202" s="5" t="s">
+        <v>678</v>
       </c>
       <c r="E202" t="str">
         <f>_xlfn.IFNA(MATCH(D202,A:A,0),"")</f>
@@ -5326,7 +5301,7 @@
         <v>2110</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>9</v>
+        <v>679</v>
       </c>
       <c r="E203" t="str">
         <f>_xlfn.IFNA(MATCH(D203,A:A,0),"")</f>
@@ -5334,15 +5309,11 @@
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" s="17" t="s">
-        <v>585</v>
-      </c>
       <c r="B204">
         <v>2120</v>
       </c>
-      <c r="C204" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A204,"***")</f>
-        <v>REM SUBROUTINE ***CHECKHORIZONTAL***</v>
+      <c r="C204" s="5" t="s">
+        <v>680</v>
       </c>
       <c r="E204" t="str">
         <f>_xlfn.IFNA(MATCH(D204,A:A,0),"")</f>
@@ -5353,8 +5324,8 @@
       <c r="B205">
         <v>2130</v>
       </c>
-      <c r="C205" t="s">
-        <v>586</v>
+      <c r="C205" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E205" t="str">
         <f>_xlfn.IFNA(MATCH(D205,A:A,0),"")</f>
@@ -5362,11 +5333,15 @@
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="17" t="s">
+        <v>591</v>
+      </c>
       <c r="B206">
         <v>2140</v>
       </c>
-      <c r="C206" t="s">
-        <v>671</v>
+      <c r="C206" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A206,"***")</f>
+        <v>REM SUBROUTINE ***CHECKOVERLAP***</v>
       </c>
       <c r="E206" t="str">
         <f>_xlfn.IFNA(MATCH(D206,A:A,0),"")</f>
@@ -5378,7 +5353,7 @@
         <v>2150</v>
       </c>
       <c r="C207" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="E207" t="str">
         <f>_xlfn.IFNA(MATCH(D207,A:A,0),"")</f>
@@ -5390,7 +5365,7 @@
         <v>2160</v>
       </c>
       <c r="C208" t="s">
-        <v>1</v>
+        <v>666</v>
       </c>
       <c r="E208" t="str">
         <f>_xlfn.IFNA(MATCH(D208,A:A,0),"")</f>
@@ -5401,8 +5376,8 @@
       <c r="B209">
         <v>2170</v>
       </c>
-      <c r="C209" s="5" t="s">
-        <v>587</v>
+      <c r="C209" t="s">
+        <v>705</v>
       </c>
       <c r="E209" t="str">
         <f>_xlfn.IFNA(MATCH(D209,A:A,0),"")</f>
@@ -5413,8 +5388,8 @@
       <c r="B210">
         <v>2180</v>
       </c>
-      <c r="C210" s="5" t="s">
-        <v>9</v>
+      <c r="C210" t="s">
+        <v>668</v>
       </c>
       <c r="E210" t="str">
         <f>_xlfn.IFNA(MATCH(D210,A:A,0),"")</f>
@@ -5422,15 +5397,11 @@
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="17" t="s">
-        <v>577</v>
-      </c>
       <c r="B211">
         <v>2190</v>
       </c>
-      <c r="C211" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A211,"***")</f>
-        <v>REM SUBROUTINE ***CHECKSEQUENCE***</v>
+      <c r="C211" t="s">
+        <v>594</v>
       </c>
       <c r="E211" t="str">
         <f>_xlfn.IFNA(MATCH(D211,A:A,0),"")</f>
@@ -5442,7 +5413,7 @@
         <v>2200</v>
       </c>
       <c r="C212" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="E212" t="str">
         <f>_xlfn.IFNA(MATCH(D212,A:A,0),"")</f>
@@ -5453,8 +5424,8 @@
       <c r="B213">
         <v>2210</v>
       </c>
-      <c r="C213" s="5" t="s">
-        <v>671</v>
+      <c r="C213" t="s">
+        <v>87</v>
       </c>
       <c r="E213" t="str">
         <f>_xlfn.IFNA(MATCH(D213,A:A,0),"")</f>
@@ -5465,8 +5436,8 @@
       <c r="B214">
         <v>2220</v>
       </c>
-      <c r="C214" s="5" t="s">
-        <v>581</v>
+      <c r="C214" t="s">
+        <v>17</v>
       </c>
       <c r="E214" t="str">
         <f>_xlfn.IFNA(MATCH(D214,A:A,0),"")</f>
@@ -5477,7 +5448,7 @@
       <c r="B215">
         <v>2230</v>
       </c>
-      <c r="C215" s="5" t="s">
+      <c r="C215" t="s">
         <v>1</v>
       </c>
       <c r="E215" t="str">
@@ -5490,7 +5461,7 @@
         <v>2240</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>578</v>
+        <v>9</v>
       </c>
       <c r="E216" t="str">
         <f>_xlfn.IFNA(MATCH(D216,A:A,0),"")</f>
@@ -5498,11 +5469,15 @@
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217" s="17" t="s">
+        <v>585</v>
+      </c>
       <c r="B217">
         <v>2250</v>
       </c>
-      <c r="C217" s="5" t="s">
-        <v>671</v>
+      <c r="C217" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A217,"***")</f>
+        <v>REM SUBROUTINE ***CHECKHORIZONTAL***</v>
       </c>
       <c r="E217" t="str">
         <f>_xlfn.IFNA(MATCH(D217,A:A,0),"")</f>
@@ -5513,8 +5488,8 @@
       <c r="B218">
         <v>2260</v>
       </c>
-      <c r="C218" s="5" t="s">
-        <v>584</v>
+      <c r="C218" t="s">
+        <v>586</v>
       </c>
       <c r="E218" t="str">
         <f>_xlfn.IFNA(MATCH(D218,A:A,0),"")</f>
@@ -5525,8 +5500,8 @@
       <c r="B219">
         <v>2270</v>
       </c>
-      <c r="C219" s="5" t="s">
-        <v>1</v>
+      <c r="C219" t="s">
+        <v>667</v>
       </c>
       <c r="E219" t="str">
         <f>_xlfn.IFNA(MATCH(D219,A:A,0),"")</f>
@@ -5537,8 +5512,8 @@
       <c r="B220">
         <v>2280</v>
       </c>
-      <c r="C220" s="5" t="s">
-        <v>582</v>
+      <c r="C220" t="s">
+        <v>590</v>
       </c>
       <c r="E220" t="str">
         <f>_xlfn.IFNA(MATCH(D220,A:A,0),"")</f>
@@ -5549,8 +5524,8 @@
       <c r="B221">
         <v>2290</v>
       </c>
-      <c r="C221" s="5" t="s">
-        <v>671</v>
+      <c r="C221" t="s">
+        <v>1</v>
       </c>
       <c r="E221" t="str">
         <f>_xlfn.IFNA(MATCH(D221,A:A,0),"")</f>
@@ -5562,7 +5537,7 @@
         <v>2300</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="E222" t="str">
         <f>_xlfn.IFNA(MATCH(D222,A:A,0),"")</f>
@@ -5574,7 +5549,7 @@
         <v>2310</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E223" t="str">
         <f>_xlfn.IFNA(MATCH(D223,A:A,0),"")</f>
@@ -5582,11 +5557,15 @@
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224" s="17" t="s">
+        <v>577</v>
+      </c>
       <c r="B224">
         <v>2320</v>
       </c>
-      <c r="C224" s="5" t="s">
-        <v>579</v>
+      <c r="C224" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A224,"***")</f>
+        <v>REM SUBROUTINE ***CHECKSEQUENCE***</v>
       </c>
       <c r="E224" t="str">
         <f>_xlfn.IFNA(MATCH(D224,A:A,0),"")</f>
@@ -5597,8 +5576,8 @@
       <c r="B225">
         <v>2330</v>
       </c>
-      <c r="C225" s="5" t="s">
-        <v>9</v>
+      <c r="C225" t="s">
+        <v>580</v>
       </c>
       <c r="E225" t="str">
         <f>_xlfn.IFNA(MATCH(D225,A:A,0),"")</f>
@@ -5606,15 +5585,11 @@
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A226" s="17" t="s">
-        <v>558</v>
-      </c>
       <c r="B226">
         <v>2340</v>
       </c>
-      <c r="C226" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A226,"***")</f>
-        <v>REM SUBROUTINE ***RENDERTEXT***</v>
+      <c r="C226" s="5" t="s">
+        <v>667</v>
       </c>
       <c r="E226" t="str">
         <f>_xlfn.IFNA(MATCH(D226,A:A,0),"")</f>
@@ -5625,8 +5600,8 @@
       <c r="B227">
         <v>2350</v>
       </c>
-      <c r="C227" t="s">
-        <v>561</v>
+      <c r="C227" s="5" t="s">
+        <v>581</v>
       </c>
       <c r="E227" t="str">
         <f>_xlfn.IFNA(MATCH(D227,A:A,0),"")</f>
@@ -5638,7 +5613,7 @@
         <v>2360</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>559</v>
+        <v>1</v>
       </c>
       <c r="E228" t="str">
         <f>_xlfn.IFNA(MATCH(D228,A:A,0),"")</f>
@@ -5650,7 +5625,7 @@
         <v>2370</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>562</v>
+        <v>578</v>
       </c>
       <c r="E229" t="str">
         <f>_xlfn.IFNA(MATCH(D229,A:A,0),"")</f>
@@ -5662,7 +5637,7 @@
         <v>2380</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>563</v>
+        <v>667</v>
       </c>
       <c r="E230" t="str">
         <f>_xlfn.IFNA(MATCH(D230,A:A,0),"")</f>
@@ -5674,7 +5649,7 @@
         <v>2390</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>565</v>
+        <v>584</v>
       </c>
       <c r="E231" t="str">
         <f>_xlfn.IFNA(MATCH(D231,A:A,0),"")</f>
@@ -5698,7 +5673,7 @@
         <v>2410</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>560</v>
+        <v>582</v>
       </c>
       <c r="E233" t="str">
         <f>_xlfn.IFNA(MATCH(D233,A:A,0),"")</f>
@@ -5706,161 +5681,240 @@
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C234" s="5"/>
+      <c r="B234">
+        <v>2420</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>667</v>
+      </c>
       <c r="E234" t="str">
         <f>_xlfn.IFNA(MATCH(D234,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C235" s="5"/>
+      <c r="B235">
+        <v>2430</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>583</v>
+      </c>
       <c r="E235" t="str">
         <f>_xlfn.IFNA(MATCH(D235,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C236" s="5"/>
+      <c r="B236">
+        <v>2440</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="E236" t="str">
         <f>_xlfn.IFNA(MATCH(D236,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B237">
+        <v>2450</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>579</v>
+      </c>
       <c r="E237" t="str">
         <f>_xlfn.IFNA(MATCH(D237,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C238" s="5"/>
+      <c r="B238">
+        <v>2460</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="E238" t="str">
         <f>_xlfn.IFNA(MATCH(D238,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="B239">
+        <v>2470</v>
+      </c>
+      <c r="C239" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A239,"***")</f>
+        <v>REM SUBROUTINE ***RENDERTEXT***</v>
+      </c>
       <c r="E239" t="str">
         <f>_xlfn.IFNA(MATCH(D239,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C240" s="5"/>
+      <c r="B240">
+        <v>2480</v>
+      </c>
+      <c r="C240" t="s">
+        <v>561</v>
+      </c>
       <c r="E240" t="str">
         <f>_xlfn.IFNA(MATCH(D240,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="241" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B241">
+        <v>2490</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>559</v>
+      </c>
       <c r="E241" t="str">
         <f>_xlfn.IFNA(MATCH(D241,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="242" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C242" s="5"/>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B242">
+        <v>2500</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>562</v>
+      </c>
       <c r="E242" t="str">
         <f>_xlfn.IFNA(MATCH(D242,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="243" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B243">
+        <v>2510</v>
+      </c>
+      <c r="C243" s="5" t="s">
+        <v>563</v>
+      </c>
       <c r="E243" t="str">
         <f>_xlfn.IFNA(MATCH(D243,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="244" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C244" s="5"/>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B244">
+        <v>2520</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>565</v>
+      </c>
       <c r="E244" t="str">
         <f>_xlfn.IFNA(MATCH(D244,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="245" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C245" s="5"/>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B245">
+        <v>2530</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="E245" t="str">
         <f>_xlfn.IFNA(MATCH(D245,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="246" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C246" s="5"/>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B246">
+        <v>2540</v>
+      </c>
+      <c r="C246" s="5" t="s">
+        <v>560</v>
+      </c>
       <c r="E246" t="str">
         <f>_xlfn.IFNA(MATCH(D246,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="247" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C247" s="5"/>
       <c r="E247" t="str">
         <f>_xlfn.IFNA(MATCH(D247,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="248" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C248" s="5"/>
       <c r="E248" t="str">
         <f>_xlfn.IFNA(MATCH(D248,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="249" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C249" s="5"/>
       <c r="E249" t="str">
         <f>_xlfn.IFNA(MATCH(D249,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="250" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E250" t="str">
         <f>_xlfn.IFNA(MATCH(D250,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="251" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C251" s="5"/>
       <c r="E251" t="str">
         <f>_xlfn.IFNA(MATCH(D251,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="252" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E252" t="str">
         <f>_xlfn.IFNA(MATCH(D252,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="253" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C253" s="5"/>
       <c r="E253" t="str">
         <f>_xlfn.IFNA(MATCH(D253,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="254" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C254" s="5"/>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E254" t="str">
         <f>_xlfn.IFNA(MATCH(D254,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="255" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C255" s="5"/>
       <c r="E255" t="str">
         <f>_xlfn.IFNA(MATCH(D255,A:A,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="256" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E256" t="str">
         <f>_xlfn.IFNA(MATCH(D256,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="257" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C257" s="5"/>
       <c r="E257" t="str">
         <f>_xlfn.IFNA(MATCH(D257,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="258" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C258" s="5"/>
       <c r="E258" t="str">
         <f>_xlfn.IFNA(MATCH(D258,A:A,0),"")</f>
         <v/>
@@ -5874,7 +5928,6 @@
       </c>
     </row>
     <row r="260" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C260" s="5"/>
       <c r="E260" t="str">
         <f>_xlfn.IFNA(MATCH(D260,A:A,0),"")</f>
         <v/>
@@ -5911,12 +5964,14 @@
       </c>
     </row>
     <row r="266" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C266" s="5"/>
       <c r="E266" t="str">
         <f>_xlfn.IFNA(MATCH(D266,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="267" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C267" s="5"/>
       <c r="E267" t="str">
         <f>_xlfn.IFNA(MATCH(D267,A:A,0),"")</f>
         <v/>
@@ -5947,12 +6002,14 @@
       </c>
     </row>
     <row r="272" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C272" s="5"/>
       <c r="E272" t="str">
         <f>_xlfn.IFNA(MATCH(D272,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="273" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C273" s="5"/>
       <c r="E273" t="str">
         <f>_xlfn.IFNA(MATCH(D273,A:A,0),"")</f>
         <v/>
@@ -5965,14 +6022,12 @@
       </c>
     </row>
     <row r="275" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C275" s="5"/>
       <c r="E275" t="str">
         <f>_xlfn.IFNA(MATCH(D275,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="276" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C276" s="5"/>
       <c r="E276" t="str">
         <f>_xlfn.IFNA(MATCH(D276,A:A,0),"")</f>
         <v/>
@@ -5997,67 +6052,138 @@
       </c>
     </row>
     <row r="280" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C280" s="5"/>
       <c r="E280" t="str">
         <f>_xlfn.IFNA(MATCH(D280,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="281" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C281" s="5"/>
       <c r="E281" t="str">
         <f>_xlfn.IFNA(MATCH(D281,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="282" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C282" s="5"/>
       <c r="E282" t="str">
         <f>_xlfn.IFNA(MATCH(D282,A:A,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="283" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C283" s="5"/>
+      <c r="E283" t="str">
+        <f>_xlfn.IFNA(MATCH(D283,A:A,0),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="284" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C284" s="5"/>
+      <c r="E284" t="str">
+        <f>_xlfn.IFNA(MATCH(D284,A:A,0),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="285" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C285" s="5"/>
+      <c r="E285" t="str">
+        <f>_xlfn.IFNA(MATCH(D285,A:A,0),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="286" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C286" s="5"/>
+      <c r="E286" t="str">
+        <f>_xlfn.IFNA(MATCH(D286,A:A,0),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="287" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C287" s="5"/>
+      <c r="E287" t="str">
+        <f>_xlfn.IFNA(MATCH(D287,A:A,0),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="288" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C288" s="5"/>
-    </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="E288" t="str">
+        <f>_xlfn.IFNA(MATCH(D288,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="289" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C289" s="5"/>
-    </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C290" s="5"/>
-    </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C291" s="5"/>
-    </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C292" s="5"/>
-    </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C313" s="5"/>
-    </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C314" s="5"/>
-    </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C318" s="5"/>
-    </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C321" s="5"/>
+      <c r="E289" t="str">
+        <f>_xlfn.IFNA(MATCH(D289,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="290" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E290" t="str">
+        <f>_xlfn.IFNA(MATCH(D290,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="291" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E291" t="str">
+        <f>_xlfn.IFNA(MATCH(D291,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="292" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E292" t="str">
+        <f>_xlfn.IFNA(MATCH(D292,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="293" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C293" s="5"/>
+      <c r="E293" t="str">
+        <f>_xlfn.IFNA(MATCH(D293,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="294" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C294" s="5"/>
+      <c r="E294" t="str">
+        <f>_xlfn.IFNA(MATCH(D294,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="295" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C295" s="5"/>
+      <c r="E295" t="str">
+        <f>_xlfn.IFNA(MATCH(D295,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C296" s="5"/>
+    </row>
+    <row r="297" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C297" s="5"/>
+    </row>
+    <row r="298" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C298" s="5"/>
+    </row>
+    <row r="299" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C299" s="5"/>
+    </row>
+    <row r="300" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C300" s="5"/>
+    </row>
+    <row r="301" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C301" s="5"/>
+    </row>
+    <row r="302" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C302" s="5"/>
+    </row>
+    <row r="303" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C303" s="5"/>
+    </row>
+    <row r="304" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C304" s="5"/>
+    </row>
+    <row r="305" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C305" s="5"/>
+    </row>
+    <row r="326" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C326" s="5"/>
     </row>
     <row r="327" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C327" s="5"/>
@@ -6065,59 +6191,41 @@
     <row r="331" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C331" s="5"/>
     </row>
-    <row r="335" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C335" s="5"/>
-    </row>
-    <row r="339" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C339" s="5"/>
-    </row>
-    <row r="349" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C349" s="5"/>
-    </row>
-    <row r="356" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C356" s="5"/>
-    </row>
-    <row r="360" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C360" s="5"/>
-    </row>
-    <row r="365" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C365" s="5"/>
-    </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C371" s="5"/>
-    </row>
-    <row r="377" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C377" s="5"/>
-    </row>
-    <row r="380" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C380" s="5"/>
-    </row>
-    <row r="402" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C402" s="5"/>
-    </row>
-    <row r="403" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C403" s="5"/>
-    </row>
-    <row r="404" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C404" s="5"/>
-    </row>
-    <row r="405" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C405" s="5"/>
-    </row>
-    <row r="406" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C406" s="5"/>
-    </row>
-    <row r="407" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C407" s="5"/>
-    </row>
-    <row r="408" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C408" s="5"/>
-    </row>
-    <row r="409" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C409" s="5"/>
-    </row>
-    <row r="414" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C414" s="5"/>
+    <row r="334" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C334" s="5"/>
+    </row>
+    <row r="340" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C340" s="5"/>
+    </row>
+    <row r="344" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C344" s="5"/>
+    </row>
+    <row r="348" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C348" s="5"/>
+    </row>
+    <row r="352" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C352" s="5"/>
+    </row>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C362" s="5"/>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C369" s="5"/>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C373" s="5"/>
+    </row>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C378" s="5"/>
+    </row>
+    <row r="384" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C384" s="5"/>
+    </row>
+    <row r="390" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C390" s="5"/>
+    </row>
+    <row r="393" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C393" s="5"/>
     </row>
     <row r="415" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C415" s="5"/>
@@ -6134,74 +6242,101 @@
     <row r="419" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C419" s="5"/>
     </row>
+    <row r="420" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C420" s="5"/>
+    </row>
     <row r="421" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C421" s="5"/>
     </row>
     <row r="422" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C422" s="5"/>
     </row>
+    <row r="427" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C427" s="5"/>
+    </row>
+    <row r="428" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C428" s="5"/>
+    </row>
+    <row r="429" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C429" s="5"/>
+    </row>
+    <row r="430" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C430" s="5"/>
+    </row>
+    <row r="431" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C431" s="5"/>
+    </row>
+    <row r="432" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C432" s="5"/>
+    </row>
+    <row r="434" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C434" s="5"/>
+    </row>
     <row r="435" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C435" s="1"/>
-    </row>
-    <row r="436" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C436" s="1"/>
-    </row>
-    <row r="437" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C437" s="1"/>
-    </row>
-    <row r="438" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C438" s="1"/>
-    </row>
-    <row r="439" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C439" s="1"/>
-    </row>
-    <row r="441" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C441" s="1"/>
-    </row>
-    <row r="443" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C443" s="1"/>
-    </row>
-    <row r="444" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C444" s="1"/>
-    </row>
-    <row r="446" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C446" s="1"/>
+      <c r="C435" s="5"/>
     </row>
     <row r="448" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C448" s="1"/>
     </row>
+    <row r="449" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C449" s="1"/>
+    </row>
+    <row r="450" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C450" s="1"/>
+    </row>
+    <row r="451" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C451" s="1"/>
+    </row>
     <row r="452" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C452" s="1"/>
     </row>
+    <row r="454" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C454" s="1"/>
+    </row>
     <row r="456" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C456" s="1"/>
     </row>
-    <row r="458" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C458" s="1"/>
+    <row r="457" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C457" s="1"/>
     </row>
     <row r="459" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C459" s="1"/>
     </row>
-    <row r="464" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C464" s="5"/>
+    <row r="461" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C461" s="1"/>
+    </row>
+    <row r="465" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C465" s="1"/>
+    </row>
+    <row r="469" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C469" s="1"/>
+    </row>
+    <row r="471" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C471" s="1"/>
+    </row>
+    <row r="472" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C472" s="1"/>
     </row>
     <row r="477" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C477" s="5"/>
     </row>
-    <row r="481" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C481" s="5"/>
-    </row>
-    <row r="482" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C482" s="5"/>
-    </row>
-    <row r="483" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C483" s="5"/>
-    </row>
-    <row r="484" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C484" s="5"/>
-    </row>
-    <row r="487" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C487" s="5"/>
+    <row r="490" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C490" s="5"/>
+    </row>
+    <row r="494" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C494" s="5"/>
+    </row>
+    <row r="495" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C495" s="5"/>
+    </row>
+    <row r="496" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C496" s="5"/>
+    </row>
+    <row r="497" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C497" s="5"/>
+    </row>
+    <row r="500" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C500" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6215,8 +6350,8 @@
   </sheetPr>
   <dimension ref="A1:F536"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView topLeftCell="A161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235:XFD235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8884,7 +9019,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B148" s="2">
         <v>1540</v>
@@ -8939,7 +9074,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B151" s="2">
         <v>1570</v>
@@ -9120,7 +9255,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B161" s="2">
         <v>1670</v>
@@ -9277,7 +9412,7 @@
         <v/>
       </c>
       <c r="F169" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -9296,7 +9431,7 @@
         <v/>
       </c>
       <c r="F170" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -9347,7 +9482,7 @@
         <v/>
       </c>
       <c r="F173" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -9400,7 +9535,7 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B177" s="2">
         <v>1830</v>
@@ -9417,12 +9552,12 @@
         <v/>
       </c>
       <c r="F177" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B178" s="2">
         <v>1840</v>
@@ -9439,7 +9574,7 @@
         <v/>
       </c>
       <c r="F178" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -9458,7 +9593,7 @@
         <v/>
       </c>
       <c r="F179" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -9493,7 +9628,7 @@
         <v/>
       </c>
       <c r="F181" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -9544,7 +9679,7 @@
         <v/>
       </c>
       <c r="F184" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -9579,12 +9714,12 @@
         <v/>
       </c>
       <c r="F186" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B187" s="2">
         <v>1930</v>
@@ -9601,7 +9736,7 @@
         <v/>
       </c>
       <c r="F187" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
@@ -9620,7 +9755,7 @@
         <v/>
       </c>
       <c r="F188" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -9639,7 +9774,7 @@
         <v/>
       </c>
       <c r="F189" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
@@ -9658,7 +9793,7 @@
         <v/>
       </c>
       <c r="F190" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
@@ -9677,7 +9812,7 @@
         <v/>
       </c>
       <c r="F191" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -9696,7 +9831,7 @@
         <v/>
       </c>
       <c r="F192" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
@@ -9715,7 +9850,7 @@
         <v/>
       </c>
       <c r="F193" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -9734,7 +9869,7 @@
         <v/>
       </c>
       <c r="F194" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -9753,7 +9888,7 @@
         <v/>
       </c>
       <c r="F195" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
@@ -9772,7 +9907,7 @@
         <v/>
       </c>
       <c r="F196" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
@@ -9791,7 +9926,7 @@
         <v>STOREROW</v>
       </c>
       <c r="F197" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
@@ -9826,7 +9961,7 @@
         <v/>
       </c>
       <c r="F199" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -9877,12 +10012,12 @@
         <v>COMPUTERDEPLOYED2</v>
       </c>
       <c r="F202" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B203" s="2">
         <v>2090</v>
@@ -9901,7 +10036,7 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B204" s="2">
         <v>2100</v>
@@ -9918,7 +10053,7 @@
         <v/>
       </c>
       <c r="F204" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
@@ -9937,7 +10072,7 @@
         <v/>
       </c>
       <c r="F205" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
@@ -9956,7 +10091,7 @@
         <v/>
       </c>
       <c r="F206" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
@@ -9975,12 +10110,12 @@
         <v>CONVERTNUM2LET</v>
       </c>
       <c r="F207" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B208" s="2">
         <v>2140</v>
@@ -9997,7 +10132,7 @@
         <v/>
       </c>
       <c r="F208" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
@@ -10016,7 +10151,7 @@
         <v/>
       </c>
       <c r="F209" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
@@ -10035,7 +10170,7 @@
         <v/>
       </c>
       <c r="F210" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
@@ -10070,7 +10205,7 @@
         <v/>
       </c>
       <c r="F212" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -10105,7 +10240,7 @@
         <v/>
       </c>
       <c r="F214" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -10126,7 +10261,7 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B216" s="2">
         <v>2220</v>
@@ -10159,7 +10294,7 @@
         <v>DODUPCHECK</v>
       </c>
       <c r="F217" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
@@ -10194,7 +10329,7 @@
         <v/>
       </c>
       <c r="F219" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
@@ -10213,7 +10348,7 @@
         <v/>
       </c>
       <c r="F220" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -10232,7 +10367,7 @@
         <v/>
       </c>
       <c r="F221" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -10251,7 +10386,7 @@
         <v/>
       </c>
       <c r="F222" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
@@ -10270,7 +10405,7 @@
         <v/>
       </c>
       <c r="F223" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -10289,7 +10424,7 @@
         <v/>
       </c>
       <c r="F224" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
@@ -10327,7 +10462,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B227" s="2">
         <v>2330</v>
@@ -10346,7 +10481,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B228" s="2">
         <v>2340</v>
@@ -10381,7 +10516,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B230" s="2">
         <v>2360</v>
@@ -10398,12 +10533,12 @@
         <v>PICKALLSHIPLOCS</v>
       </c>
       <c r="F230" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B231" s="2">
         <v>2370</v>
@@ -10422,7 +10557,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B232" s="2">
         <v>2380</v>

</xml_diff>

<commit_message>
preparing program for compaction
</commit_message>
<xml_diff>
--- a/battleship.xlsx
+++ b/battleship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28807A27-B579-754A-A9EE-A921B48357F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C830A30-5DDB-2D44-ABC5-236308CEF771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
@@ -3940,20 +3940,19 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>874</v>
-      </c>
       <c r="B19">
         <v>270</v>
       </c>
       <c r="C19" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A19,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A20,"***")</f>
         <v>REM LABEL ***GAMELOOP***</v>
       </c>
       <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="20" t="s">
+        <v>874</v>
+      </c>
       <c r="B20">
         <v>280</v>
       </c>
@@ -4007,10 +4006,10 @@
       </c>
       <c r="C23" s="5" t="str">
         <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D23,A:A,0),0)," :: REM GOTO ",D23,"")</f>
-        <v>GOTO 270 :: REM GOTO GAMELOOP</v>
+        <v>GOTO 280 :: REM GOTO GAMELOOP</v>
       </c>
       <c r="D23" s="20" t="str">
-        <f>A19</f>
+        <f>A20</f>
         <v>GAMELOOP</v>
       </c>
     </row>
@@ -4847,20 +4846,19 @@
       <c r="D86" s="18"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="20" t="s">
-        <v>865</v>
-      </c>
       <c r="B87">
         <v>950</v>
       </c>
       <c r="C87" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A87,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A88,"***")</f>
         <v>REM LABEL ***DEPLOYMANSHIP***</v>
       </c>
       <c r="D87" s="18"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" s="18"/>
+      <c r="A88" s="20" t="s">
+        <v>865</v>
+      </c>
       <c r="B88">
         <v>960</v>
       </c>
@@ -4937,10 +4935,10 @@
       </c>
       <c r="C93" s="5" t="str">
         <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D93,A:A,0),0)," :: REM GOTO ",D93,"")</f>
-        <v>IF ERRVAL=1 THEN 950 :: REM GOTO DEPLOYMANSHIP</v>
+        <v>IF ERRVAL=1 THEN 960 :: REM GOTO DEPLOYMANSHIP</v>
       </c>
       <c r="D93" s="20" t="str">
-        <f>A87</f>
+        <f>A88</f>
         <v>DEPLOYMANSHIP</v>
       </c>
     </row>
@@ -5127,20 +5125,19 @@
       <c r="D107" s="18"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="20" t="s">
-        <v>866</v>
-      </c>
       <c r="B108">
         <v>1160</v>
       </c>
       <c r="C108" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A108,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A109,"***")</f>
         <v>REM LABEL ***DEPLOYCOMPSHIP***</v>
       </c>
       <c r="D108" s="18"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="18"/>
+      <c r="A109" s="20" t="s">
+        <v>866</v>
+      </c>
       <c r="B109">
         <v>1170</v>
       </c>
@@ -5260,10 +5257,10 @@
       </c>
       <c r="C119" t="str">
         <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D119,A:A,0),0)," :: REM GOTO ",D119,"")</f>
-        <v>IF ERRVAL=1 THEN 1160 :: REM GOTO DEPLOYCOMPSHIP</v>
+        <v>IF ERRVAL=1 THEN 1170 :: REM GOTO DEPLOYCOMPSHIP</v>
       </c>
       <c r="D119" s="20" t="str">
-        <f>A108</f>
+        <f>A109</f>
         <v>DEPLOYCOMPSHIP</v>
       </c>
     </row>
@@ -5586,20 +5583,19 @@
       <c r="D145" s="18"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="20" t="s">
-        <v>896</v>
-      </c>
       <c r="B146">
         <v>1540</v>
       </c>
       <c r="C146" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A146,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A147,"***")</f>
         <v>REM LABEL ***TURNLOOP***</v>
       </c>
       <c r="D146" s="18"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="20"/>
+      <c r="A147" s="20" t="s">
+        <v>896</v>
+      </c>
       <c r="B147">
         <v>1550</v>
       </c>
@@ -5666,10 +5662,10 @@
       </c>
       <c r="C151" s="5" t="str">
         <f>_xlfn.CONCAT("IF WINNER=0 OR WINNER=1 THEN ",INDEX(B:B,MATCH(D151,A:A,0),0)," :: REM GOTO ",D151,"")</f>
-        <v>IF WINNER=0 OR WINNER=1 THEN 1630 :: REM GOTO GAMEOVER</v>
+        <v>IF WINNER=0 OR WINNER=1 THEN 1640 :: REM GOTO GAMEOVER</v>
       </c>
       <c r="D151" s="20" t="str">
-        <f>A155</f>
+        <f>A156</f>
         <v>GAMEOVER</v>
       </c>
     </row>
@@ -5707,28 +5703,27 @@
       </c>
       <c r="C154" s="5" t="str">
         <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D154,A:A,0),0)," :: REM GOTO ",D154,"")</f>
-        <v>GOTO 1540 :: REM GOTO TURNLOOP</v>
+        <v>GOTO 1550 :: REM GOTO TURNLOOP</v>
       </c>
       <c r="D154" s="20" t="str">
-        <f>A146</f>
+        <f>A147</f>
         <v>TURNLOOP</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="20" t="s">
-        <v>675</v>
-      </c>
       <c r="B155">
         <v>1630</v>
       </c>
       <c r="C155" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A155,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A156,"***")</f>
         <v>REM LABEL ***GAMEOVER***</v>
       </c>
       <c r="D155" s="18"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="20"/>
+      <c r="A156" s="20" t="s">
+        <v>675</v>
+      </c>
       <c r="B156">
         <v>1640</v>
       </c>
@@ -5829,19 +5824,19 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="20" t="s">
-        <v>1019</v>
-      </c>
       <c r="B164">
         <v>1720</v>
       </c>
       <c r="C164" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A164,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A165,"***")</f>
         <v>REM LABEL ***INPUTLOOP***</v>
       </c>
       <c r="D164" s="18"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="20" t="s">
+        <v>1019</v>
+      </c>
       <c r="B165">
         <v>1730</v>
       </c>
@@ -5888,10 +5883,10 @@
       </c>
       <c r="C168" s="5" t="str">
         <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D168,A:A,0),0)," :: REM GOTO ",D168,"")</f>
-        <v>IF ERRVAL=1 THEN 1720 :: REM GOTO INPUTLOOP</v>
+        <v>IF ERRVAL=1 THEN 1730 :: REM GOTO INPUTLOOP</v>
       </c>
       <c r="D168" s="20" t="str">
-        <f>A164</f>
+        <f>A165</f>
         <v>INPUTLOOP</v>
       </c>
     </row>
@@ -6298,20 +6293,19 @@
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" s="20" t="s">
-        <v>982</v>
-      </c>
       <c r="B200">
         <v>2080</v>
       </c>
       <c r="C200" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A200,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A201,"***")</f>
         <v>REM LABEL ***AISTART***</v>
       </c>
       <c r="D200" s="18"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="20"/>
+      <c r="A201" s="20" t="s">
+        <v>982</v>
+      </c>
       <c r="B201">
         <v>2090</v>
       </c>
@@ -6327,10 +6321,10 @@
       </c>
       <c r="C202" t="str">
         <f>_xlfn.CONCAT("IF QLEN=0 THEN GOSUB ",INDEX(B:B,MATCH(D202,A:A,0),0)," :: REM GOSUB ",D202,)</f>
-        <v>IF QLEN=0 THEN GOSUB 2210 :: REM GOSUB EMPTYQUEUE</v>
+        <v>IF QLEN=0 THEN GOSUB 2220 :: REM GOSUB EMPTYQUEUE</v>
       </c>
       <c r="D202" s="17" t="str">
-        <f>A213</f>
+        <f>A214</f>
         <v>EMPTYQUEUE</v>
       </c>
       <c r="E202" s="20"/>
@@ -6342,10 +6336,10 @@
       </c>
       <c r="C203" t="str">
         <f>_xlfn.CONCAT("IF QLEN=0 THEN GOTO ",INDEX(B:B,MATCH(D203,A:A,0),0)," :: REM GOTO ",D203)</f>
-        <v>IF QLEN=0 THEN GOTO 2160 :: REM GOTO VALIDATESHOT</v>
+        <v>IF QLEN=0 THEN GOTO 2170 :: REM GOTO VALIDATESHOT</v>
       </c>
       <c r="D203" s="20" t="str">
-        <f>A208</f>
+        <f>A209</f>
         <v>VALIDATESHOT</v>
       </c>
       <c r="E203" s="20"/>
@@ -6357,10 +6351,10 @@
       </c>
       <c r="C204" t="str">
         <f>_xlfn.CONCAT("IF OFFSET=0 THEN GOSUB ",INDEX(B:B,MATCH(D204,A:A,0),0)," :: REM GOSUB ",D204)</f>
-        <v>IF OFFSET=0 THEN GOSUB 2250 :: REM GOSUB OFFSETZERO</v>
+        <v>IF OFFSET=0 THEN GOSUB 2260 :: REM GOSUB OFFSETZERO</v>
       </c>
       <c r="D204" s="20" t="str">
-        <f>A217</f>
+        <f>A218</f>
         <v>OFFSETZERO</v>
       </c>
       <c r="E204" s="17"/>
@@ -6374,7 +6368,7 @@
         <v>1044</v>
       </c>
       <c r="D205" s="17" t="str">
-        <f>A217</f>
+        <f>A218</f>
         <v>OFFSETZERO</v>
       </c>
       <c r="E205" s="17"/>
@@ -6402,21 +6396,20 @@
       <c r="E207" s="5"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" s="20" t="s">
-        <v>993</v>
-      </c>
       <c r="B208">
         <v>2160</v>
       </c>
       <c r="C208" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A208,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A209,"***")</f>
         <v>REM LABEL ***VALIDATESHOT***</v>
       </c>
       <c r="D208" s="18"/>
       <c r="E208" s="5"/>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209"/>
+      <c r="A209" s="20" t="s">
+        <v>993</v>
+      </c>
       <c r="B209">
         <v>2170</v>
       </c>
@@ -6439,10 +6432,10 @@
       </c>
       <c r="C210" t="str">
         <f>_xlfn.CONCAT("IF ERRVAL=1 THEN OFFSET=0 :: GOTO ",INDEX(B:B,MATCH(D210,A:A,0),0)," :: REM GOTO ",D210,"")</f>
-        <v>IF ERRVAL=1 THEN OFFSET=0 :: GOTO 2080 :: REM GOTO AISTART</v>
+        <v>IF ERRVAL=1 THEN OFFSET=0 :: GOTO 2090 :: REM GOTO AISTART</v>
       </c>
       <c r="D210" s="20" t="str">
-        <f>A200</f>
+        <f>A201</f>
         <v>AISTART</v>
       </c>
       <c r="E210" s="5"/>
@@ -6472,20 +6465,19 @@
       <c r="E212" s="5"/>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A213" s="17" t="s">
-        <v>984</v>
-      </c>
       <c r="B213">
         <v>2210</v>
       </c>
       <c r="C213" t="str">
-        <f>_xlfn.CONCAT("REM GOSUB ***",A213,"***")</f>
+        <f>_xlfn.CONCAT("REM GOSUB ***",A214,"***")</f>
         <v>REM GOSUB ***EMPTYQUEUE***</v>
       </c>
       <c r="D213" s="18"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A214"/>
+      <c r="A214" s="17" t="s">
+        <v>984</v>
+      </c>
       <c r="B214">
         <v>2220</v>
       </c>
@@ -6515,19 +6507,19 @@
       <c r="D216" s="18"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A217" s="17" t="s">
-        <v>981</v>
-      </c>
       <c r="B217">
         <v>2250</v>
       </c>
       <c r="C217" t="str">
-        <f>_xlfn.CONCAT("REM GOSUB ***",A217,"***")</f>
+        <f>_xlfn.CONCAT("REM GOSUB ***",A218,"***")</f>
         <v>REM GOSUB ***OFFSETZERO***</v>
       </c>
       <c r="D217" s="18"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218" s="17" t="s">
+        <v>981</v>
+      </c>
       <c r="B218">
         <v>2260</v>
       </c>
@@ -8270,20 +8262,19 @@
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A358" s="20" t="s">
-        <v>1026</v>
-      </c>
       <c r="B358">
         <v>3660</v>
       </c>
       <c r="C358" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A358,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A359,"***")</f>
         <v>REM LABEL ***ASKAUTO***</v>
       </c>
       <c r="D358" s="18"/>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A359" s="18"/>
+      <c r="A359" s="20" t="s">
+        <v>1026</v>
+      </c>
       <c r="B359">
         <v>3670</v>
       </c>
@@ -8299,10 +8290,10 @@
       </c>
       <c r="C360" s="5" t="str">
         <f>_xlfn.CONCAT("IF AUTODEPLOY$="""" THEN  ",INDEX(B:B,MATCH(D360,A:A,0),0)," :: REM GOTO ",D360,"")</f>
-        <v>IF AUTODEPLOY$="" THEN  3660 :: REM GOTO ASKAUTO</v>
+        <v>IF AUTODEPLOY$="" THEN  3670 :: REM GOTO ASKAUTO</v>
       </c>
       <c r="D360" s="20" t="str">
-        <f>A358</f>
+        <f>A359</f>
         <v>ASKAUTO</v>
       </c>
     </row>
@@ -9024,20 +9015,19 @@
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A409" s="20" t="s">
-        <v>1027</v>
-      </c>
       <c r="B409">
         <v>4170</v>
       </c>
       <c r="C409" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A409,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A410,"***")</f>
         <v>REM LABEL ***ASKPLAYAGAIN***</v>
       </c>
       <c r="D409" s="18"/>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A410" s="18"/>
+      <c r="A410" s="20" t="s">
+        <v>1027</v>
+      </c>
       <c r="B410">
         <v>4180</v>
       </c>
@@ -9053,10 +9043,10 @@
       </c>
       <c r="C411" s="5" t="str">
         <f>_xlfn.CONCAT("IF PLAYAGAIN$="""" THEN  ",INDEX(B:B,MATCH(D411,A:A,0),0)," :: REM GOTO ",D411,"")</f>
-        <v>IF PLAYAGAIN$="" THEN  4170 :: REM GOTO ASKPLAYAGAIN</v>
+        <v>IF PLAYAGAIN$="" THEN  4180 :: REM GOTO ASKPLAYAGAIN</v>
       </c>
       <c r="D411" s="20" t="str">
-        <f>A409</f>
+        <f>A410</f>
         <v>ASKPLAYAGAIN</v>
       </c>
     </row>
@@ -9108,20 +9098,19 @@
       <c r="D415" s="18"/>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A416" s="19" t="s">
-        <v>700</v>
-      </c>
       <c r="B416">
         <v>4240</v>
       </c>
       <c r="C416" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A416,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A417,"***")</f>
         <v>REM LABEL ***GETROW***</v>
       </c>
       <c r="D416" s="18"/>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A417" s="18"/>
+      <c r="A417" s="19" t="s">
+        <v>700</v>
+      </c>
       <c r="B417">
         <v>4250</v>
       </c>
@@ -9137,28 +9126,27 @@
       </c>
       <c r="C418" s="5" t="str">
         <f>_xlfn.CONCAT("IF INPUTROW$="""" THEN  ",INDEX(B:B,MATCH(D418,A:A,0),0)," :: REM GOTO ",D418,"")</f>
-        <v>IF INPUTROW$="" THEN  4240 :: REM GOTO GETROW</v>
+        <v>IF INPUTROW$="" THEN  4250 :: REM GOTO GETROW</v>
       </c>
       <c r="D418" s="20" t="str">
-        <f>A416</f>
+        <f>A417</f>
         <v>GETROW</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A419" s="19" t="s">
-        <v>699</v>
-      </c>
       <c r="B419">
         <v>4270</v>
       </c>
       <c r="C419" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A419,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A420,"***")</f>
         <v>REM LABEL ***GETCOL***</v>
       </c>
       <c r="D419" s="18"/>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A420" s="18"/>
+      <c r="A420" s="19" t="s">
+        <v>699</v>
+      </c>
       <c r="B420">
         <v>4280</v>
       </c>
@@ -9174,10 +9162,10 @@
       </c>
       <c r="C421" s="5" t="str">
         <f>_xlfn.CONCAT("IF INPUTCOL&gt;10 THEN  ",INDEX(B:B,MATCH(D421,A:A,0),0)," :: REM GOTO ",D421,"")</f>
-        <v>IF INPUTCOL&gt;10 THEN  4270 :: REM GOTO GETCOL</v>
+        <v>IF INPUTCOL&gt;10 THEN  4280 :: REM GOTO GETCOL</v>
       </c>
       <c r="D421" s="20" t="str">
-        <f>A419</f>
+        <f>A420</f>
         <v>GETCOL</v>
       </c>
     </row>
@@ -9188,10 +9176,10 @@
       </c>
       <c r="C422" s="5" t="str">
         <f>_xlfn.CONCAT("IF INPUTCOL&lt;1 THEN  ",INDEX(B:B,MATCH(D422,A:A,0),0)," :: REM GOTO ",D422,"")</f>
-        <v>IF INPUTCOL&lt;1 THEN  4270 :: REM GOTO GETCOL</v>
+        <v>IF INPUTCOL&lt;1 THEN  4280 :: REM GOTO GETCOL</v>
       </c>
       <c r="D422" s="20" t="str">
-        <f>A419</f>
+        <f>A420</f>
         <v>GETCOL</v>
       </c>
     </row>
@@ -10560,10 +10548,10 @@
       </c>
       <c r="C535" t="str">
         <f>_xlfn.CONCAT("IF VALUE=Q(I) THEN DINDEX=I :: GOTO ",INDEX(B:B,MATCH(D535,A:A,0),0)," :: REM GOTO ",D535)</f>
-        <v>IF VALUE=Q(I) THEN DINDEX=I :: GOTO 5460 :: REM GOTO CONTRACT</v>
+        <v>IF VALUE=Q(I) THEN DINDEX=I :: GOTO 5470 :: REM GOTO CONTRACT</v>
       </c>
       <c r="D535" s="20" t="str">
-        <f>A538</f>
+        <f>A539</f>
         <v>CONTRACT</v>
       </c>
     </row>
@@ -10592,20 +10580,19 @@
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A538" s="20" t="s">
-        <v>1043</v>
-      </c>
       <c r="B538">
         <v>5460</v>
       </c>
       <c r="C538" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A538,"***")</f>
+        <f>_xlfn.CONCAT("REM LABEL ***",A539,"***")</f>
         <v>REM LABEL ***CONTRACT***</v>
       </c>
       <c r="D538" s="20"/>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A539"/>
+      <c r="A539" s="20" t="s">
+        <v>1043</v>
+      </c>
       <c r="B539">
         <v>5470</v>
       </c>

</xml_diff>

<commit_message>
fixed bug where ship could be diagonal
</commit_message>
<xml_diff>
--- a/battleship.xlsx
+++ b/battleship.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanwo/projects/ti994a/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C830A30-5DDB-2D44-ABC5-236308CEF771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCDB9A0-C575-2A41-A996-6B40A18CAEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="49500" windowHeight="28300" xr2:uid="{F2DCDACA-2E8A-E041-BEAE-FEED980AFD9D}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="1053">
   <si>
     <t>CALL CLEAR</t>
   </si>
@@ -3188,6 +3188,18 @@
   </si>
   <si>
     <t>REVERSED=0</t>
+  </si>
+  <si>
+    <t>ERRVAL,(CURRENTSHIP),SHIP()</t>
+  </si>
+  <si>
+    <t>CHECKSTRAIGHT</t>
+  </si>
+  <si>
+    <t>PROW=INT(SHIP(I-1)/16) ::PCOL=SHIP(I-1)-INT(SHIP(I-1)/16)*16</t>
+  </si>
+  <si>
+    <t>ERRVAL,CURRENTSHIP,SHIP()</t>
   </si>
 </sst>
 </file>
@@ -3725,7 +3737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB3D0CF-00CA-1047-A168-192C0697CE9E}">
-  <dimension ref="A1:H812"/>
+  <dimension ref="A1:H824"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -4057,7 +4069,7 @@
         <v>CALL GETHOLECHAR(HOLECHAR)</v>
       </c>
       <c r="D27" s="18" t="str">
-        <f>A544</f>
+        <f>A556</f>
         <v>GETHOLECHAR</v>
       </c>
       <c r="E27" t="s">
@@ -4084,7 +4096,7 @@
         <v>CALL GETFILLCHAR(FILLCHAR)</v>
       </c>
       <c r="D29" s="18" t="str">
-        <f>A548</f>
+        <f>A560</f>
         <v>GETFILLCHAR</v>
       </c>
       <c r="E29" t="s">
@@ -4111,7 +4123,7 @@
         <v>CALL GETHITCHAR(HITCHAR)</v>
       </c>
       <c r="D31" s="18" t="str">
-        <f>A552</f>
+        <f>A564</f>
         <v>GETHITCHAR</v>
       </c>
       <c r="E31" t="s">
@@ -4138,7 +4150,7 @@
         <v>CALL GETSHIPCHAR(SHIPCHAR)</v>
       </c>
       <c r="D33" s="18" t="str">
-        <f>A556</f>
+        <f>A568</f>
         <v>GETSHIPCHAR</v>
       </c>
       <c r="E33" t="s">
@@ -4165,7 +4177,7 @@
         <v>CALL GETTENCHAR(TENCHAR)</v>
       </c>
       <c r="D35" s="18" t="str">
-        <f>A560</f>
+        <f>A572</f>
         <v>GETTENCHAR</v>
       </c>
       <c r="E35" t="s">
@@ -4192,7 +4204,7 @@
         <v>CALL GETMISSCHAR(MISSCHAR)</v>
       </c>
       <c r="D37" s="18" t="str">
-        <f>A564</f>
+        <f>A576</f>
         <v>GETMISSCHAR</v>
       </c>
       <c r="E37" t="s">
@@ -4219,7 +4231,7 @@
         <v>CALL GETSUNKCHAR(SUNKCHAR)</v>
       </c>
       <c r="D39" s="18" t="str">
-        <f>A568</f>
+        <f>A580</f>
         <v>GETSUNKCHAR</v>
       </c>
       <c r="E39" t="s">
@@ -4448,7 +4460,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D58" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E58" t="s">
@@ -4598,7 +4610,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D68" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E68" t="s">
@@ -4683,7 +4695,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D73" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E73" t="s">
@@ -4710,7 +4722,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
       </c>
       <c r="D75" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E75" t="s">
@@ -4828,7 +4840,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D85" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E85" t="s">
@@ -4952,7 +4964,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D94" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E94" t="s">
@@ -5073,7 +5085,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D104" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E104" t="s">
@@ -5090,7 +5102,7 @@
         <v>CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D105" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="E105" t="s">
@@ -5107,7 +5119,7 @@
         <v>CALL GETSHIPCHAR(SHIPCHAR)</v>
       </c>
       <c r="D106" s="18" t="str">
-        <f>A556</f>
+        <f>A568</f>
         <v>GETSHIPCHAR</v>
       </c>
       <c r="E106" t="s">
@@ -5146,7 +5158,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D109" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E109" t="s">
@@ -5243,7 +5255,7 @@
         <v>CALL CHECKOVERLAP(ERRVAL,(PLAYER),(CURRENTSHIP),SHIP(),SHIPS(,,))</v>
       </c>
       <c r="D118" s="18" t="str">
-        <f>A501</f>
+        <f>A513</f>
         <v>CHECKOVERLAP</v>
       </c>
       <c r="E118" t="s">
@@ -5304,7 +5316,7 @@
         <v>CALL GETDEBUGFLAG(DEBUG)</v>
       </c>
       <c r="D123" s="18" t="str">
-        <f>A598</f>
+        <f>A610</f>
         <v>GETDEBUGFLAG</v>
       </c>
       <c r="E123" t="s">
@@ -5454,7 +5466,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D135" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E135" t="s">
@@ -5481,7 +5493,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
       </c>
       <c r="D137" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E137" t="s">
@@ -5538,7 +5550,7 @@
         <v>CALL QUEUEINIT(Q(),QLEN)</v>
       </c>
       <c r="D142" s="18" t="str">
-        <f>A520</f>
+        <f>A532</f>
         <v>QUEUEINIT</v>
       </c>
       <c r="E142" t="s">
@@ -5565,7 +5577,7 @@
         <v>CALL GETAUTOPLAY(AUTOPLAY)</v>
       </c>
       <c r="D144" s="18" t="str">
-        <f>A602</f>
+        <f>A614</f>
         <v>GETAUTOPLAY</v>
       </c>
       <c r="E144" t="s">
@@ -5679,7 +5691,7 @@
         <v>CALL GETAUTOPLAY(AUTOPLAY)</v>
       </c>
       <c r="D152" s="20" t="str">
-        <f>A602</f>
+        <f>A614</f>
         <v>GETAUTOPLAY</v>
       </c>
       <c r="E152" t="s">
@@ -5870,7 +5882,7 @@
         <v>CALL CHECKVALIDSHOT(ERRVAL,(ROW),(COL),0,SHOTS(,,))</v>
       </c>
       <c r="D167" s="18" t="str">
-        <f>A456</f>
+        <f>A458</f>
         <v>CHECKVALIDSHOT</v>
       </c>
       <c r="E167" t="s">
@@ -5954,7 +5966,7 @@
         <v>CALL GETMENUORIG(MROW,MCOL)</v>
       </c>
       <c r="D173" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E173" t="s">
@@ -6065,7 +6077,7 @@
         <v>CALL CHECKHIT(HIT,SHIP,(LOC),(1-PLAYER),SHIPS(,,))</v>
       </c>
       <c r="D182" s="18" t="str">
-        <f>A462</f>
+        <f>A464</f>
         <v>CHECKHIT</v>
       </c>
       <c r="E182" t="s">
@@ -6082,7 +6094,7 @@
         <v>IF PLAYER=1 AND HIT=1 THEN CALL QUEUEADD(Q(),QLEN,(LOC),ERRVAL)</v>
       </c>
       <c r="D183" s="18" t="str">
-        <f>A526</f>
+        <f>A538</f>
         <v>QUEUEADD</v>
       </c>
       <c r="E183" t="s">
@@ -6235,7 +6247,7 @@
         <v>CALL QUEUEDEL(Q(),QLEN,(SUNKLOC),ERRVAL)</v>
       </c>
       <c r="D195" s="18" t="str">
-        <f>A531</f>
+        <f>A543</f>
         <v>QUEUEDEL</v>
       </c>
       <c r="E195" t="s">
@@ -6418,7 +6430,7 @@
         <v>CALL CHECKVALIDSHOT(ERRVAL,(ROW),(COL),1,SHOTS(,,))</v>
       </c>
       <c r="D209" s="18" t="str">
-        <f>A456</f>
+        <f>A458</f>
         <v>CHECKVALIDSHOT</v>
       </c>
       <c r="E209" t="s">
@@ -6880,7 +6892,7 @@
         <v>CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D249" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="E249" t="s">
@@ -6897,7 +6909,7 @@
         <v>CALL GETFILLCHAR(FILLCHAR)</v>
       </c>
       <c r="D250" s="18" t="str">
-        <f>A548</f>
+        <f>A560</f>
         <v>GETFILLCHAR</v>
       </c>
       <c r="E250" t="s">
@@ -6978,7 +6990,7 @@
         <v>CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D257" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="E257" t="s">
@@ -6995,7 +7007,7 @@
         <v>CALL GETHOLECHAR(HOLECHAR)</v>
       </c>
       <c r="D258" s="18" t="str">
-        <f>A544</f>
+        <f>A556</f>
         <v>GETHOLECHAR</v>
       </c>
       <c r="E258" t="s">
@@ -7096,7 +7108,7 @@
         <v>CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D267" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="E267" t="s">
@@ -7113,7 +7125,7 @@
         <v>CALL GETTENCHAR(TENCHAR)</v>
       </c>
       <c r="D268" s="18" t="str">
-        <f>A560</f>
+        <f>A572</f>
         <v>GETTENCHAR</v>
       </c>
       <c r="E268" t="s">
@@ -7254,7 +7266,7 @@
         <v>CALL GETAUXORIG(ROW,COL)</v>
       </c>
       <c r="D281" s="18" t="str">
-        <f>A590</f>
+        <f>A602</f>
         <v>GETAUXORIG</v>
       </c>
       <c r="E281" t="s">
@@ -7271,7 +7283,7 @@
         <v>CALL GETHOLECHAR(HOLECHAR)</v>
       </c>
       <c r="D282" s="18" t="str">
-        <f>A544</f>
+        <f>A556</f>
         <v>GETHOLECHAR</v>
       </c>
       <c r="E282" t="s">
@@ -7355,7 +7367,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D289" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E289" t="s">
@@ -7372,7 +7384,7 @@
         <v>CALL GETSHIPCHAR(SHIPCHAR)</v>
       </c>
       <c r="D290" s="18" t="str">
-        <f>A556</f>
+        <f>A568</f>
         <v>GETSHIPCHAR</v>
       </c>
       <c r="E290" t="s">
@@ -7389,7 +7401,7 @@
         <v>CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D291" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="E291" t="s">
@@ -7483,7 +7495,7 @@
         <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D299" s="18" t="str">
-        <f>A572</f>
+        <f>A584</f>
         <v>GETNUMSHIPS</v>
       </c>
       <c r="E299" t="s">
@@ -7500,7 +7512,7 @@
         <v>CALL GETAUXORIG(ROW,COL)</v>
       </c>
       <c r="D300" s="18" t="str">
-        <f>A590</f>
+        <f>A602</f>
         <v>GETAUXORIG</v>
       </c>
       <c r="E300" t="s">
@@ -7517,7 +7529,7 @@
         <v>CALL GETSHIPCHAR(SHIPCHAR)</v>
       </c>
       <c r="D301" s="18" t="str">
-        <f>A556</f>
+        <f>A568</f>
         <v>GETSHIPCHAR</v>
       </c>
       <c r="E301" t="s">
@@ -7544,7 +7556,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
       </c>
       <c r="D303" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E303" t="s">
@@ -7648,7 +7660,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D312" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E312" t="s">
@@ -7712,7 +7724,7 @@
         <v>IF HIT=1 THEN CALL GETHITCHAR(CHARVAL) ELSE CALL GETMISSCHAR(CHARVAL)</v>
       </c>
       <c r="D317" s="18" t="str">
-        <f>A552</f>
+        <f>A564</f>
         <v>GETHITCHAR</v>
       </c>
       <c r="E317" s="18" t="s">
@@ -7732,11 +7744,11 @@
         <v>IF PLAYER=1 THEN CALL GETAUXORIG(ROW,COL) ELSE CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D318" s="18" t="str">
-        <f>A590</f>
+        <f>A602</f>
         <v>GETAUXORIG</v>
       </c>
       <c r="E318" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="F318" t="s">
@@ -7834,7 +7846,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(SHIP))</v>
       </c>
       <c r="D326" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E326" t="s">
@@ -7851,11 +7863,11 @@
         <v>IF PLAYER=0 THEN CALL GETAUXORIG(ROW,COL) ELSE CALL GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D327" s="18" t="str">
-        <f>A590</f>
+        <f>A602</f>
         <v>GETAUXORIG</v>
       </c>
       <c r="E327" s="18" t="str">
-        <f>A586</f>
+        <f>A598</f>
         <v>GETBOARDORIG</v>
       </c>
       <c r="F327" t="s">
@@ -7872,7 +7884,7 @@
         <v>CALL GETSUNKCHAR(SUNKCHAR)</v>
       </c>
       <c r="D328" s="18" t="str">
-        <f>A568</f>
+        <f>A580</f>
         <v>GETSUNKCHAR</v>
       </c>
       <c r="E328" s="5" t="s">
@@ -7949,7 +7961,7 @@
         <v>CALL GETSHIPNAME(SHIPNAME$,(SHIP))</v>
       </c>
       <c r="D335" s="18" t="str">
-        <f>A581</f>
+        <f>A593</f>
         <v>GETSHIPNAME</v>
       </c>
       <c r="E335" t="s">
@@ -7966,7 +7978,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D336" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E336" t="s">
@@ -8091,7 +8103,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D346" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E346" t="s">
@@ -8155,7 +8167,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D351" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E351" t="s">
@@ -8344,7 +8356,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D364" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E364" t="s">
@@ -8429,7 +8441,7 @@
         <v>CALL GETSHIPNAME(SHIPNAME$,(CURRENTSHIP))</v>
       </c>
       <c r="D369" s="18" t="str">
-        <f>A581</f>
+        <f>A593</f>
         <v>GETSHIPNAME</v>
       </c>
       <c r="E369" t="s">
@@ -8480,7 +8492,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D372" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E372" t="s">
@@ -8578,7 +8590,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D380" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E380" t="s">
@@ -8714,7 +8726,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D389" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E389" t="s">
@@ -8881,7 +8893,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D400" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E400" t="s">
@@ -9240,7 +9252,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D427" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E427" t="s">
@@ -9257,7 +9269,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D428" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E428" t="s">
@@ -9368,7 +9380,7 @@
         <v>CALL GETMENUORIG(ROW,COL)</v>
       </c>
       <c r="D437" s="18" t="str">
-        <f>A594</f>
+        <f>A606</f>
         <v>GETMENUORIG</v>
       </c>
       <c r="E437" t="s">
@@ -9469,7 +9481,7 @@
         <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
       </c>
       <c r="D445" s="18" t="str">
-        <f>A576</f>
+        <f>A588</f>
         <v>GETSHIPLEN</v>
       </c>
       <c r="E445" t="s">
@@ -9483,14 +9495,14 @@
       </c>
       <c r="C446" s="18" t="str">
         <f>IF(ISBLANK(E446),_xlfn.CONCAT("CALL ",D446),_xlfn.CONCAT("CALL ",D446,"(",E446,")"))</f>
-        <v>CALL CHECKHORIZONTAL(HORIZONTAL,(CURRENTSHIP),SHIP())</v>
+        <v>CALL CHECKSTRAIGHT(ERRVAL,(CURRENTSHIP),SHIP())</v>
       </c>
       <c r="D446" s="18" t="str">
-        <f>A473</f>
-        <v>CHECKHORIZONTAL</v>
+        <f>A485</f>
+        <v>CHECKSTRAIGHT</v>
       </c>
       <c r="E446" t="s">
-        <v>817</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.2">
@@ -9498,28 +9510,39 @@
       <c r="B447">
         <v>4550</v>
       </c>
-      <c r="C447" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="D447" s="18"/>
+      <c r="C447" t="str">
+        <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D447,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF ERRVAL=1 THEN 4650 :: REM SUBEND</v>
+      </c>
+      <c r="D447" s="20" t="str">
+        <f>A457</f>
+        <v>CHECKVALIDSHIP.SUBEND</v>
+      </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A448" s="18"/>
       <c r="B448">
         <v>4560</v>
       </c>
-      <c r="C448" s="5" t="s">
-        <v>726</v>
-      </c>
-      <c r="D448" s="18"/>
+      <c r="C448" s="18" t="str">
+        <f>IF(ISBLANK(E448),_xlfn.CONCAT("CALL ",D448),_xlfn.CONCAT("CALL ",D448,"(",E448,")"))</f>
+        <v>CALL CHECKHORIZONTAL(HORIZONTAL,(CURRENTSHIP),SHIP())</v>
+      </c>
+      <c r="D448" s="18" t="str">
+        <f>A475</f>
+        <v>CHECKHORIZONTAL</v>
+      </c>
+      <c r="E448" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A449" s="18"/>
       <c r="B449">
         <v>4570</v>
       </c>
-      <c r="C449" s="5" t="s">
-        <v>1040</v>
+      <c r="C449" s="1" t="s">
+        <v>876</v>
       </c>
       <c r="D449" s="18"/>
     </row>
@@ -9529,7 +9552,7 @@
         <v>4580</v>
       </c>
       <c r="C450" s="5" t="s">
-        <v>693</v>
+        <v>726</v>
       </c>
       <c r="D450" s="18"/>
     </row>
@@ -9539,7 +9562,7 @@
         <v>4590</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>1</v>
+        <v>1040</v>
       </c>
       <c r="D451" s="18"/>
     </row>
@@ -9548,31 +9571,20 @@
       <c r="B452">
         <v>4600</v>
       </c>
-      <c r="C452" s="18" t="str">
-        <f>IF(ISBLANK(E452),_xlfn.CONCAT("CALL ",D452),_xlfn.CONCAT("CALL ",D452,"(",E452,")"))</f>
-        <v>CALL CHECKSEQUENTIAL(ERRVAL,(CURRENTSHIP),SEQUENCE())</v>
-      </c>
-      <c r="D452" s="18" t="str">
-        <f>A483</f>
-        <v>CHECKSEQUENTIAL</v>
-      </c>
-      <c r="E452" t="s">
-        <v>1034</v>
-      </c>
+      <c r="C452" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="D452" s="18"/>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A453" s="18"/>
       <c r="B453">
         <v>4610</v>
       </c>
-      <c r="C453" t="str">
-        <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D453,A:A,0),0)," :: REM SUBEND")</f>
-        <v>IF ERRVAL=1 THEN 4630 :: REM SUBEND</v>
-      </c>
-      <c r="D453" s="20" t="str">
-        <f>A455</f>
-        <v>CHECKVALIDSHIP.SUBEND</v>
-      </c>
+      <c r="C453" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D453" s="18"/>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A454" s="18"/>
@@ -9581,63 +9593,70 @@
       </c>
       <c r="C454" s="18" t="str">
         <f>IF(ISBLANK(E454),_xlfn.CONCAT("CALL ",D454),_xlfn.CONCAT("CALL ",D454,"(",E454,")"))</f>
+        <v>CALL CHECKSEQUENTIAL(ERRVAL,(CURRENTSHIP),SEQUENCE())</v>
+      </c>
+      <c r="D454" s="18" t="str">
+        <f>A495</f>
+        <v>CHECKSEQUENTIAL</v>
+      </c>
+      <c r="E454" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A455" s="18"/>
+      <c r="B455">
+        <v>4630</v>
+      </c>
+      <c r="C455" t="str">
+        <f>_xlfn.CONCAT("IF ERRVAL=1 THEN ",INDEX(B:B,MATCH(D455,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF ERRVAL=1 THEN 4650 :: REM SUBEND</v>
+      </c>
+      <c r="D455" s="20" t="str">
+        <f>A457</f>
+        <v>CHECKVALIDSHIP.SUBEND</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A456" s="18"/>
+      <c r="B456">
+        <v>4640</v>
+      </c>
+      <c r="C456" s="18" t="str">
+        <f>IF(ISBLANK(E456),_xlfn.CONCAT("CALL ",D456),_xlfn.CONCAT("CALL ",D456,"(",E456,")"))</f>
         <v>CALL CHECKOVERLAP(ERRVAL,(PLAYER),(CURRENTSHIP),SHIP(),SHIPS(,,))</v>
       </c>
-      <c r="D454" s="18" t="str">
-        <f>A501</f>
+      <c r="D456" s="18" t="str">
+        <f>A513</f>
         <v>CHECKOVERLAP</v>
       </c>
-      <c r="E454" t="s">
+      <c r="E456" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A455" s="20" t="str">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A457" s="20" t="str">
         <f>_xlfn.CONCAT(A441,".SUBEND")</f>
         <v>CHECKVALIDSHIP.SUBEND</v>
       </c>
-      <c r="B455">
-        <v>4630</v>
-      </c>
-      <c r="C455" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="D455" s="18"/>
-    </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A456" s="18" t="s">
-        <v>856</v>
-      </c>
-      <c r="B456">
-        <v>4640</v>
-      </c>
-      <c r="C456" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A456,"***")</f>
-        <v>REM SUBROUTINE ***CHECKVALIDSHOT***</v>
-      </c>
-      <c r="D456" s="18"/>
-    </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A457" s="18"/>
       <c r="B457">
         <v>4650</v>
       </c>
-      <c r="C457" t="str">
-        <f>IF(ISBLANK(E457),_xlfn.CONCAT("SUB ",A456),_xlfn.CONCAT("SUB ",A456,"(",E457,")"))</f>
-        <v>SUB CHECKVALIDSHOT(ERRVAL,ROW,COL,PLAYER,SHOTS(,,))</v>
+      <c r="C457" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D457" s="18"/>
-      <c r="E457" t="s">
-        <v>1030</v>
-      </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A458" s="18"/>
+      <c r="A458" s="18" t="s">
+        <v>856</v>
+      </c>
       <c r="B458">
         <v>4660</v>
       </c>
-      <c r="C458" t="s">
-        <v>1031</v>
+      <c r="C458" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A458,"***")</f>
+        <v>REM SUBROUTINE ***CHECKVALIDSHOT***</v>
       </c>
       <c r="D458" s="18"/>
     </row>
@@ -9647,12 +9666,12 @@
         <v>4670</v>
       </c>
       <c r="C459" t="str">
-        <f>_xlfn.CONCAT("IF ROW&lt;1 OR ROW&gt;10 OR COL&lt;1 OR COL&gt;10 THEN ERRVAL=1 :: GOTO  ",INDEX(B:B,MATCH(D459,A:A,0),0)," :: REM GOTO SUBEND")</f>
-        <v>IF ROW&lt;1 OR ROW&gt;10 OR COL&lt;1 OR COL&gt;10 THEN ERRVAL=1 :: GOTO  4690 :: REM GOTO SUBEND</v>
-      </c>
-      <c r="D459" s="20" t="str">
-        <f>A461</f>
-        <v>CHECKVALIDSHOT.SUBEND</v>
+        <f>IF(ISBLANK(E459),_xlfn.CONCAT("SUB ",A458),_xlfn.CONCAT("SUB ",A458,"(",E459,")"))</f>
+        <v>SUB CHECKVALIDSHOT(ERRVAL,ROW,COL,PLAYER,SHOTS(,,))</v>
+      </c>
+      <c r="D459" s="18"/>
+      <c r="E459" t="s">
+        <v>1030</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.2">
@@ -9660,58 +9679,58 @@
       <c r="B460">
         <v>4680</v>
       </c>
-      <c r="C460" s="5" t="s">
-        <v>1032</v>
+      <c r="C460" t="s">
+        <v>1031</v>
       </c>
       <c r="D460" s="18"/>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A461" s="20" t="str">
-        <f>_xlfn.CONCAT(A456,".SUBEND")</f>
-        <v>CHECKVALIDSHOT.SUBEND</v>
-      </c>
+      <c r="A461" s="18"/>
       <c r="B461">
         <v>4690</v>
       </c>
-      <c r="C461" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="D461" s="18"/>
+      <c r="C461" t="str">
+        <f>_xlfn.CONCAT("IF ROW&lt;1 OR ROW&gt;10 OR COL&lt;1 OR COL&gt;10 THEN ERRVAL=1 :: GOTO  ",INDEX(B:B,MATCH(D461,A:A,0),0)," :: REM GOTO SUBEND")</f>
+        <v>IF ROW&lt;1 OR ROW&gt;10 OR COL&lt;1 OR COL&gt;10 THEN ERRVAL=1 :: GOTO  4710 :: REM GOTO SUBEND</v>
+      </c>
+      <c r="D461" s="20" t="str">
+        <f>A463</f>
+        <v>CHECKVALIDSHOT.SUBEND</v>
+      </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A462" s="18" t="s">
-        <v>772</v>
-      </c>
+      <c r="A462" s="18"/>
       <c r="B462">
         <v>4700</v>
       </c>
-      <c r="C462" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A462,"***")</f>
-        <v>REM SUBROUTINE ***CHECKHIT***</v>
+      <c r="C462" s="5" t="s">
+        <v>1032</v>
       </c>
       <c r="D462" s="18"/>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A463" s="18"/>
+      <c r="A463" s="20" t="str">
+        <f>_xlfn.CONCAT(A458,".SUBEND")</f>
+        <v>CHECKVALIDSHOT.SUBEND</v>
+      </c>
       <c r="B463">
         <v>4710</v>
       </c>
-      <c r="C463" t="str">
-        <f>IF(ISBLANK(E463),_xlfn.CONCAT("SUB ",A462),_xlfn.CONCAT("SUB ",A462,"(",E463,")"))</f>
-        <v>SUB CHECKHIT(HIT,SHIP,LOC,PLAYER,SHIPS(,,))</v>
+      <c r="C463" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D463" s="18"/>
-      <c r="E463" t="s">
-        <v>778</v>
-      </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A464" s="18"/>
+      <c r="A464" s="18" t="s">
+        <v>772</v>
+      </c>
       <c r="B464">
         <v>4720</v>
       </c>
-      <c r="C464" t="s">
-        <v>771</v>
+      <c r="C464" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A464,"***")</f>
+        <v>REM SUBROUTINE ***CHECKHIT***</v>
       </c>
       <c r="D464" s="18"/>
     </row>
@@ -9720,16 +9739,13 @@
       <c r="B465">
         <v>4730</v>
       </c>
-      <c r="C465" s="18" t="str">
-        <f t="shared" ref="C465:C467" si="7">IF(ISBLANK(E465),_xlfn.CONCAT("CALL ",D465),_xlfn.CONCAT("CALL ",D465,"(",E465,")"))</f>
-        <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
-      </c>
-      <c r="D465" s="18" t="str">
-        <f>A572</f>
-        <v>GETNUMSHIPS</v>
-      </c>
+      <c r="C465" t="str">
+        <f>IF(ISBLANK(E465),_xlfn.CONCAT("SUB ",A464),_xlfn.CONCAT("SUB ",A464,"(",E465,")"))</f>
+        <v>SUB CHECKHIT(HIT,SHIP,LOC,PLAYER,SHIPS(,,))</v>
+      </c>
+      <c r="D465" s="18"/>
       <c r="E465" t="s">
-        <v>706</v>
+        <v>778</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.2">
@@ -9737,8 +9753,8 @@
       <c r="B466">
         <v>4740</v>
       </c>
-      <c r="C466" s="5" t="s">
-        <v>575</v>
+      <c r="C466" t="s">
+        <v>771</v>
       </c>
       <c r="D466" s="18"/>
     </row>
@@ -9748,15 +9764,15 @@
         <v>4750</v>
       </c>
       <c r="C467" s="18" t="str">
-        <f t="shared" si="7"/>
-        <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
+        <f t="shared" ref="C467:C469" si="7">IF(ISBLANK(E467),_xlfn.CONCAT("CALL ",D467),_xlfn.CONCAT("CALL ",D467,"(",E467,")"))</f>
+        <v>CALL GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D467" s="18" t="str">
-        <f>A576</f>
-        <v>GETSHIPLEN</v>
+        <f>A584</f>
+        <v>GETNUMSHIPS</v>
       </c>
       <c r="E467" t="s">
-        <v>790</v>
+        <v>706</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.2">
@@ -9764,8 +9780,8 @@
       <c r="B468">
         <v>4760</v>
       </c>
-      <c r="C468" t="s">
-        <v>724</v>
+      <c r="C468" s="5" t="s">
+        <v>575</v>
       </c>
       <c r="D468" s="18"/>
     </row>
@@ -9774,13 +9790,16 @@
       <c r="B469">
         <v>4770</v>
       </c>
-      <c r="C469" s="5" t="str">
-        <f>_xlfn.CONCAT("IF SHIPS(PLAYER,I,J)=LOC THEN HIT=1 :: SHIP=I :: GOTO ",INDEX(B:B,MATCH(D469,A:A,0),0)," :: REM SUBEND")</f>
-        <v>IF SHIPS(PLAYER,I,J)=LOC THEN HIT=1 :: SHIP=I :: GOTO 4800 :: REM SUBEND</v>
-      </c>
-      <c r="D469" s="20" t="str">
-        <f>A472</f>
-        <v>CHECKHIT.SUBEND</v>
+      <c r="C469" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
+      </c>
+      <c r="D469" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E469" t="s">
+        <v>790</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.2">
@@ -9788,8 +9807,8 @@
       <c r="B470">
         <v>4780</v>
       </c>
-      <c r="C470" s="5" t="s">
-        <v>14</v>
+      <c r="C470" t="s">
+        <v>724</v>
       </c>
       <c r="D470" s="18"/>
     </row>
@@ -9798,58 +9817,58 @@
       <c r="B471">
         <v>4790</v>
       </c>
-      <c r="C471" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D471" s="18"/>
+      <c r="C471" s="5" t="str">
+        <f>_xlfn.CONCAT("IF SHIPS(PLAYER,I,J)=LOC THEN HIT=1 :: SHIP=I :: GOTO ",INDEX(B:B,MATCH(D471,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF SHIPS(PLAYER,I,J)=LOC THEN HIT=1 :: SHIP=I :: GOTO 4820 :: REM SUBEND</v>
+      </c>
+      <c r="D471" s="20" t="str">
+        <f>A474</f>
+        <v>CHECKHIT.SUBEND</v>
+      </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A472" s="20" t="str">
-        <f>_xlfn.CONCAT(A462,".SUBEND")</f>
-        <v>CHECKHIT.SUBEND</v>
-      </c>
+      <c r="A472" s="18"/>
       <c r="B472">
         <v>4800</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>555</v>
+        <v>14</v>
       </c>
       <c r="D472" s="18"/>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A473" s="18" t="s">
-        <v>563</v>
-      </c>
+      <c r="A473" s="18"/>
       <c r="B473">
         <v>4810</v>
       </c>
-      <c r="C473" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A473,"***")</f>
-        <v>REM SUBROUTINE ***CHECKHORIZONTAL***</v>
+      <c r="C473" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D473" s="18"/>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A474" s="18"/>
+      <c r="A474" s="20" t="str">
+        <f>_xlfn.CONCAT(A464,".SUBEND")</f>
+        <v>CHECKHIT.SUBEND</v>
+      </c>
       <c r="B474">
         <v>4820</v>
       </c>
-      <c r="C474" t="str">
-        <f>IF(ISBLANK(E474),_xlfn.CONCAT("SUB ",A473),_xlfn.CONCAT("SUB ",A473,"(",E474,")"))</f>
-        <v>SUB CHECKHORIZONTAL(HORIZONTAL,CURRENTSHIP,SHIP())</v>
+      <c r="C474" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D474" s="18"/>
-      <c r="E474" t="s">
-        <v>723</v>
-      </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A475" s="18"/>
+      <c r="A475" s="18" t="s">
+        <v>563</v>
+      </c>
       <c r="B475">
         <v>4830</v>
       </c>
-      <c r="C475" t="s">
-        <v>564</v>
+      <c r="C475" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A475,"***")</f>
+        <v>REM SUBROUTINE ***CHECKHORIZONTAL***</v>
       </c>
       <c r="D475" s="18"/>
     </row>
@@ -9858,16 +9877,13 @@
       <c r="B476">
         <v>4840</v>
       </c>
-      <c r="C476" s="18" t="str">
-        <f>IF(ISBLANK(E476),_xlfn.CONCAT("CALL ",D476),_xlfn.CONCAT("CALL ",D476,"(",E476,")"))</f>
-        <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
-      </c>
-      <c r="D476" s="18" t="str">
-        <f>A576</f>
-        <v>GETSHIPLEN</v>
-      </c>
+      <c r="C476" t="str">
+        <f>IF(ISBLANK(E476),_xlfn.CONCAT("SUB ",A475),_xlfn.CONCAT("SUB ",A475,"(",E476,")"))</f>
+        <v>SUB CHECKHORIZONTAL(HORIZONTAL,CURRENTSHIP,SHIP())</v>
+      </c>
+      <c r="D476" s="18"/>
       <c r="E476" t="s">
-        <v>807</v>
+        <v>723</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.2">
@@ -9876,7 +9892,7 @@
         <v>4850</v>
       </c>
       <c r="C477" t="s">
-        <v>722</v>
+        <v>564</v>
       </c>
       <c r="D477" s="18"/>
     </row>
@@ -9885,32 +9901,35 @@
       <c r="B478">
         <v>4860</v>
       </c>
-      <c r="C478" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="D478" s="18"/>
+      <c r="C478" s="18" t="str">
+        <f>IF(ISBLANK(E478),_xlfn.CONCAT("CALL ",D478),_xlfn.CONCAT("CALL ",D478,"(",E478,")"))</f>
+        <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
+      </c>
+      <c r="D478" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E478" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A479" s="18"/>
       <c r="B479">
         <v>4870</v>
       </c>
-      <c r="C479" t="str">
-        <f>_xlfn.CONCAT("IF PREV&lt;&gt;CURR THEN ",INDEX(B:B,MATCH(D479,A:A,0),0)," :: REM SUBEND")</f>
-        <v>IF PREV&lt;&gt;CURR THEN 4900 :: REM SUBEND</v>
-      </c>
-      <c r="D479" s="20" t="str">
-        <f>A482</f>
-        <v>CHECKHORIZONTAL.SUBEND</v>
-      </c>
+      <c r="C479" t="s">
+        <v>722</v>
+      </c>
+      <c r="D479" s="18"/>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A480" s="18"/>
       <c r="B480">
         <v>4880</v>
       </c>
-      <c r="C480" t="s">
-        <v>1</v>
+      <c r="C480" s="5" t="s">
+        <v>685</v>
       </c>
       <c r="D480" s="18"/>
     </row>
@@ -9919,165 +9938,179 @@
       <c r="B481">
         <v>4890</v>
       </c>
-      <c r="C481" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="D481" s="18"/>
+      <c r="C481" t="str">
+        <f>_xlfn.CONCAT("IF PREV&lt;&gt;CURR THEN ",INDEX(B:B,MATCH(D481,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF PREV&lt;&gt;CURR THEN 4920 :: REM SUBEND</v>
+      </c>
+      <c r="D481" s="20" t="str">
+        <f>A484</f>
+        <v>CHECKHORIZONTAL.SUBEND</v>
+      </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A482" s="20" t="str">
-        <f>_xlfn.CONCAT(A473,".SUBEND")</f>
-        <v>CHECKHORIZONTAL.SUBEND</v>
-      </c>
+      <c r="A482" s="18"/>
       <c r="B482">
         <v>4900</v>
       </c>
-      <c r="C482" s="5" t="s">
-        <v>555</v>
+      <c r="C482" t="s">
+        <v>1</v>
       </c>
       <c r="D482" s="18"/>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A483" s="18" t="s">
-        <v>857</v>
-      </c>
+      <c r="A483" s="18"/>
       <c r="B483">
         <v>4910</v>
       </c>
-      <c r="C483" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A483,"***")</f>
-        <v>REM SUBROUTINE ***CHECKSEQUENTIAL***</v>
+      <c r="C483" s="5" t="s">
+        <v>565</v>
       </c>
       <c r="D483" s="18"/>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A484" s="18"/>
+      <c r="A484" s="20" t="str">
+        <f>_xlfn.CONCAT(A475,".SUBEND")</f>
+        <v>CHECKHORIZONTAL.SUBEND</v>
+      </c>
       <c r="B484">
         <v>4920</v>
       </c>
-      <c r="C484" t="str">
-        <f>IF(ISBLANK(E484),_xlfn.CONCAT("SUB ",A483),_xlfn.CONCAT("SUB ",A483,"(",E484,")"))</f>
-        <v>SUB CHECKSEQUENTIAL(ERRVAL,CURRENTSHIP,SEQUENCE())</v>
+      <c r="C484" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D484" s="18"/>
-      <c r="E484" t="s">
-        <v>1036</v>
-      </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A485" s="18"/>
+      <c r="A485" s="18" t="s">
+        <v>1050</v>
+      </c>
       <c r="B485">
         <v>4930</v>
       </c>
-      <c r="C485" t="s">
-        <v>1031</v>
+      <c r="C485" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A485,"***")</f>
+        <v>REM SUBROUTINE ***CHECKSTRAIGHT***</v>
       </c>
       <c r="D485" s="18"/>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A486" s="18"/>
+      <c r="A486" s="20"/>
       <c r="B486">
         <v>4940</v>
       </c>
-      <c r="C486" s="18" t="str">
-        <f>IF(ISBLANK(E486),_xlfn.CONCAT("CALL ",D486),_xlfn.CONCAT("CALL ",D486,"(",E486,")"))</f>
-        <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
-      </c>
-      <c r="D486" s="18" t="str">
-        <f>A576</f>
-        <v>GETSHIPLEN</v>
-      </c>
+      <c r="C486" t="str">
+        <f>IF(ISBLANK(E486),_xlfn.CONCAT("SUB ",A485),_xlfn.CONCAT("SUB ",A485,"(",E486,")"))</f>
+        <v>SUB CHECKSTRAIGHT(ERRVAL,CURRENTSHIP,SHIP())</v>
+      </c>
+      <c r="D486" s="18"/>
       <c r="E486" t="s">
-        <v>807</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A487" s="18"/>
+      <c r="A487" s="20"/>
       <c r="B487">
         <v>4950</v>
       </c>
       <c r="C487" t="s">
-        <v>694</v>
+        <v>1031</v>
       </c>
       <c r="D487" s="18"/>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A488" s="18"/>
+      <c r="A488" s="20"/>
       <c r="B488">
         <v>4960</v>
       </c>
-      <c r="C488" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="D488" s="18"/>
+      <c r="C488" s="18" t="str">
+        <f>IF(ISBLANK(E488),_xlfn.CONCAT("CALL ",D488),_xlfn.CONCAT("CALL ",D488,"(",E488,")"))</f>
+        <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
+      </c>
+      <c r="D488" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E488" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A489" s="18"/>
+      <c r="A489" s="20"/>
       <c r="B489">
         <v>4970</v>
       </c>
-      <c r="C489" s="5" t="s">
-        <v>697</v>
+      <c r="C489" t="s">
+        <v>722</v>
       </c>
       <c r="D489" s="18"/>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A490" s="18"/>
+      <c r="A490" s="20"/>
       <c r="B490">
         <v>4980</v>
       </c>
       <c r="C490" s="5" t="s">
-        <v>1</v>
+        <v>1040</v>
       </c>
       <c r="D490" s="18"/>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A491" s="18"/>
+      <c r="A491" s="20"/>
       <c r="B491">
         <v>4990</v>
       </c>
       <c r="C491" s="5" t="s">
-        <v>561</v>
+        <v>1051</v>
       </c>
       <c r="D491" s="18"/>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A492" s="18"/>
+      <c r="A492" s="20"/>
       <c r="B492">
         <v>5000</v>
       </c>
-      <c r="C492" s="5" t="s">
-        <v>722</v>
-      </c>
-      <c r="D492" s="18"/>
+      <c r="C492" t="str">
+        <f>_xlfn.CONCAT("IF (ROW&lt;&gt;PROW) AND (COL&lt;&gt;PCOL) THEN ERRVAL=1 :: GOTO ",INDEX(B:B,MATCH(D492,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF (ROW&lt;&gt;PROW) AND (COL&lt;&gt;PCOL) THEN ERRVAL=1 :: GOTO 5020 :: REM SUBEND</v>
+      </c>
+      <c r="D492" s="20" t="str">
+        <f>A494</f>
+        <v>CHECKSTRAIGHT.SUBEND</v>
+      </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A493" s="18"/>
+      <c r="A493" s="20"/>
       <c r="B493">
         <v>5010</v>
       </c>
-      <c r="C493" s="5" t="s">
-        <v>562</v>
+      <c r="C493" t="s">
+        <v>1</v>
       </c>
       <c r="D493" s="18"/>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A494" s="18"/>
+      <c r="A494" s="20" t="str">
+        <f>_xlfn.CONCAT(A485,".SUBEND")</f>
+        <v>CHECKSTRAIGHT.SUBEND</v>
+      </c>
       <c r="B494">
         <v>5020</v>
       </c>
       <c r="C494" s="5" t="s">
-        <v>1</v>
+        <v>555</v>
       </c>
       <c r="D494" s="18"/>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A495" s="18"/>
+      <c r="A495" s="18" t="s">
+        <v>857</v>
+      </c>
       <c r="B495">
         <v>5030</v>
       </c>
-      <c r="C495" s="5" t="s">
-        <v>695</v>
+      <c r="C495" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A495,"***")</f>
+        <v>REM SUBROUTINE ***CHECKSEQUENTIAL***</v>
       </c>
       <c r="D495" s="18"/>
     </row>
@@ -10086,18 +10119,22 @@
       <c r="B496">
         <v>5040</v>
       </c>
-      <c r="C496" s="5" t="s">
-        <v>722</v>
+      <c r="C496" t="str">
+        <f>IF(ISBLANK(E496),_xlfn.CONCAT("SUB ",A495),_xlfn.CONCAT("SUB ",A495,"(",E496,")"))</f>
+        <v>SUB CHECKSEQUENTIAL(ERRVAL,CURRENTSHIP,SEQUENCE())</v>
       </c>
       <c r="D496" s="18"/>
+      <c r="E496" t="s">
+        <v>1036</v>
+      </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A497" s="18"/>
       <c r="B497">
         <v>5050</v>
       </c>
-      <c r="C497" s="5" t="s">
-        <v>696</v>
+      <c r="C497" t="s">
+        <v>1031</v>
       </c>
       <c r="D497" s="18"/>
     </row>
@@ -10106,18 +10143,25 @@
       <c r="B498">
         <v>5060</v>
       </c>
-      <c r="C498" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D498" s="18"/>
+      <c r="C498" s="18" t="str">
+        <f>IF(ISBLANK(E498),_xlfn.CONCAT("CALL ",D498),_xlfn.CONCAT("CALL ",D498,"(",E498,")"))</f>
+        <v>CALL GETSHIPLEN(SHIPLEN,(CURRENTSHIP))</v>
+      </c>
+      <c r="D498" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E498" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A499" s="18"/>
       <c r="B499">
         <v>5070</v>
       </c>
-      <c r="C499" s="5" t="s">
-        <v>1037</v>
+      <c r="C499" t="s">
+        <v>694</v>
       </c>
       <c r="D499" s="18"/>
     </row>
@@ -10127,20 +10171,17 @@
         <v>5080</v>
       </c>
       <c r="C500" s="5" t="s">
-        <v>555</v>
+        <v>722</v>
       </c>
       <c r="D500" s="18"/>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A501" s="18" t="s">
-        <v>566</v>
-      </c>
+      <c r="A501" s="18"/>
       <c r="B501">
         <v>5090</v>
       </c>
-      <c r="C501" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A501,"***")</f>
-        <v>REM SUBROUTINE ***CHECKOVERLAP***</v>
+      <c r="C501" s="5" t="s">
+        <v>697</v>
       </c>
       <c r="D501" s="18"/>
     </row>
@@ -10149,14 +10190,10 @@
       <c r="B502">
         <v>5100</v>
       </c>
-      <c r="C502" t="str">
-        <f>IF(ISBLANK(E502),_xlfn.CONCAT("SUB ",A501),_xlfn.CONCAT("SUB ",A501,"(",E502,")"))</f>
-        <v>SUB CHECKOVERLAP(ERRVAL,PLAYER,CURRENTSHIP,SHIP(),SHIPS(,,))</v>
+      <c r="C502" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D502" s="18"/>
-      <c r="E502" t="s">
-        <v>1033</v>
-      </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A503" s="18"/>
@@ -10164,7 +10201,7 @@
         <v>5110</v>
       </c>
       <c r="C503" s="5" t="s">
-        <v>1031</v>
+        <v>561</v>
       </c>
       <c r="D503" s="18"/>
     </row>
@@ -10173,25 +10210,18 @@
       <c r="B504">
         <v>5120</v>
       </c>
-      <c r="C504" s="18" t="str">
-        <f>IF(ISBLANK(E504),_xlfn.CONCAT("CALL ",D504),_xlfn.CONCAT("CALL ",D504,"(",E504,")"))</f>
-        <v>CALL GETSHIPLEN(CURRENTSHIPLEN,(CURRENTSHIP))</v>
-      </c>
-      <c r="D504" s="18" t="str">
-        <f>A576</f>
-        <v>GETSHIPLEN</v>
-      </c>
-      <c r="E504" t="s">
-        <v>824</v>
-      </c>
+      <c r="C504" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="D504" s="18"/>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A505" s="18"/>
       <c r="B505">
         <v>5130</v>
       </c>
-      <c r="C505" t="s">
-        <v>567</v>
+      <c r="C505" s="5" t="s">
+        <v>562</v>
       </c>
       <c r="D505" s="18"/>
     </row>
@@ -10200,25 +10230,18 @@
       <c r="B506">
         <v>5140</v>
       </c>
-      <c r="C506" s="18" t="str">
-        <f>IF(ISBLANK(E506),_xlfn.CONCAT("CALL ",D506),_xlfn.CONCAT("CALL ",D506,"(",E506,")"))</f>
-        <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
-      </c>
-      <c r="D506" s="18" t="str">
-        <f>A576</f>
-        <v>GETSHIPLEN</v>
-      </c>
-      <c r="E506" t="s">
-        <v>790</v>
-      </c>
+      <c r="C506" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D506" s="18"/>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A507" s="18"/>
       <c r="B507">
         <v>5150</v>
       </c>
-      <c r="C507" t="s">
-        <v>724</v>
+      <c r="C507" s="5" t="s">
+        <v>695</v>
       </c>
       <c r="D507" s="18"/>
     </row>
@@ -10227,8 +10250,8 @@
       <c r="B508">
         <v>5160</v>
       </c>
-      <c r="C508" t="s">
-        <v>680</v>
+      <c r="C508" s="5" t="s">
+        <v>722</v>
       </c>
       <c r="D508" s="18"/>
     </row>
@@ -10237,8 +10260,8 @@
       <c r="B509">
         <v>5170</v>
       </c>
-      <c r="C509" t="s">
-        <v>725</v>
+      <c r="C509" s="5" t="s">
+        <v>696</v>
       </c>
       <c r="D509" s="18"/>
     </row>
@@ -10247,8 +10270,8 @@
       <c r="B510">
         <v>5180</v>
       </c>
-      <c r="C510" t="s">
-        <v>684</v>
+      <c r="C510" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="D510" s="18"/>
     </row>
@@ -10257,32 +10280,31 @@
       <c r="B511">
         <v>5190</v>
       </c>
-      <c r="C511" s="5" t="str">
-        <f>_xlfn.CONCAT("IF LOC=STOREDLOC THEN ERRVAL=1 :: GOTO ",INDEX(B:B,MATCH(D511,A:A,0),0)," :: REM SUBEND")</f>
-        <v>IF LOC=STOREDLOC THEN ERRVAL=1 :: GOTO 5230 :: REM SUBEND</v>
-      </c>
-      <c r="D511" s="20" t="str">
-        <f>A515</f>
-        <v>CHECKOVERLAP.SUBEND</v>
-      </c>
+      <c r="C511" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D511" s="18"/>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A512" s="18"/>
       <c r="B512">
         <v>5200</v>
       </c>
-      <c r="C512" t="s">
-        <v>84</v>
+      <c r="C512" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D512" s="18"/>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A513" s="18"/>
+      <c r="A513" s="18" t="s">
+        <v>566</v>
+      </c>
       <c r="B513">
         <v>5210</v>
       </c>
-      <c r="C513" t="s">
-        <v>14</v>
+      <c r="C513" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A513,"***")</f>
+        <v>REM SUBROUTINE ***CHECKOVERLAP***</v>
       </c>
       <c r="D513" s="18"/>
     </row>
@@ -10291,60 +10313,68 @@
       <c r="B514">
         <v>5220</v>
       </c>
-      <c r="C514" t="s">
-        <v>1</v>
+      <c r="C514" t="str">
+        <f>IF(ISBLANK(E514),_xlfn.CONCAT("SUB ",A513),_xlfn.CONCAT("SUB ",A513,"(",E514,")"))</f>
+        <v>SUB CHECKOVERLAP(ERRVAL,PLAYER,CURRENTSHIP,SHIP(),SHIPS(,,))</v>
       </c>
       <c r="D514" s="18"/>
+      <c r="E514" t="s">
+        <v>1033</v>
+      </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A515" s="20" t="str">
-        <f>_xlfn.CONCAT(A501,".SUBEND")</f>
-        <v>CHECKOVERLAP.SUBEND</v>
-      </c>
+      <c r="A515" s="18"/>
       <c r="B515">
         <v>5230</v>
       </c>
       <c r="C515" s="5" t="s">
-        <v>555</v>
+        <v>1031</v>
       </c>
       <c r="D515" s="18"/>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A516" s="18" t="s">
-        <v>954</v>
-      </c>
+      <c r="A516" s="18"/>
       <c r="B516">
         <v>5240</v>
       </c>
-      <c r="C516" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A516,"***")</f>
-        <v>REM SUBROUTINE ***QUEUESIZE***</v>
-      </c>
-      <c r="D516" s="18"/>
+      <c r="C516" s="18" t="str">
+        <f>IF(ISBLANK(E516),_xlfn.CONCAT("CALL ",D516),_xlfn.CONCAT("CALL ",D516,"(",E516,")"))</f>
+        <v>CALL GETSHIPLEN(CURRENTSHIPLEN,(CURRENTSHIP))</v>
+      </c>
+      <c r="D516" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E516" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A517" s="18"/>
       <c r="B517">
         <v>5250</v>
       </c>
-      <c r="C517" t="str">
-        <f>IF(ISBLANK(E517),_xlfn.CONCAT("SUB ",A516),_xlfn.CONCAT("SUB ",A516,"(",E517,")"))</f>
-        <v>SUB QUEUESIZE(QSIZE)</v>
+      <c r="C517" t="s">
+        <v>567</v>
       </c>
       <c r="D517" s="18"/>
-      <c r="E517" t="s">
-        <v>955</v>
-      </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A518" s="18"/>
       <c r="B518">
         <v>5260</v>
       </c>
-      <c r="C518" t="s">
-        <v>956</v>
-      </c>
-      <c r="D518" s="18"/>
+      <c r="C518" s="18" t="str">
+        <f>IF(ISBLANK(E518),_xlfn.CONCAT("CALL ",D518),_xlfn.CONCAT("CALL ",D518,"(",E518,")"))</f>
+        <v>CALL GETSHIPLEN(SHIPLEN,(I))</v>
+      </c>
+      <c r="D518" s="18" t="str">
+        <f>A588</f>
+        <v>GETSHIPLEN</v>
+      </c>
+      <c r="E518" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A519" s="18"/>
@@ -10352,20 +10382,17 @@
         <v>5270</v>
       </c>
       <c r="C519" t="s">
-        <v>555</v>
+        <v>724</v>
       </c>
       <c r="D519" s="18"/>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A520" s="18" t="s">
-        <v>953</v>
-      </c>
+      <c r="A520" s="18"/>
       <c r="B520">
         <v>5280</v>
       </c>
-      <c r="C520" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A520,"***")</f>
-        <v>REM SUBROUTINE ***QUEUEINIT***</v>
+      <c r="C520" t="s">
+        <v>680</v>
       </c>
       <c r="D520" s="18"/>
     </row>
@@ -10374,41 +10401,34 @@
       <c r="B521">
         <v>5290</v>
       </c>
-      <c r="C521" t="str">
-        <f>IF(ISBLANK(E521),_xlfn.CONCAT("SUB ",A520),_xlfn.CONCAT("SUB ",A520,"(",E521,")"))</f>
-        <v>SUB QUEUEINIT(Q(),QLEN)</v>
+      <c r="C521" t="s">
+        <v>725</v>
       </c>
       <c r="D521" s="18"/>
-      <c r="E521" t="s">
-        <v>944</v>
-      </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A522" s="18"/>
       <c r="B522">
         <v>5300</v>
       </c>
-      <c r="C522" s="18" t="str">
-        <f>IF(ISBLANK(E522),_xlfn.CONCAT("CALL ",D522),_xlfn.CONCAT("CALL ",D522,"(",E522,")"))</f>
-        <v>CALL QUEUESIZE(QSIZE)</v>
-      </c>
-      <c r="D522" s="18" t="str">
-        <f>A516</f>
-        <v>QUEUESIZE</v>
-      </c>
-      <c r="E522" t="s">
-        <v>955</v>
-      </c>
+      <c r="C522" t="s">
+        <v>684</v>
+      </c>
+      <c r="D522" s="18"/>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A523" s="18"/>
       <c r="B523">
         <v>5310</v>
       </c>
-      <c r="C523" t="s">
-        <v>963</v>
-      </c>
-      <c r="D523" s="18"/>
+      <c r="C523" s="5" t="str">
+        <f>_xlfn.CONCAT("IF LOC=STOREDLOC THEN ERRVAL=1 :: GOTO ",INDEX(B:B,MATCH(D523,A:A,0),0)," :: REM SUBEND")</f>
+        <v>IF LOC=STOREDLOC THEN ERRVAL=1 :: GOTO 5350 :: REM SUBEND</v>
+      </c>
+      <c r="D523" s="20" t="str">
+        <f>A527</f>
+        <v>CHECKOVERLAP.SUBEND</v>
+      </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A524" s="18"/>
@@ -10416,7 +10436,7 @@
         <v>5320</v>
       </c>
       <c r="C524" t="s">
-        <v>958</v>
+        <v>84</v>
       </c>
       <c r="D524" s="18"/>
     </row>
@@ -10426,63 +10446,59 @@
         <v>5330</v>
       </c>
       <c r="C525" t="s">
-        <v>555</v>
+        <v>14</v>
       </c>
       <c r="D525" s="18"/>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A526" s="18" t="s">
-        <v>945</v>
-      </c>
+      <c r="A526" s="18"/>
       <c r="B526">
         <v>5340</v>
       </c>
-      <c r="C526" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A526,"***")</f>
-        <v>REM SUBROUTINE ***QUEUEADD***</v>
+      <c r="C526" t="s">
+        <v>1</v>
       </c>
       <c r="D526" s="18"/>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A527" s="18"/>
+      <c r="A527" s="20" t="str">
+        <f>_xlfn.CONCAT(A513,".SUBEND")</f>
+        <v>CHECKOVERLAP.SUBEND</v>
+      </c>
       <c r="B527">
         <v>5350</v>
       </c>
-      <c r="C527" t="str">
-        <f>IF(ISBLANK(E527),_xlfn.CONCAT("SUB ",A526),_xlfn.CONCAT("SUB ",A526,"(",E527,")"))</f>
-        <v>SUB QUEUEADD(Q(),QLEN,VALUE,ERRVAL)</v>
+      <c r="C527" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D527" s="18"/>
-      <c r="E527" t="s">
-        <v>968</v>
-      </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A528" s="18"/>
+      <c r="A528" s="18" t="s">
+        <v>954</v>
+      </c>
       <c r="B528">
         <v>5360</v>
       </c>
-      <c r="C528" s="18" t="str">
-        <f>IF(ISBLANK(E528),_xlfn.CONCAT("CALL ",D528),_xlfn.CONCAT("CALL ",D528,"(",E528,")"))</f>
-        <v>CALL QUEUESIZE(QSIZE)</v>
-      </c>
-      <c r="D528" s="18" t="str">
-        <f>A516</f>
-        <v>QUEUESIZE</v>
-      </c>
-      <c r="E528" t="s">
-        <v>955</v>
-      </c>
+      <c r="C528" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A528,"***")</f>
+        <v>REM SUBROUTINE ***QUEUESIZE***</v>
+      </c>
+      <c r="D528" s="18"/>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A529" s="18"/>
       <c r="B529">
         <v>5370</v>
       </c>
-      <c r="C529" t="s">
-        <v>971</v>
+      <c r="C529" t="str">
+        <f>IF(ISBLANK(E529),_xlfn.CONCAT("SUB ",A528),_xlfn.CONCAT("SUB ",A528,"(",E529,")"))</f>
+        <v>SUB QUEUESIZE(QSIZE)</v>
       </c>
       <c r="D529" s="18"/>
+      <c r="E529" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A530" s="18"/>
@@ -10490,70 +10506,73 @@
         <v>5380</v>
       </c>
       <c r="C530" t="s">
-        <v>555</v>
+        <v>956</v>
       </c>
       <c r="D530" s="18"/>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A531" s="18" t="s">
-        <v>959</v>
-      </c>
+      <c r="A531" s="18"/>
       <c r="B531">
         <v>5390</v>
       </c>
-      <c r="C531" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A531,"***")</f>
-        <v>REM SUBROUTINE ***QUEUEDEL***</v>
+      <c r="C531" t="s">
+        <v>555</v>
       </c>
       <c r="D531" s="18"/>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A532" s="18"/>
+      <c r="A532" s="18" t="s">
+        <v>953</v>
+      </c>
       <c r="B532">
         <v>5400</v>
       </c>
       <c r="C532" t="str">
-        <f>IF(ISBLANK(E532),_xlfn.CONCAT("SUB ",A531),_xlfn.CONCAT("SUB ",A531,"(",E532,")"))</f>
-        <v>SUB QUEUEDEL(Q(),QLEN,VALUE,ERRVAL)</v>
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A532,"***")</f>
+        <v>REM SUBROUTINE ***QUEUEINIT***</v>
       </c>
       <c r="D532" s="18"/>
-      <c r="E532" t="s">
-        <v>968</v>
-      </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A533" s="18"/>
       <c r="B533">
         <v>5410</v>
       </c>
-      <c r="C533" t="s">
-        <v>961</v>
+      <c r="C533" t="str">
+        <f>IF(ISBLANK(E533),_xlfn.CONCAT("SUB ",A532),_xlfn.CONCAT("SUB ",A532,"(",E533,")"))</f>
+        <v>SUB QUEUEINIT(Q(),QLEN)</v>
       </c>
       <c r="D533" s="18"/>
+      <c r="E533" t="s">
+        <v>944</v>
+      </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A534" s="18"/>
       <c r="B534">
         <v>5420</v>
       </c>
-      <c r="C534" t="s">
-        <v>960</v>
-      </c>
-      <c r="D534" s="18"/>
+      <c r="C534" s="18" t="str">
+        <f>IF(ISBLANK(E534),_xlfn.CONCAT("CALL ",D534),_xlfn.CONCAT("CALL ",D534,"(",E534,")"))</f>
+        <v>CALL QUEUESIZE(QSIZE)</v>
+      </c>
+      <c r="D534" s="18" t="str">
+        <f>A528</f>
+        <v>QUEUESIZE</v>
+      </c>
+      <c r="E534" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A535" s="18"/>
       <c r="B535">
         <v>5430</v>
       </c>
-      <c r="C535" t="str">
-        <f>_xlfn.CONCAT("IF VALUE=Q(I) THEN DINDEX=I :: GOTO ",INDEX(B:B,MATCH(D535,A:A,0),0)," :: REM GOTO ",D535)</f>
-        <v>IF VALUE=Q(I) THEN DINDEX=I :: GOTO 5470 :: REM GOTO CONTRACT</v>
-      </c>
-      <c r="D535" s="20" t="str">
-        <f>A539</f>
-        <v>CONTRACT</v>
-      </c>
+      <c r="C535" t="s">
+        <v>963</v>
+      </c>
+      <c r="D535" s="18"/>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A536" s="18"/>
@@ -10561,123 +10580,128 @@
         <v>5440</v>
       </c>
       <c r="C536" t="s">
-        <v>1</v>
+        <v>958</v>
       </c>
       <c r="D536" s="18"/>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A537" s="20"/>
+      <c r="A537" s="18"/>
       <c r="B537">
         <v>5450</v>
       </c>
-      <c r="C537" t="str">
-        <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D537,A:A,0),0)," :: REM SUBEND")</f>
-        <v>GOTO 5510 :: REM SUBEND</v>
-      </c>
-      <c r="D537" s="20" t="str">
-        <f>A543</f>
-        <v>QUEUEDEL.SUBEND</v>
-      </c>
+      <c r="C537" t="s">
+        <v>555</v>
+      </c>
+      <c r="D537" s="18"/>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A538" s="18" t="s">
+        <v>945</v>
+      </c>
       <c r="B538">
         <v>5460</v>
       </c>
-      <c r="C538" s="5" t="str">
-        <f>_xlfn.CONCAT("REM LABEL ***",A539,"***")</f>
-        <v>REM LABEL ***CONTRACT***</v>
-      </c>
-      <c r="D538" s="20"/>
+      <c r="C538" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A538,"***")</f>
+        <v>REM SUBROUTINE ***QUEUEADD***</v>
+      </c>
+      <c r="D538" s="18"/>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A539" s="20" t="s">
-        <v>1043</v>
-      </c>
+      <c r="A539" s="18"/>
       <c r="B539">
         <v>5470</v>
       </c>
-      <c r="C539" t="s">
-        <v>952</v>
+      <c r="C539" t="str">
+        <f>IF(ISBLANK(E539),_xlfn.CONCAT("SUB ",A538),_xlfn.CONCAT("SUB ",A538,"(",E539,")"))</f>
+        <v>SUB QUEUEADD(Q(),QLEN,VALUE,ERRVAL)</v>
       </c>
       <c r="D539" s="18"/>
+      <c r="E539" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A540"/>
+      <c r="A540" s="18"/>
       <c r="B540">
         <v>5480</v>
       </c>
-      <c r="C540" t="s">
-        <v>962</v>
-      </c>
-      <c r="D540" s="18"/>
+      <c r="C540" s="18" t="str">
+        <f>IF(ISBLANK(E540),_xlfn.CONCAT("CALL ",D540),_xlfn.CONCAT("CALL ",D540,"(",E540,")"))</f>
+        <v>CALL QUEUESIZE(QSIZE)</v>
+      </c>
+      <c r="D540" s="18" t="str">
+        <f>A528</f>
+        <v>QUEUESIZE</v>
+      </c>
+      <c r="E540" t="s">
+        <v>955</v>
+      </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A541"/>
+      <c r="A541" s="18"/>
       <c r="B541">
         <v>5490</v>
       </c>
       <c r="C541" t="s">
-        <v>1</v>
+        <v>971</v>
       </c>
       <c r="D541" s="18"/>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A542"/>
+      <c r="A542" s="18"/>
       <c r="B542">
         <v>5500</v>
       </c>
       <c r="C542" t="s">
-        <v>970</v>
+        <v>555</v>
       </c>
       <c r="D542" s="18"/>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A543" s="20" t="str">
-        <f>_xlfn.CONCAT(A531,".SUBEND")</f>
-        <v>QUEUEDEL.SUBEND</v>
+      <c r="A543" s="18" t="s">
+        <v>959</v>
       </c>
       <c r="B543">
         <v>5510</v>
       </c>
-      <c r="C543" t="s">
-        <v>555</v>
+      <c r="C543" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A543,"***")</f>
+        <v>REM SUBROUTINE ***QUEUEDEL***</v>
       </c>
       <c r="D543" s="18"/>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A544" s="18" t="s">
-        <v>737</v>
-      </c>
+      <c r="A544" s="18"/>
       <c r="B544">
         <v>5520</v>
       </c>
       <c r="C544" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A544,"***")</f>
-        <v>REM SUBROUTINE ***GETHOLECHAR***</v>
+        <f>IF(ISBLANK(E544),_xlfn.CONCAT("SUB ",A543),_xlfn.CONCAT("SUB ",A543,"(",E544,")"))</f>
+        <v>SUB QUEUEDEL(Q(),QLEN,VALUE,ERRVAL)</v>
       </c>
       <c r="D544" s="18"/>
+      <c r="E544" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A545" s="18"/>
       <c r="B545">
         <v>5530</v>
       </c>
-      <c r="C545" t="str">
-        <f>IF(ISBLANK(E545),_xlfn.CONCAT("SUB ",A544),_xlfn.CONCAT("SUB ",A544,"(",E545,")"))</f>
-        <v>SUB GETHOLECHAR(CHARVAL)</v>
+      <c r="C545" t="s">
+        <v>961</v>
       </c>
       <c r="D545" s="18"/>
-      <c r="E545" t="s">
-        <v>747</v>
-      </c>
     </row>
     <row r="546" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A546" s="18"/>
       <c r="B546">
         <v>5540</v>
       </c>
-      <c r="C546" s="5" t="s">
-        <v>745</v>
+      <c r="C546" t="s">
+        <v>960</v>
       </c>
       <c r="D546" s="18"/>
     </row>
@@ -10686,115 +10710,114 @@
       <c r="B547">
         <v>5550</v>
       </c>
-      <c r="C547" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="D547" s="18"/>
+      <c r="C547" t="str">
+        <f>_xlfn.CONCAT("IF VALUE=Q(I) THEN DINDEX=I :: GOTO ",INDEX(B:B,MATCH(D547,A:A,0),0)," :: REM GOTO ",D547)</f>
+        <v>IF VALUE=Q(I) THEN DINDEX=I :: GOTO 5590 :: REM GOTO CONTRACT</v>
+      </c>
+      <c r="D547" s="20" t="str">
+        <f>A551</f>
+        <v>CONTRACT</v>
+      </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A548" s="18" t="s">
-        <v>749</v>
-      </c>
+      <c r="A548" s="18"/>
       <c r="B548">
         <v>5560</v>
       </c>
-      <c r="C548" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A548,"***")</f>
-        <v>REM SUBROUTINE ***GETFILLCHAR***</v>
+      <c r="C548" t="s">
+        <v>1</v>
       </c>
       <c r="D548" s="18"/>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A549" s="18"/>
+      <c r="A549" s="20"/>
       <c r="B549">
         <v>5570</v>
       </c>
       <c r="C549" t="str">
-        <f>IF(ISBLANK(E549),_xlfn.CONCAT("SUB ",A548),_xlfn.CONCAT("SUB ",A548,"(",E549,")"))</f>
-        <v>SUB GETFILLCHAR(CHARVAL)</v>
-      </c>
-      <c r="D549" s="18"/>
-      <c r="E549" t="s">
-        <v>747</v>
+        <f>_xlfn.CONCAT("GOTO ",INDEX(B:B,MATCH(D549,A:A,0),0)," :: REM SUBEND")</f>
+        <v>GOTO 5630 :: REM SUBEND</v>
+      </c>
+      <c r="D549" s="20" t="str">
+        <f>A555</f>
+        <v>QUEUEDEL.SUBEND</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A550" s="18"/>
       <c r="B550">
         <v>5580</v>
       </c>
-      <c r="C550" s="5" t="s">
-        <v>750</v>
-      </c>
-      <c r="D550" s="18"/>
+      <c r="C550" s="5" t="str">
+        <f>_xlfn.CONCAT("REM LABEL ***",A551,"***")</f>
+        <v>REM LABEL ***CONTRACT***</v>
+      </c>
+      <c r="D550" s="20"/>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A551" s="18"/>
+      <c r="A551" s="20" t="s">
+        <v>1043</v>
+      </c>
       <c r="B551">
         <v>5590</v>
       </c>
-      <c r="C551" s="5" t="s">
-        <v>555</v>
+      <c r="C551" t="s">
+        <v>952</v>
       </c>
       <c r="D551" s="18"/>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A552" s="18" t="s">
-        <v>753</v>
-      </c>
+      <c r="A552"/>
       <c r="B552">
         <v>5600</v>
       </c>
-      <c r="C552" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A552,"***")</f>
-        <v>REM SUBROUTINE ***GETHITCHAR***</v>
+      <c r="C552" t="s">
+        <v>962</v>
       </c>
       <c r="D552" s="18"/>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A553" s="18"/>
+      <c r="A553"/>
       <c r="B553">
         <v>5610</v>
       </c>
-      <c r="C553" t="str">
-        <f>IF(ISBLANK(E553),_xlfn.CONCAT("SUB ",A552),_xlfn.CONCAT("SUB ",A552,"(",E553,")"))</f>
-        <v>SUB GETHITCHAR(CHARVAL)</v>
+      <c r="C553" t="s">
+        <v>1</v>
       </c>
       <c r="D553" s="18"/>
-      <c r="E553" t="s">
-        <v>747</v>
-      </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A554" s="18"/>
+      <c r="A554"/>
       <c r="B554">
         <v>5620</v>
       </c>
-      <c r="C554" s="5" t="s">
-        <v>754</v>
+      <c r="C554" t="s">
+        <v>970</v>
       </c>
       <c r="D554" s="18"/>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A555" s="18"/>
+      <c r="A555" s="20" t="str">
+        <f>_xlfn.CONCAT(A543,".SUBEND")</f>
+        <v>QUEUEDEL.SUBEND</v>
+      </c>
       <c r="B555">
         <v>5630</v>
       </c>
-      <c r="C555" s="5" t="s">
+      <c r="C555" t="s">
         <v>555</v>
       </c>
       <c r="D555" s="18"/>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A556" s="18" t="s">
-        <v>713</v>
+        <v>737</v>
       </c>
       <c r="B556">
         <v>5640</v>
       </c>
       <c r="C556" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A556,"***")</f>
-        <v>REM SUBROUTINE ***GETSHIPCHAR***</v>
+        <v>REM SUBROUTINE ***GETHOLECHAR***</v>
       </c>
       <c r="D556" s="18"/>
     </row>
@@ -10805,7 +10828,7 @@
       </c>
       <c r="C557" t="str">
         <f>IF(ISBLANK(E557),_xlfn.CONCAT("SUB ",A556),_xlfn.CONCAT("SUB ",A556,"(",E557,")"))</f>
-        <v>SUB GETSHIPCHAR(CHARVAL)</v>
+        <v>SUB GETHOLECHAR(CHARVAL)</v>
       </c>
       <c r="D557" s="18"/>
       <c r="E557" t="s">
@@ -10818,7 +10841,7 @@
         <v>5660</v>
       </c>
       <c r="C558" s="5" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="D558" s="18"/>
     </row>
@@ -10834,14 +10857,14 @@
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A560" s="18" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="B560">
         <v>5680</v>
       </c>
       <c r="C560" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A560,"***")</f>
-        <v>REM SUBROUTINE ***GETTENCHAR***</v>
+        <v>REM SUBROUTINE ***GETFILLCHAR***</v>
       </c>
       <c r="D560" s="18"/>
     </row>
@@ -10852,7 +10875,7 @@
       </c>
       <c r="C561" t="str">
         <f>IF(ISBLANK(E561),_xlfn.CONCAT("SUB ",A560),_xlfn.CONCAT("SUB ",A560,"(",E561,")"))</f>
-        <v>SUB GETTENCHAR(CHARVAL)</v>
+        <v>SUB GETFILLCHAR(CHARVAL)</v>
       </c>
       <c r="D561" s="18"/>
       <c r="E561" t="s">
@@ -10865,7 +10888,7 @@
         <v>5700</v>
       </c>
       <c r="C562" s="5" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="D562" s="18"/>
     </row>
@@ -10881,14 +10904,14 @@
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A564" s="18" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B564">
         <v>5720</v>
       </c>
       <c r="C564" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A564,"***")</f>
-        <v>REM SUBROUTINE ***GETMISSCHAR***</v>
+        <v>REM SUBROUTINE ***GETHITCHAR***</v>
       </c>
       <c r="D564" s="18"/>
     </row>
@@ -10899,7 +10922,7 @@
       </c>
       <c r="C565" t="str">
         <f>IF(ISBLANK(E565),_xlfn.CONCAT("SUB ",A564),_xlfn.CONCAT("SUB ",A564,"(",E565,")"))</f>
-        <v>SUB GETMISSCHAR(CHARVAL)</v>
+        <v>SUB GETHITCHAR(CHARVAL)</v>
       </c>
       <c r="D565" s="18"/>
       <c r="E565" t="s">
@@ -10912,7 +10935,7 @@
         <v>5740</v>
       </c>
       <c r="C566" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D566" s="18"/>
     </row>
@@ -10928,14 +10951,14 @@
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A568" s="18" t="s">
-        <v>762</v>
+        <v>713</v>
       </c>
       <c r="B568">
         <v>5760</v>
       </c>
       <c r="C568" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A568,"***")</f>
-        <v>REM SUBROUTINE ***GETSUNKCHAR***</v>
+        <v>REM SUBROUTINE ***GETSHIPCHAR***</v>
       </c>
       <c r="D568" s="18"/>
     </row>
@@ -10946,7 +10969,7 @@
       </c>
       <c r="C569" t="str">
         <f>IF(ISBLANK(E569),_xlfn.CONCAT("SUB ",A568),_xlfn.CONCAT("SUB ",A568,"(",E569,")"))</f>
-        <v>SUB GETSUNKCHAR(CHARVAL)</v>
+        <v>SUB GETSHIPCHAR(CHARVAL)</v>
       </c>
       <c r="D569" s="18"/>
       <c r="E569" t="s">
@@ -10959,7 +10982,7 @@
         <v>5780</v>
       </c>
       <c r="C570" s="5" t="s">
-        <v>763</v>
+        <v>744</v>
       </c>
       <c r="D570" s="18"/>
     </row>
@@ -10975,14 +10998,14 @@
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A572" s="18" t="s">
-        <v>705</v>
+        <v>743</v>
       </c>
       <c r="B572">
         <v>5800</v>
       </c>
       <c r="C572" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A572,"***")</f>
-        <v>REM SUBROUTINE ***GETNUMSHIPS***</v>
+        <v>REM SUBROUTINE ***GETTENCHAR***</v>
       </c>
       <c r="D572" s="18"/>
     </row>
@@ -10993,11 +11016,11 @@
       </c>
       <c r="C573" t="str">
         <f>IF(ISBLANK(E573),_xlfn.CONCAT("SUB ",A572),_xlfn.CONCAT("SUB ",A572,"(",E573,")"))</f>
-        <v>SUB GETNUMSHIPS(NUMSHIPS)</v>
+        <v>SUB GETTENCHAR(CHARVAL)</v>
       </c>
       <c r="D573" s="18"/>
       <c r="E573" t="s">
-        <v>706</v>
+        <v>747</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.2">
@@ -11005,8 +11028,8 @@
       <c r="B574">
         <v>5820</v>
       </c>
-      <c r="C574" t="s">
-        <v>550</v>
+      <c r="C574" s="5" t="s">
+        <v>746</v>
       </c>
       <c r="D574" s="18"/>
     </row>
@@ -11015,21 +11038,21 @@
       <c r="B575">
         <v>5830</v>
       </c>
-      <c r="C575" t="s">
+      <c r="C575" s="5" t="s">
         <v>555</v>
       </c>
       <c r="D575" s="18"/>
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A576" s="18" t="s">
-        <v>717</v>
+        <v>755</v>
       </c>
       <c r="B576">
         <v>5840</v>
       </c>
       <c r="C576" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A576,"***")</f>
-        <v>REM SUBROUTINE ***GETSHIPLEN***</v>
+        <v>REM SUBROUTINE ***GETMISSCHAR***</v>
       </c>
       <c r="D576" s="18"/>
     </row>
@@ -11040,11 +11063,11 @@
       </c>
       <c r="C577" t="str">
         <f>IF(ISBLANK(E577),_xlfn.CONCAT("SUB ",A576),_xlfn.CONCAT("SUB ",A576,"(",E577,")"))</f>
-        <v>SUB GETSHIPLEN(SHIPLEN,INDEX)</v>
+        <v>SUB GETMISSCHAR(CHARVAL)</v>
       </c>
       <c r="D577" s="18"/>
       <c r="E577" t="s">
-        <v>718</v>
+        <v>747</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.2">
@@ -11052,8 +11075,8 @@
       <c r="B578">
         <v>5860</v>
       </c>
-      <c r="C578" t="s">
-        <v>614</v>
+      <c r="C578" s="5" t="s">
+        <v>756</v>
       </c>
       <c r="D578" s="18"/>
     </row>
@@ -11062,65 +11085,68 @@
       <c r="B579">
         <v>5870</v>
       </c>
-      <c r="C579" t="s">
-        <v>721</v>
+      <c r="C579" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D579" s="18"/>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A580" s="18"/>
+      <c r="A580" s="18" t="s">
+        <v>762</v>
+      </c>
       <c r="B580">
         <v>5880</v>
       </c>
-      <c r="C580" s="5" t="s">
-        <v>555</v>
+      <c r="C580" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A580,"***")</f>
+        <v>REM SUBROUTINE ***GETSUNKCHAR***</v>
       </c>
       <c r="D580" s="18"/>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A581" s="18" t="s">
-        <v>716</v>
-      </c>
+      <c r="A581" s="18"/>
       <c r="B581">
         <v>5890</v>
       </c>
       <c r="C581" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A581,"***")</f>
-        <v>REM SUBROUTINE ***GETSHIPNAME***</v>
+        <f>IF(ISBLANK(E581),_xlfn.CONCAT("SUB ",A580),_xlfn.CONCAT("SUB ",A580,"(",E581,")"))</f>
+        <v>SUB GETSUNKCHAR(CHARVAL)</v>
       </c>
       <c r="D581" s="18"/>
+      <c r="E581" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A582" s="18"/>
       <c r="B582">
         <v>5900</v>
       </c>
-      <c r="C582" t="str">
-        <f>IF(ISBLANK(E582),_xlfn.CONCAT("SUB ",A581),_xlfn.CONCAT("SUB ",A581,"(",E582,")"))</f>
-        <v>SUB GETSHIPNAME(SHIPNAME$,INDEX)</v>
+      <c r="C582" s="5" t="s">
+        <v>763</v>
       </c>
       <c r="D582" s="18"/>
-      <c r="E582" t="s">
-        <v>719</v>
-      </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A583" s="18"/>
       <c r="B583">
         <v>5910</v>
       </c>
-      <c r="C583" t="s">
-        <v>615</v>
+      <c r="C583" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D583" s="18"/>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A584" s="18"/>
+      <c r="A584" s="18" t="s">
+        <v>705</v>
+      </c>
       <c r="B584">
         <v>5920</v>
       </c>
-      <c r="C584" t="s">
-        <v>720</v>
+      <c r="C584" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A584,"***")</f>
+        <v>REM SUBROUTINE ***GETNUMSHIPS***</v>
       </c>
       <c r="D584" s="18"/>
     </row>
@@ -11129,21 +11155,22 @@
       <c r="B585">
         <v>5930</v>
       </c>
-      <c r="C585" s="5" t="s">
-        <v>555</v>
+      <c r="C585" t="str">
+        <f>IF(ISBLANK(E585),_xlfn.CONCAT("SUB ",A584),_xlfn.CONCAT("SUB ",A584,"(",E585,")"))</f>
+        <v>SUB GETNUMSHIPS(NUMSHIPS)</v>
       </c>
       <c r="D585" s="18"/>
+      <c r="E585" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A586" s="18" t="s">
-        <v>707</v>
-      </c>
+      <c r="A586" s="18"/>
       <c r="B586">
         <v>5940</v>
       </c>
-      <c r="C586" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A586,"***")</f>
-        <v>REM SUBROUTINE ***GETBOARDORIG***</v>
+      <c r="C586" t="s">
+        <v>550</v>
       </c>
       <c r="D586" s="18"/>
     </row>
@@ -11152,22 +11179,21 @@
       <c r="B587">
         <v>5950</v>
       </c>
-      <c r="C587" t="str">
-        <f>IF(ISBLANK(E587),_xlfn.CONCAT("SUB ",A586),_xlfn.CONCAT("SUB ",A586,"(",E587,")"))</f>
-        <v>SUB GETBOARDORIG(ROW,COL)</v>
+      <c r="C587" t="s">
+        <v>555</v>
       </c>
       <c r="D587" s="18"/>
-      <c r="E587" t="s">
-        <v>689</v>
-      </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A588" s="18"/>
+      <c r="A588" s="18" t="s">
+        <v>717</v>
+      </c>
       <c r="B588">
         <v>5960</v>
       </c>
-      <c r="C588" t="s">
-        <v>708</v>
+      <c r="C588" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A588,"***")</f>
+        <v>REM SUBROUTINE ***GETSHIPLEN***</v>
       </c>
       <c r="D588" s="18"/>
     </row>
@@ -11176,21 +11202,22 @@
       <c r="B589">
         <v>5970</v>
       </c>
-      <c r="C589" s="5" t="s">
-        <v>555</v>
+      <c r="C589" t="str">
+        <f>IF(ISBLANK(E589),_xlfn.CONCAT("SUB ",A588),_xlfn.CONCAT("SUB ",A588,"(",E589,")"))</f>
+        <v>SUB GETSHIPLEN(SHIPLEN,INDEX)</v>
       </c>
       <c r="D589" s="18"/>
+      <c r="E589" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A590" s="18" t="s">
-        <v>711</v>
-      </c>
+      <c r="A590" s="18"/>
       <c r="B590">
         <v>5980</v>
       </c>
-      <c r="C590" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A590,"***")</f>
-        <v>REM SUBROUTINE ***GETAUXORIG***</v>
+      <c r="C590" t="s">
+        <v>614</v>
       </c>
       <c r="D590" s="18"/>
     </row>
@@ -11199,73 +11226,69 @@
       <c r="B591">
         <v>5990</v>
       </c>
-      <c r="C591" t="str">
-        <f>IF(ISBLANK(E591),_xlfn.CONCAT("SUB ",A590),_xlfn.CONCAT("SUB ",A590,"(",E591,")"))</f>
-        <v>SUB GETAUXORIG(ROW,COL)</v>
+      <c r="C591" t="s">
+        <v>721</v>
       </c>
       <c r="D591" s="18"/>
-      <c r="E591" t="s">
-        <v>689</v>
-      </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A592" s="18"/>
       <c r="B592">
         <v>6000</v>
       </c>
-      <c r="C592" t="s">
-        <v>709</v>
+      <c r="C592" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D592" s="18"/>
     </row>
-    <row r="593" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A593" s="18"/>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A593" s="18" t="s">
+        <v>716</v>
+      </c>
       <c r="B593">
         <v>6010</v>
       </c>
-      <c r="C593" s="5" t="s">
-        <v>555</v>
+      <c r="C593" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A593,"***")</f>
+        <v>REM SUBROUTINE ***GETSHIPNAME***</v>
       </c>
       <c r="D593" s="18"/>
     </row>
-    <row r="594" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A594" s="18" t="s">
-        <v>710</v>
-      </c>
+    <row r="594" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A594" s="18"/>
       <c r="B594">
         <v>6020</v>
       </c>
       <c r="C594" t="str">
-        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A594,"***")</f>
-        <v>REM SUBROUTINE ***GETMENUORIG***</v>
+        <f>IF(ISBLANK(E594),_xlfn.CONCAT("SUB ",A593),_xlfn.CONCAT("SUB ",A593,"(",E594,")"))</f>
+        <v>SUB GETSHIPNAME(SHIPNAME$,INDEX)</v>
       </c>
       <c r="D594" s="18"/>
-    </row>
-    <row r="595" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E594" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A595" s="18"/>
       <c r="B595">
         <v>6030</v>
       </c>
-      <c r="C595" t="str">
-        <f>IF(ISBLANK(E595),_xlfn.CONCAT("SUB ",A594),_xlfn.CONCAT("SUB ",A594,"(",E595,")"))</f>
-        <v>SUB GETMENUORIG(ROW,COL)</v>
+      <c r="C595" t="s">
+        <v>615</v>
       </c>
       <c r="D595" s="18"/>
-      <c r="E595" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="596" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="596" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A596" s="18"/>
       <c r="B596">
         <v>6040</v>
       </c>
       <c r="C596" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="D596" s="18"/>
     </row>
-    <row r="597" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A597" s="18"/>
       <c r="B597">
         <v>6050</v>
@@ -11275,44 +11298,44 @@
       </c>
       <c r="D597" s="18"/>
     </row>
-    <row r="598" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A598" s="18" t="s">
-        <v>733</v>
+        <v>707</v>
       </c>
       <c r="B598">
         <v>6060</v>
       </c>
       <c r="C598" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A598,"***")</f>
-        <v>REM SUBROUTINE ***GETDEBUGFLAG***</v>
+        <v>REM SUBROUTINE ***GETBOARDORIG***</v>
       </c>
       <c r="D598" s="18"/>
     </row>
-    <row r="599" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A599" s="18"/>
       <c r="B599">
         <v>6070</v>
       </c>
       <c r="C599" t="str">
         <f>IF(ISBLANK(E599),_xlfn.CONCAT("SUB ",A598),_xlfn.CONCAT("SUB ",A598,"(",E599,")"))</f>
-        <v>SUB GETDEBUGFLAG(DEBUG)</v>
+        <v>SUB GETBOARDORIG(ROW,COL)</v>
       </c>
       <c r="D599" s="18"/>
       <c r="E599" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="600" spans="1:6" x14ac:dyDescent="0.2">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A600" s="18"/>
       <c r="B600">
         <v>6080</v>
       </c>
-      <c r="C600" s="5" t="s">
-        <v>1022</v>
+      <c r="C600" t="s">
+        <v>708</v>
       </c>
       <c r="D600" s="18"/>
     </row>
-    <row r="601" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A601" s="18"/>
       <c r="B601">
         <v>6090</v>
@@ -11321,49 +11344,45 @@
         <v>555</v>
       </c>
       <c r="D601" s="18"/>
-      <c r="F601" t="str">
-        <f>_xlfn.IFNA(MATCH(D601,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="602" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A602" s="18" t="s">
-        <v>1013</v>
+        <v>711</v>
       </c>
       <c r="B602">
         <v>6100</v>
       </c>
       <c r="C602" t="str">
         <f>_xlfn.CONCAT("REM SUBROUTINE ***",A602,"***")</f>
-        <v>REM SUBROUTINE ***GETAUTOPLAY***</v>
+        <v>REM SUBROUTINE ***GETAUXORIG***</v>
       </c>
       <c r="D602" s="18"/>
     </row>
-    <row r="603" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A603" s="18"/>
       <c r="B603">
         <v>6110</v>
       </c>
       <c r="C603" t="str">
         <f>IF(ISBLANK(E603),_xlfn.CONCAT("SUB ",A602),_xlfn.CONCAT("SUB ",A602,"(",E603,")"))</f>
-        <v>SUB GETAUTOPLAY(AUTOPLAY)</v>
+        <v>SUB GETAUXORIG(ROW,COL)</v>
       </c>
       <c r="D603" s="18"/>
       <c r="E603" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="604" spans="1:6" x14ac:dyDescent="0.2">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A604" s="18"/>
       <c r="B604">
         <v>6120</v>
       </c>
-      <c r="C604" s="5" t="s">
-        <v>1024</v>
+      <c r="C604" t="s">
+        <v>709</v>
       </c>
       <c r="D604" s="18"/>
     </row>
-    <row r="605" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A605" s="18"/>
       <c r="B605">
         <v>6130</v>
@@ -11372,134 +11391,255 @@
         <v>555</v>
       </c>
       <c r="D605" s="18"/>
-      <c r="F605" t="str">
-        <f>_xlfn.IFNA(MATCH(D605,A:A,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="606" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C606" s="5"/>
-    </row>
-    <row r="607" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C607" s="5"/>
-    </row>
-    <row r="608" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C608" s="5"/>
-    </row>
-    <row r="609" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C609" s="5"/>
-    </row>
-    <row r="610" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A610"/>
-      <c r="C610" s="5"/>
-    </row>
-    <row r="611" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A611"/>
-      <c r="C611" s="5"/>
-    </row>
-    <row r="612" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A612"/>
-      <c r="C612" s="5"/>
-    </row>
-    <row r="613" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A613"/>
-      <c r="C613" s="5"/>
-    </row>
-    <row r="614" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A614"/>
-      <c r="C614" s="5"/>
-    </row>
-    <row r="615" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A615"/>
-      <c r="C615" s="5"/>
-    </row>
-    <row r="616" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A616"/>
-      <c r="C616" s="5"/>
-    </row>
-    <row r="617" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A617"/>
-      <c r="C617" s="5"/>
-    </row>
-    <row r="638" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A638"/>
-      <c r="C638" s="5"/>
-    </row>
-    <row r="639" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A639"/>
-      <c r="C639" s="5"/>
-    </row>
-    <row r="643" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A643"/>
-      <c r="C643" s="5"/>
-    </row>
-    <row r="646" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A646"/>
-      <c r="C646" s="5"/>
-    </row>
-    <row r="652" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A652"/>
-      <c r="C652" s="5"/>
-    </row>
-    <row r="656" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A656"/>
-      <c r="C656" s="5"/>
-    </row>
-    <row r="660" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A660"/>
-      <c r="C660" s="5"/>
+    </row>
+    <row r="606" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A606" s="18" t="s">
+        <v>710</v>
+      </c>
+      <c r="B606">
+        <v>6140</v>
+      </c>
+      <c r="C606" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A606,"***")</f>
+        <v>REM SUBROUTINE ***GETMENUORIG***</v>
+      </c>
+      <c r="D606" s="18"/>
+    </row>
+    <row r="607" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A607" s="18"/>
+      <c r="B607">
+        <v>6150</v>
+      </c>
+      <c r="C607" t="str">
+        <f>IF(ISBLANK(E607),_xlfn.CONCAT("SUB ",A606),_xlfn.CONCAT("SUB ",A606,"(",E607,")"))</f>
+        <v>SUB GETMENUORIG(ROW,COL)</v>
+      </c>
+      <c r="D607" s="18"/>
+      <c r="E607" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A608" s="18"/>
+      <c r="B608">
+        <v>6160</v>
+      </c>
+      <c r="C608" t="s">
+        <v>712</v>
+      </c>
+      <c r="D608" s="18"/>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A609" s="18"/>
+      <c r="B609">
+        <v>6170</v>
+      </c>
+      <c r="C609" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="D609" s="18"/>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A610" s="18" t="s">
+        <v>733</v>
+      </c>
+      <c r="B610">
+        <v>6180</v>
+      </c>
+      <c r="C610" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A610,"***")</f>
+        <v>REM SUBROUTINE ***GETDEBUGFLAG***</v>
+      </c>
+      <c r="D610" s="18"/>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A611" s="18"/>
+      <c r="B611">
+        <v>6190</v>
+      </c>
+      <c r="C611" t="str">
+        <f>IF(ISBLANK(E611),_xlfn.CONCAT("SUB ",A610),_xlfn.CONCAT("SUB ",A610,"(",E611,")"))</f>
+        <v>SUB GETDEBUGFLAG(DEBUG)</v>
+      </c>
+      <c r="D611" s="18"/>
+      <c r="E611" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A612" s="18"/>
+      <c r="B612">
+        <v>6200</v>
+      </c>
+      <c r="C612" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D612" s="18"/>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A613" s="18"/>
+      <c r="B613">
+        <v>6210</v>
+      </c>
+      <c r="C613" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="D613" s="18"/>
+      <c r="F613" t="str">
+        <f>_xlfn.IFNA(MATCH(D613,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A614" s="18" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B614">
+        <v>6220</v>
+      </c>
+      <c r="C614" t="str">
+        <f>_xlfn.CONCAT("REM SUBROUTINE ***",A614,"***")</f>
+        <v>REM SUBROUTINE ***GETAUTOPLAY***</v>
+      </c>
+      <c r="D614" s="18"/>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A615" s="18"/>
+      <c r="B615">
+        <v>6230</v>
+      </c>
+      <c r="C615" t="str">
+        <f>IF(ISBLANK(E615),_xlfn.CONCAT("SUB ",A614),_xlfn.CONCAT("SUB ",A614,"(",E615,")"))</f>
+        <v>SUB GETAUTOPLAY(AUTOPLAY)</v>
+      </c>
+      <c r="D615" s="18"/>
+      <c r="E615" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A616" s="18"/>
+      <c r="B616">
+        <v>6240</v>
+      </c>
+      <c r="C616" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D616" s="18"/>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A617" s="18"/>
+      <c r="B617">
+        <v>6250</v>
+      </c>
+      <c r="C617" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="D617" s="18"/>
+      <c r="F617" t="str">
+        <f>_xlfn.IFNA(MATCH(D617,A:A,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C618" s="5"/>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C619" s="5"/>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C620" s="5"/>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C621" s="5"/>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A622"/>
+      <c r="C622" s="5"/>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A623"/>
+      <c r="C623" s="5"/>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A624"/>
+      <c r="C624" s="5"/>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A625"/>
+      <c r="C625" s="5"/>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A626"/>
+      <c r="C626" s="5"/>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A627"/>
+      <c r="C627" s="5"/>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A628"/>
+      <c r="C628" s="5"/>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A629"/>
+      <c r="C629" s="5"/>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A650"/>
+      <c r="C650" s="5"/>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A651"/>
+      <c r="C651" s="5"/>
+    </row>
+    <row r="655" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A655"/>
+      <c r="C655" s="5"/>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A658"/>
+      <c r="C658" s="5"/>
     </row>
     <row r="664" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A664"/>
       <c r="C664" s="5"/>
     </row>
-    <row r="674" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A674"/>
-      <c r="C674" s="5"/>
-    </row>
-    <row r="681" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A681"/>
-      <c r="C681" s="5"/>
-    </row>
-    <row r="685" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A685"/>
-      <c r="C685" s="5"/>
-    </row>
-    <row r="690" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C690" s="5"/>
-    </row>
-    <row r="696" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C696" s="5"/>
-    </row>
-    <row r="702" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="668" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A668"/>
+      <c r="C668" s="5"/>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A672"/>
+      <c r="C672" s="5"/>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A676"/>
+      <c r="C676" s="5"/>
+    </row>
+    <row r="686" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A686"/>
+      <c r="C686" s="5"/>
+    </row>
+    <row r="693" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A693"/>
+      <c r="C693" s="5"/>
+    </row>
+    <row r="697" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A697"/>
+      <c r="C697" s="5"/>
+    </row>
+    <row r="702" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C702" s="5"/>
     </row>
-    <row r="705" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C705" s="5"/>
-    </row>
-    <row r="727" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C727" s="5"/>
-    </row>
-    <row r="728" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C728" s="5"/>
-    </row>
-    <row r="729" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C729" s="5"/>
-    </row>
-    <row r="730" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C730" s="5"/>
-    </row>
-    <row r="731" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C731" s="5"/>
-    </row>
-    <row r="732" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C732" s="5"/>
-    </row>
-    <row r="733" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C733" s="5"/>
-    </row>
-    <row r="734" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C734" s="5"/>
+    <row r="708" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C708" s="5"/>
+    </row>
+    <row r="714" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C714" s="5"/>
+    </row>
+    <row r="717" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C717" s="5"/>
     </row>
     <row r="739" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C739" s="5"/>
@@ -11519,44 +11659,56 @@
     <row r="744" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C744" s="5"/>
     </row>
+    <row r="745" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C745" s="5"/>
+    </row>
     <row r="746" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C746" s="5"/>
     </row>
-    <row r="747" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C747" s="5"/>
-    </row>
-    <row r="760" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C760" s="1"/>
-    </row>
-    <row r="761" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C761" s="1"/>
-    </row>
-    <row r="762" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C762" s="1"/>
-    </row>
-    <row r="763" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C763" s="1"/>
-    </row>
-    <row r="764" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C764" s="1"/>
-    </row>
-    <row r="766" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C766" s="1"/>
-    </row>
-    <row r="768" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C768" s="1"/>
-    </row>
-    <row r="769" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C769" s="1"/>
-    </row>
-    <row r="771" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C771" s="1"/>
+    <row r="751" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C751" s="5"/>
+    </row>
+    <row r="752" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C752" s="5"/>
+    </row>
+    <row r="753" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C753" s="5"/>
+    </row>
+    <row r="754" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C754" s="5"/>
+    </row>
+    <row r="755" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C755" s="5"/>
+    </row>
+    <row r="756" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C756" s="5"/>
+    </row>
+    <row r="758" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C758" s="5"/>
+    </row>
+    <row r="759" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C759" s="5"/>
+    </row>
+    <row r="772" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C772" s="1"/>
     </row>
     <row r="773" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C773" s="1"/>
     </row>
-    <row r="777" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C777" s="1"/>
+    <row r="774" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C774" s="1"/>
+    </row>
+    <row r="775" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C775" s="1"/>
+    </row>
+    <row r="776" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C776" s="1"/>
+    </row>
+    <row r="778" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C778" s="1"/>
+    </row>
+    <row r="780" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C780" s="1"/>
     </row>
     <row r="781" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C781" s="1"/>
@@ -11564,29 +11716,41 @@
     <row r="783" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C783" s="1"/>
     </row>
-    <row r="784" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C784" s="1"/>
+    <row r="785" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C785" s="1"/>
     </row>
     <row r="789" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C789" s="5"/>
-    </row>
-    <row r="802" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C802" s="5"/>
-    </row>
-    <row r="806" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C806" s="5"/>
-    </row>
-    <row r="807" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C807" s="5"/>
-    </row>
-    <row r="808" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C808" s="5"/>
-    </row>
-    <row r="809" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C809" s="5"/>
-    </row>
-    <row r="812" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C812" s="5"/>
+      <c r="C789" s="1"/>
+    </row>
+    <row r="793" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C793" s="1"/>
+    </row>
+    <row r="795" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C795" s="1"/>
+    </row>
+    <row r="796" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C796" s="1"/>
+    </row>
+    <row r="801" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C801" s="5"/>
+    </row>
+    <row r="814" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C814" s="5"/>
+    </row>
+    <row r="818" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C818" s="5"/>
+    </row>
+    <row r="819" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C819" s="5"/>
+    </row>
+    <row r="820" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C820" s="5"/>
+    </row>
+    <row r="821" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C821" s="5"/>
+    </row>
+    <row r="824" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C824" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>